<commit_message>
Improved accuracy of cosh function.
git-svn-id: https://svn.code.sf.net/p/half/code/branches/clean@365 ba856b29-48f5-46b1-a3e5-b459205bce89
</commit_message>
<xml_diff>
--- a/test/results.xlsx
+++ b/test/results.xlsx
@@ -2458,10 +2458,10 @@
         <v>11136</v>
       </c>
       <c r="F24" s="2">
-        <v>9654</v>
+        <v>8956</v>
       </c>
       <c r="G24" s="2">
-        <v>8909</v>
+        <v>8358</v>
       </c>
       <c r="H24" s="2">
         <v>2</v>
@@ -2476,18 +2476,18 @@
         <v>13892</v>
       </c>
       <c r="L24" s="2">
-        <v>10245</v>
+        <v>10288</v>
       </c>
       <c r="M24" s="2">
-        <v>3353</v>
+        <v>3095</v>
       </c>
       <c r="N24" s="8">
         <f t="shared" si="0"/>
-        <v>1.0612181479179614</v>
+        <v>1.1487271103171059</v>
       </c>
       <c r="O24" s="8">
         <f t="shared" si="1"/>
-        <v>0.37636098327533957</v>
+        <v>0.37030390045465422</v>
       </c>
       <c r="P24" s="2">
         <v>0</v>
@@ -2502,18 +2502,18 @@
         <v>6771</v>
       </c>
       <c r="T24" s="2">
-        <v>10426</v>
+        <v>10423</v>
       </c>
       <c r="U24" s="2">
-        <v>2962</v>
+        <v>2961</v>
       </c>
       <c r="V24" s="8">
         <f t="shared" si="2"/>
-        <v>1.0799668531178785</v>
+        <v>1.163800803930326</v>
       </c>
       <c r="W24" s="9">
         <f t="shared" si="3"/>
-        <v>0.33247278033449323</v>
+        <v>0.35427135678391958</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
@@ -2524,19 +2524,19 @@
         <v>0</v>
       </c>
       <c r="C25" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D25" s="2">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E25" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F25" s="2">
-        <v>7205</v>
+        <v>7230</v>
       </c>
       <c r="G25" s="2">
-        <v>6501</v>
+        <v>6475</v>
       </c>
       <c r="H25" s="2">
         <v>2</v>
@@ -2551,18 +2551,18 @@
         <v>19670</v>
       </c>
       <c r="L25" s="2">
-        <v>10253</v>
+        <v>10276</v>
       </c>
       <c r="M25" s="2">
-        <v>3419</v>
+        <v>3171</v>
       </c>
       <c r="N25" s="8">
         <f t="shared" si="0"/>
-        <v>1.4230395558639835</v>
+        <v>1.4213001383125865</v>
       </c>
       <c r="O25" s="8">
         <f t="shared" si="1"/>
-        <v>0.52591908937086607</v>
+        <v>0.48972972972972972</v>
       </c>
       <c r="P25" s="2">
         <v>0</v>
@@ -2577,18 +2577,18 @@
         <v>13542</v>
       </c>
       <c r="T25" s="2">
-        <v>10405</v>
+        <v>10376</v>
       </c>
       <c r="U25" s="2">
-        <v>2950</v>
+        <v>2925</v>
       </c>
       <c r="V25" s="8">
         <f t="shared" si="2"/>
-        <v>1.4441360166551007</v>
+        <v>1.4351313969571231</v>
       </c>
       <c r="W25" s="9">
         <f t="shared" si="3"/>
-        <v>0.4537763421012152</v>
+        <v>0.45173745173745172</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
@@ -2608,10 +2608,10 @@
         <v>10632</v>
       </c>
       <c r="F26" s="2">
-        <v>9754</v>
+        <v>9782</v>
       </c>
       <c r="G26" s="2">
-        <v>8573</v>
+        <v>8505</v>
       </c>
       <c r="H26" s="2">
         <v>0</v>
@@ -2626,18 +2626,18 @@
         <v>6053</v>
       </c>
       <c r="L26" s="2">
-        <v>4967</v>
+        <v>4959</v>
       </c>
       <c r="M26" s="2">
-        <v>1670</v>
+        <v>1667</v>
       </c>
       <c r="N26" s="8">
         <f t="shared" si="0"/>
-        <v>0.50922698380151732</v>
+        <v>0.506951543651605</v>
       </c>
       <c r="O26" s="8">
         <f t="shared" si="1"/>
-        <v>0.19479762043625334</v>
+        <v>0.1960023515579071</v>
       </c>
       <c r="P26" s="2">
         <v>0</v>
@@ -2652,18 +2652,18 @@
         <v>1468</v>
       </c>
       <c r="T26" s="2">
-        <v>5024</v>
+        <v>5029</v>
       </c>
       <c r="U26" s="2">
-        <v>1633</v>
+        <v>1626</v>
       </c>
       <c r="V26" s="8">
         <f t="shared" si="2"/>
-        <v>0.51507074020914501</v>
+        <v>0.51410754446943363</v>
       </c>
       <c r="W26" s="9">
         <f t="shared" si="3"/>
-        <v>0.19048174501341419</v>
+        <v>0.19118165784832453</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
@@ -2833,10 +2833,10 @@
         <v>0</v>
       </c>
       <c r="F29" s="2">
-        <v>4680</v>
+        <v>3975</v>
       </c>
       <c r="G29" s="2">
-        <v>3922</v>
+        <v>3351</v>
       </c>
       <c r="H29" s="2">
         <v>0</v>
@@ -2851,18 +2851,18 @@
         <v>3009</v>
       </c>
       <c r="L29" s="2">
-        <v>1886</v>
+        <v>1893</v>
       </c>
       <c r="M29" s="2">
-        <v>1217</v>
+        <v>1233</v>
       </c>
       <c r="N29" s="8">
         <f t="shared" si="0"/>
-        <v>0.402991452991453</v>
+        <v>0.47622641509433961</v>
       </c>
       <c r="O29" s="8">
         <f t="shared" si="1"/>
-        <v>0.31030086690464048</v>
+        <v>0.36794986571172783</v>
       </c>
       <c r="P29" s="2">
         <v>0</v>
@@ -2877,18 +2877,18 @@
         <v>0</v>
       </c>
       <c r="T29" s="2">
-        <v>1934</v>
+        <v>1916</v>
       </c>
       <c r="U29" s="2">
-        <v>1363</v>
+        <v>1358</v>
       </c>
       <c r="V29" s="8">
         <f t="shared" si="2"/>
-        <v>0.41324786324786322</v>
+        <v>0.48201257861635222</v>
       </c>
       <c r="W29" s="9">
         <f t="shared" si="3"/>
-        <v>0.34752677205507393</v>
+        <v>0.40525216353327365</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
@@ -3068,19 +3068,19 @@
       </c>
       <c r="N33" s="10">
         <f>AVERAGE(N6:N31)</f>
-        <v>0.50422994220586037</v>
+        <v>0.51025798323665739</v>
       </c>
       <c r="O33" s="10">
         <f>AVERAGE(O6:O31)</f>
-        <v>0.32262051489831578</v>
+        <v>0.32325925672396649</v>
       </c>
       <c r="V33" s="10">
         <f>AVERAGE(V6:V31)</f>
-        <v>0.59962052488703921</v>
+        <v>0.60510632683870269</v>
       </c>
       <c r="W33" s="10">
         <f>AVERAGE(W6:W31)</f>
-        <v>0.33512771748484116</v>
+        <v>0.33813483250017856</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
@@ -3089,19 +3089,19 @@
       </c>
       <c r="N34" s="15">
         <f>AVERAGE(N2:N31)</f>
-        <v>0.54063083784661348</v>
+        <v>0.54585514007330416</v>
       </c>
       <c r="O34" s="15">
         <f>AVERAGE(O2:O31)</f>
-        <v>0.37806958299638999</v>
+        <v>0.37862315924528728</v>
       </c>
       <c r="V34" s="15">
         <f>AVERAGE(V2:V31)</f>
-        <v>0.70045452580441536</v>
+        <v>0.70520888749585686</v>
       </c>
       <c r="W34" s="15">
         <f>AVERAGE(W2:W31)</f>
-        <v>0.42021238717919773</v>
+        <v>0.42281855352582354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved accuracy and performance of arc functions.
git-svn-id: https://svn.code.sf.net/p/half/code/branches/clean@366 ba856b29-48f5-46b1-a3e5-b459205bce89
</commit_message>
<xml_diff>
--- a/test/results.xlsx
+++ b/test/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Nh</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>all</t>
+  </si>
+  <si>
+    <t>lgamma</t>
+  </si>
+  <si>
+    <t>tgamma</t>
   </si>
 </sst>
 </file>
@@ -222,7 +228,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -333,15 +339,6 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -378,12 +375,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -394,13 +439,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,13 +467,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF66FF66"/>
+      <color rgb="FFFF5050"/>
+      <color rgb="FFFFCC66"/>
+      <color rgb="FFFFFF66"/>
+      <color rgb="FFCCFF33"/>
+      <color rgb="FFFFFF99"/>
       <color rgb="FF99FF99"/>
-      <color rgb="FFCCFF99"/>
+      <color rgb="FF66FF33"/>
+      <color rgb="FF00FF00"/>
       <color rgb="FFFFFFCC"/>
-      <color rgb="FF99FF66"/>
-      <color rgb="FF66FF33"/>
-      <color rgb="FFFFFF99"/>
-      <color rgb="FF00FF00"/>
     </mruColors>
   </colors>
   <extLst>
@@ -714,7 +774,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W34"/>
+  <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -907,11 +967,11 @@
         <v>2294</v>
       </c>
       <c r="N3" s="8">
-        <f t="shared" ref="N3:N31" si="0">L3/F3</f>
+        <f t="shared" ref="N3:N33" si="0">L3/F3</f>
         <v>0.48485287722858383</v>
       </c>
       <c r="O3" s="8">
-        <f t="shared" ref="O3:O31" si="1">M3/G3</f>
+        <f t="shared" ref="O3:O33" si="1">M3/G3</f>
         <v>0.56266862889379443</v>
       </c>
       <c r="P3" s="2">
@@ -933,11 +993,11 @@
         <v>2649</v>
       </c>
       <c r="V3" s="8">
-        <f t="shared" ref="V3:V31" si="2">T3/F3</f>
+        <f t="shared" ref="V3:V33" si="2">T3/F3</f>
         <v>0.89897086534280335</v>
       </c>
       <c r="W3" s="9">
-        <f t="shared" ref="W3:W31" si="3">U3/G3</f>
+        <f t="shared" ref="W3:W33" si="3">U3/G3</f>
         <v>0.64974245768947758</v>
       </c>
     </row>
@@ -2149,19 +2209,19 @@
         <v>0</v>
       </c>
       <c r="C20" s="2">
-        <v>3788</v>
+        <v>4</v>
       </c>
       <c r="D20" s="2">
-        <v>6907</v>
+        <v>4</v>
       </c>
       <c r="E20" s="2">
-        <v>6907</v>
+        <v>4</v>
       </c>
       <c r="F20" s="2">
-        <v>4303</v>
+        <v>4060</v>
       </c>
       <c r="G20" s="2">
-        <v>4188</v>
+        <v>3836</v>
       </c>
       <c r="H20" s="2">
         <v>0</v>
@@ -2176,18 +2236,18 @@
         <v>4057</v>
       </c>
       <c r="L20" s="2">
-        <v>742</v>
+        <v>768</v>
       </c>
       <c r="M20" s="2">
-        <v>725</v>
+        <v>749</v>
       </c>
       <c r="N20" s="8">
         <f t="shared" si="0"/>
-        <v>0.172437834069254</v>
+        <v>0.18916256157635469</v>
       </c>
       <c r="O20" s="8">
         <f t="shared" si="1"/>
-        <v>0.17311365807067813</v>
+        <v>0.19525547445255476</v>
       </c>
       <c r="P20" s="2">
         <v>0</v>
@@ -2202,18 +2262,18 @@
         <v>0</v>
       </c>
       <c r="T20" s="2">
-        <v>948</v>
+        <v>953</v>
       </c>
       <c r="U20" s="2">
-        <v>832</v>
+        <v>845</v>
       </c>
       <c r="V20" s="8">
         <f t="shared" si="2"/>
-        <v>0.22031141064373694</v>
+        <v>0.23472906403940888</v>
       </c>
       <c r="W20" s="9">
         <f t="shared" si="3"/>
-        <v>0.19866284622731614</v>
+        <v>0.22028154327424401</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
@@ -2233,10 +2293,10 @@
         <v>0</v>
       </c>
       <c r="F21" s="2">
-        <v>4027</v>
+        <v>3842</v>
       </c>
       <c r="G21" s="2">
-        <v>4058</v>
+        <v>3768</v>
       </c>
       <c r="H21" s="2">
         <v>3</v>
@@ -2251,18 +2311,18 @@
         <v>1</v>
       </c>
       <c r="L21" s="2">
-        <v>787</v>
+        <v>793</v>
       </c>
       <c r="M21" s="2">
-        <v>802</v>
+        <v>808</v>
       </c>
       <c r="N21" s="8">
         <f t="shared" si="0"/>
-        <v>0.19543084181773032</v>
+        <v>0.20640291514836023</v>
       </c>
       <c r="O21" s="8">
         <f t="shared" si="1"/>
-        <v>0.1976343026121242</v>
+        <v>0.21443736730360935</v>
       </c>
       <c r="P21" s="2">
         <v>0</v>
@@ -2277,18 +2337,18 @@
         <v>0</v>
       </c>
       <c r="T21" s="2">
-        <v>972</v>
+        <v>983</v>
       </c>
       <c r="U21" s="2">
         <v>825</v>
       </c>
       <c r="V21" s="8">
         <f t="shared" si="2"/>
-        <v>0.2413707474546809</v>
+        <v>0.25585632483081727</v>
       </c>
       <c r="W21" s="9">
         <f t="shared" si="3"/>
-        <v>0.20330211927057665</v>
+        <v>0.21894904458598727</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
@@ -2296,22 +2356,22 @@
         <v>42</v>
       </c>
       <c r="B22" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C22" s="2">
-        <v>6706</v>
+        <v>720</v>
       </c>
       <c r="D22" s="2">
-        <v>5387</v>
+        <v>720</v>
       </c>
       <c r="E22" s="2">
-        <v>5387</v>
+        <v>720</v>
       </c>
       <c r="F22" s="2">
-        <v>6037</v>
+        <v>5624</v>
       </c>
       <c r="G22" s="2">
-        <v>5762</v>
+        <v>5243</v>
       </c>
       <c r="H22" s="2">
         <v>6</v>
@@ -2326,18 +2386,18 @@
         <v>3525</v>
       </c>
       <c r="L22" s="2">
-        <v>2236</v>
+        <v>2195</v>
       </c>
       <c r="M22" s="2">
-        <v>1729</v>
+        <v>1726</v>
       </c>
       <c r="N22" s="8">
         <f t="shared" si="0"/>
-        <v>0.37038264038429686</v>
+        <v>0.39029160739687058</v>
       </c>
       <c r="O22" s="8">
         <f t="shared" si="1"/>
-        <v>0.30006942034015965</v>
+        <v>0.32920083921419035</v>
       </c>
       <c r="P22" s="2">
         <v>0</v>
@@ -2352,18 +2412,18 @@
         <v>0</v>
       </c>
       <c r="T22" s="2">
-        <v>2695</v>
+        <v>2694</v>
       </c>
       <c r="U22" s="2">
-        <v>1946</v>
+        <v>1949</v>
       </c>
       <c r="V22" s="8">
         <f t="shared" si="2"/>
-        <v>0.44641378167964219</v>
+        <v>0.47901849217638692</v>
       </c>
       <c r="W22" s="9">
         <f t="shared" si="3"/>
-        <v>0.33772995487677887</v>
+        <v>0.371733740225062</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
@@ -2931,11 +2991,11 @@
       <c r="M30" s="2">
         <v>1608</v>
       </c>
-      <c r="N30" s="8">
+      <c r="N30" s="15">
         <f t="shared" si="0"/>
         <v>0.42830916100605837</v>
       </c>
-      <c r="O30" s="8">
+      <c r="O30" s="15">
         <f t="shared" si="1"/>
         <v>0.21767970759442262</v>
       </c>
@@ -2957,156 +3017,468 @@
       <c r="U30" s="2">
         <v>1759</v>
       </c>
-      <c r="V30" s="8">
+      <c r="V30" s="15">
         <f t="shared" si="2"/>
         <v>0.53185239581420962</v>
       </c>
-      <c r="W30" s="9">
+      <c r="W30" s="16">
         <f t="shared" si="3"/>
         <v>0.23812102341952077</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="11" t="s">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="12">
+      <c r="B31" s="2">
         <v>164</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31" s="2">
         <v>185</v>
       </c>
-      <c r="D31" s="12">
+      <c r="D31" s="2">
         <v>185</v>
       </c>
-      <c r="E31" s="12">
+      <c r="E31" s="2">
         <v>185</v>
       </c>
-      <c r="F31" s="12">
+      <c r="F31" s="2">
         <v>5296</v>
       </c>
-      <c r="G31" s="12">
+      <c r="G31" s="2">
         <v>7450</v>
       </c>
-      <c r="H31" s="12">
+      <c r="H31" s="2">
         <v>2</v>
       </c>
-      <c r="I31" s="12">
+      <c r="I31" s="2">
         <v>14454</v>
       </c>
-      <c r="J31" s="12">
+      <c r="J31" s="2">
         <v>13053</v>
       </c>
-      <c r="K31" s="12">
+      <c r="K31" s="2">
         <v>14454</v>
       </c>
-      <c r="L31" s="12">
+      <c r="L31" s="2">
         <v>4979</v>
       </c>
-      <c r="M31" s="12">
+      <c r="M31" s="2">
         <v>2652</v>
       </c>
-      <c r="N31" s="13">
+      <c r="N31" s="15">
         <f t="shared" si="0"/>
         <v>0.94014350453172202</v>
       </c>
-      <c r="O31" s="13">
+      <c r="O31" s="15">
         <f t="shared" si="1"/>
         <v>0.35597315436241611</v>
       </c>
-      <c r="P31" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="12">
+      <c r="P31" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="2">
         <v>13867</v>
       </c>
-      <c r="R31" s="12">
+      <c r="R31" s="2">
         <v>11569</v>
       </c>
-      <c r="S31" s="12">
+      <c r="S31" s="2">
         <v>13867</v>
       </c>
-      <c r="T31" s="12">
+      <c r="T31" s="2">
         <v>5292</v>
       </c>
-      <c r="U31" s="12">
+      <c r="U31" s="2">
         <v>3064</v>
       </c>
-      <c r="V31" s="13">
+      <c r="V31" s="15">
         <f t="shared" si="2"/>
         <v>0.99924471299093653</v>
       </c>
-      <c r="W31" s="14">
+      <c r="W31" s="16">
         <f t="shared" si="3"/>
         <v>0.41127516778523487</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
+      <c r="A32" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="2">
+        <v>65536</v>
+      </c>
+      <c r="C32" s="2">
+        <v>65536</v>
+      </c>
+      <c r="D32" s="2">
+        <v>65536</v>
+      </c>
+      <c r="E32" s="2">
+        <v>65536</v>
+      </c>
+      <c r="F32" s="2">
+        <v>22222</v>
+      </c>
+      <c r="G32" s="2">
+        <v>22222</v>
+      </c>
+      <c r="H32" s="2">
+        <v>6</v>
+      </c>
+      <c r="I32" s="2">
+        <v>5</v>
+      </c>
+      <c r="J32" s="2">
+        <v>5</v>
+      </c>
+      <c r="K32" s="2">
+        <v>6</v>
+      </c>
+      <c r="L32" s="2">
+        <v>9084</v>
+      </c>
+      <c r="M32" s="2">
+        <v>5827</v>
+      </c>
+      <c r="N32" s="15">
+        <f t="shared" si="0"/>
+        <v>0.40878408784087839</v>
+      </c>
+      <c r="O32" s="15">
+        <f t="shared" si="1"/>
+        <v>0.26221762217622174</v>
+      </c>
+      <c r="P32" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="2">
+        <v>0</v>
+      </c>
+      <c r="R32" s="2">
+        <v>0</v>
+      </c>
+      <c r="S32" s="2">
+        <v>0</v>
+      </c>
+      <c r="T32" s="2">
+        <v>9800</v>
+      </c>
+      <c r="U32" s="2">
+        <v>7285</v>
+      </c>
+      <c r="V32" s="15">
+        <f t="shared" si="2"/>
+        <v>0.44100441004410046</v>
+      </c>
+      <c r="W32" s="16">
+        <f t="shared" si="3"/>
+        <v>0.32782827828278283</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="11">
+        <v>65536</v>
+      </c>
+      <c r="C33" s="11">
+        <v>65536</v>
+      </c>
+      <c r="D33" s="11">
+        <v>65536</v>
+      </c>
+      <c r="E33" s="11">
+        <v>65536</v>
+      </c>
+      <c r="F33" s="11">
+        <v>22222</v>
+      </c>
+      <c r="G33" s="11">
+        <v>22222</v>
+      </c>
+      <c r="H33" s="11">
+        <v>2</v>
+      </c>
+      <c r="I33" s="11">
+        <v>11169</v>
+      </c>
+      <c r="J33" s="11">
+        <v>1975</v>
+      </c>
+      <c r="K33" s="11">
+        <v>13140</v>
+      </c>
+      <c r="L33" s="11">
+        <v>9598</v>
+      </c>
+      <c r="M33" s="11">
+        <v>5366</v>
+      </c>
+      <c r="N33" s="12">
+        <f t="shared" si="0"/>
+        <v>0.43191431914319145</v>
+      </c>
+      <c r="O33" s="12">
+        <f t="shared" si="1"/>
+        <v>0.24147241472414724</v>
+      </c>
+      <c r="P33" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="11">
+        <v>8867</v>
+      </c>
+      <c r="R33" s="11">
+        <v>927</v>
+      </c>
+      <c r="S33" s="11">
+        <v>9794</v>
+      </c>
+      <c r="T33" s="11">
+        <v>22644</v>
+      </c>
+      <c r="U33" s="11">
+        <v>15498</v>
+      </c>
+      <c r="V33" s="12">
+        <f t="shared" si="2"/>
+        <v>1.0189901899018989</v>
+      </c>
+      <c r="W33" s="13">
+        <f t="shared" si="3"/>
+        <v>0.69741697416974169</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A34" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="N32" s="10">
+      <c r="B34" s="26">
+        <f>COUNTIF(B2:B5,"=0")/4</f>
+        <v>1</v>
+      </c>
+      <c r="C34" s="26">
+        <f t="shared" ref="C34:E34" si="4">COUNTIF(C2:C5,"=0")/4</f>
+        <v>1</v>
+      </c>
+      <c r="D34" s="26">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E34" s="26">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="26">
+        <f>COUNTIF(H2:H5,"=0")/4</f>
+        <v>1</v>
+      </c>
+      <c r="I34" s="26">
+        <f t="shared" ref="I34:K34" si="5">COUNTIF(I2:I5,"=0")/4</f>
+        <v>0.5</v>
+      </c>
+      <c r="J34" s="26">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="K34" s="26">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="17">
         <f>AVERAGE(N2:N5)</f>
         <v>0.77723665951150944</v>
       </c>
-      <c r="O32" s="10">
+      <c r="O34" s="17">
         <f>AVERAGE(O2:O5)</f>
         <v>0.73848852563387224</v>
       </c>
-      <c r="V32" s="10">
+      <c r="P34" s="26">
+        <f>COUNTIF(P2:P5,"=0")/4</f>
+        <v>1</v>
+      </c>
+      <c r="Q34" s="26">
+        <f t="shared" ref="Q34:S34" si="6">COUNTIF(Q2:Q5,"=0")/4</f>
+        <v>1</v>
+      </c>
+      <c r="R34" s="26">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="S34" s="26">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="17">
         <f>AVERAGE(V2:V5)</f>
         <v>1.3558755317673605</v>
       </c>
-      <c r="W32" s="10">
+      <c r="W34" s="18">
         <f>AVERAGE(W2:W5)</f>
         <v>0.97326274019251668</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A35" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="N33" s="10">
-        <f>AVERAGE(N6:N31)</f>
-        <v>0.51025798323665739</v>
-      </c>
-      <c r="O33" s="10">
-        <f>AVERAGE(O6:O31)</f>
-        <v>0.32325925672396649</v>
-      </c>
-      <c r="V33" s="10">
-        <f>AVERAGE(V6:V31)</f>
-        <v>0.60510632683870269</v>
-      </c>
-      <c r="W33" s="10">
-        <f>AVERAGE(W6:W31)</f>
-        <v>0.33813483250017856</v>
+      <c r="B35" s="27">
+        <f>COUNTIF(B6:B33,"=0")/28</f>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="C35" s="27">
+        <f t="shared" ref="C35:E35" si="7">COUNTIF(C6:C33,"=0")/28</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="D35" s="27">
+        <f t="shared" si="7"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="E35" s="27">
+        <f t="shared" si="7"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="27">
+        <f>COUNTIF(H6:H33,"=0")/28</f>
+        <v>0.17857142857142858</v>
+      </c>
+      <c r="I35" s="27">
+        <f t="shared" ref="I35:K35" si="8">COUNTIF(I6:I33,"=0")/28</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="J35" s="27">
+        <f t="shared" si="8"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="K35" s="27">
+        <f t="shared" si="8"/>
+        <v>0.10714285714285714</v>
+      </c>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="19">
+        <f>AVERAGE(N6:N33)</f>
+        <v>0.50553613353526672</v>
+      </c>
+      <c r="O35" s="19">
+        <f>AVERAGE(O6:O33)</f>
+        <v>0.32058953613110319</v>
+      </c>
+      <c r="P35" s="27">
+        <f>COUNTIF(P6:P33,"=0")/28</f>
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="Q35" s="27">
+        <f t="shared" ref="Q35:S35" si="9">COUNTIF(Q6:Q33,"=0")/28</f>
+        <v>0.6071428571428571</v>
+      </c>
+      <c r="R35" s="27">
+        <f t="shared" si="9"/>
+        <v>0.6428571428571429</v>
+      </c>
+      <c r="S35" s="27">
+        <f t="shared" si="9"/>
+        <v>0.6071428571428571</v>
+      </c>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="19">
+        <f>AVERAGE(V6:V33)</f>
+        <v>0.61622382282217214</v>
+      </c>
+      <c r="W35" s="20">
+        <f>AVERAGE(W6:W33)</f>
+        <v>0.35314358232742105</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A36" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="N34" s="15">
-        <f>AVERAGE(N2:N31)</f>
-        <v>0.54585514007330416</v>
-      </c>
-      <c r="O34" s="15">
-        <f>AVERAGE(O2:O31)</f>
-        <v>0.37862315924528728</v>
-      </c>
-      <c r="V34" s="15">
-        <f>AVERAGE(V2:V31)</f>
-        <v>0.70520888749585686</v>
-      </c>
-      <c r="W34" s="15">
-        <f>AVERAGE(W2:W31)</f>
-        <v>0.42281855352582354</v>
+      <c r="B36" s="28">
+        <f>COUNTIF(B2:B33,"=0")/32</f>
+        <v>0.75</v>
+      </c>
+      <c r="C36" s="28">
+        <f t="shared" ref="C36:E36" si="10">COUNTIF(C2:C33,"=0")/32</f>
+        <v>0.5</v>
+      </c>
+      <c r="D36" s="28">
+        <f t="shared" si="10"/>
+        <v>0.5</v>
+      </c>
+      <c r="E36" s="28">
+        <f t="shared" si="10"/>
+        <v>0.5</v>
+      </c>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="28">
+        <f>COUNTIF(H2:H33,"=0")/32</f>
+        <v>0.28125</v>
+      </c>
+      <c r="I36" s="28">
+        <f t="shared" ref="I36:K36" si="11">COUNTIF(I2:I33,"=0")/32</f>
+        <v>0.1875</v>
+      </c>
+      <c r="J36" s="28">
+        <f t="shared" si="11"/>
+        <v>0.1875</v>
+      </c>
+      <c r="K36" s="28">
+        <f t="shared" si="11"/>
+        <v>0.15625</v>
+      </c>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="21">
+        <f>AVERAGE(N2:N33)</f>
+        <v>0.53949869928229699</v>
+      </c>
+      <c r="O36" s="21">
+        <f>AVERAGE(O2:O33)</f>
+        <v>0.37282690981894934</v>
+      </c>
+      <c r="P36" s="28">
+        <f>COUNTIF(P2:P33,"=0")/32</f>
+        <v>0.9375</v>
+      </c>
+      <c r="Q36" s="28">
+        <f t="shared" ref="Q36:S36" si="12">COUNTIF(Q2:Q33,"=0")/32</f>
+        <v>0.65625</v>
+      </c>
+      <c r="R36" s="28">
+        <f t="shared" si="12"/>
+        <v>0.6875</v>
+      </c>
+      <c r="S36" s="28">
+        <f t="shared" si="12"/>
+        <v>0.65625</v>
+      </c>
+      <c r="T36" s="14"/>
+      <c r="U36" s="14"/>
+      <c r="V36" s="21">
+        <f>AVERAGE(V2:V33)</f>
+        <v>0.70868028644032055</v>
+      </c>
+      <c r="W36" s="22">
+        <f>AVERAGE(W2:W33)</f>
+        <v>0.43065847706055793</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="N2:O34 V2:W34">
-    <cfRule type="dataBar" priority="5">
+  <conditionalFormatting sqref="N2:O36 V2:W36">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3120,7 +3492,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:E5 H2:K5 P2:S5">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3132,7 +3504,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:E16 B23:E23 H15:K16 H23:K23 P15:S16 P23:S23">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3143,8 +3515,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:E14 H6:K14 P6:S14 B17:E22 H17:K22 P17:S22 B24:E31 H24:K31 P24:S31">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="B6:E14 H6:K14 P6:S14 B17:E22 H17:K22 P17:S22 H24:K33 P24:S33 B24:E33">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3155,8 +3527,25 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B34:E36 H34:K36 P34:S36">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FF66FF66"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D4AEBDF6-16F3-4574-8AF5-06B7A23DFE16}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B34 C34:S34 B35:S36" formulaRange="1"/>
+  </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -3173,7 +3562,22 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>N2:O34 V2:W34</xm:sqref>
+          <xm:sqref>N2:O36 V2:W36</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D4AEBDF6-16F3-4574-8AF5-06B7A23DFE16}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B34:E36 H34:K36 P34:S36</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Improved accuracy of tanh and expm1 functions.
git-svn-id: https://svn.code.sf.net/p/half/code/branches/clean@368 ba856b29-48f5-46b1-a3e5-b459205bce89
</commit_message>
<xml_diff>
--- a/test/results.xlsx
+++ b/test/results.xlsx
@@ -211,7 +211,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,13 +234,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="16">
@@ -439,11 +451,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -473,8 +486,10 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1266,12 +1281,12 @@
         <v>0</v>
       </c>
       <c r="F6" s="2">
-        <v>7628</v>
+        <v>6371</v>
       </c>
       <c r="G6" s="2">
         <v>7131</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="29">
         <v>6190</v>
       </c>
       <c r="I6" s="2">
@@ -1287,21 +1302,21 @@
         <v>9848</v>
       </c>
       <c r="M6" s="2">
-        <v>2138</v>
+        <v>2176</v>
       </c>
       <c r="N6" s="2">
-        <v>2353</v>
+        <v>2255</v>
       </c>
       <c r="O6" s="1">
         <v>1157</v>
       </c>
       <c r="P6" s="8">
         <f t="shared" si="0"/>
-        <v>0.28028316727844782</v>
+        <v>0.34154763773347985</v>
       </c>
       <c r="Q6" s="8">
         <f t="shared" si="1"/>
-        <v>0.32996774645912214</v>
+        <v>0.31622493338942642</v>
       </c>
       <c r="R6" s="8">
         <f t="shared" si="2"/>
@@ -1320,21 +1335,21 @@
         <v>6772</v>
       </c>
       <c r="W6" s="2">
-        <v>2611</v>
+        <v>2709</v>
       </c>
       <c r="X6" s="2">
-        <v>2322</v>
+        <v>2474</v>
       </c>
       <c r="Y6" s="1">
         <v>1514</v>
       </c>
       <c r="Z6" s="8">
         <f t="shared" si="3"/>
-        <v>0.34229155742003148</v>
+        <v>0.42520797363051327</v>
       </c>
       <c r="AA6" s="9">
         <f t="shared" si="4"/>
-        <v>0.32562053007993269</v>
+        <v>0.34693591361660359</v>
       </c>
       <c r="AB6" s="9">
         <f t="shared" si="5"/>
@@ -1358,12 +1373,12 @@
         <v>0</v>
       </c>
       <c r="F7" s="2">
-        <v>5054</v>
+        <v>4807</v>
       </c>
       <c r="G7" s="2">
         <v>5292</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="29">
         <v>4740</v>
       </c>
       <c r="I7" s="2">
@@ -1379,21 +1394,21 @@
         <v>9218</v>
       </c>
       <c r="M7" s="2">
-        <v>8104</v>
+        <v>8173</v>
       </c>
       <c r="N7" s="2">
-        <v>4548</v>
+        <v>4664</v>
       </c>
       <c r="O7" s="1">
         <v>3138</v>
       </c>
       <c r="P7" s="8">
         <f t="shared" si="0"/>
-        <v>1.6034823901859914</v>
+        <v>1.700228832951945</v>
       </c>
       <c r="Q7" s="8">
         <f t="shared" si="1"/>
-        <v>0.85941043083900226</v>
+        <v>0.88133030990173844</v>
       </c>
       <c r="R7" s="8">
         <f t="shared" si="2"/>
@@ -1412,21 +1427,21 @@
         <v>6144</v>
       </c>
       <c r="W7" s="2">
-        <v>7270</v>
+        <v>7364</v>
       </c>
       <c r="X7" s="2">
-        <v>4434</v>
+        <v>4589</v>
       </c>
       <c r="Y7" s="1">
         <v>3433</v>
       </c>
       <c r="Z7" s="8">
         <f t="shared" si="3"/>
-        <v>1.4384645825089037</v>
+        <v>1.5319325982941543</v>
       </c>
       <c r="AA7" s="9">
         <f t="shared" si="4"/>
-        <v>0.83786848072562359</v>
+        <v>0.86715797430083141</v>
       </c>
       <c r="AB7" s="9">
         <f t="shared" si="5"/>
@@ -1441,51 +1456,51 @@
         <v>20</v>
       </c>
       <c r="C8" s="2">
-        <v>9899</v>
+        <v>310</v>
       </c>
       <c r="D8" s="2">
-        <v>10180</v>
+        <v>591</v>
       </c>
       <c r="E8" s="2">
         <v>310</v>
       </c>
       <c r="F8" s="2">
-        <v>9146</v>
+        <v>7271</v>
       </c>
       <c r="G8" s="2">
         <v>8932</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="29">
         <v>7931</v>
       </c>
       <c r="I8" s="2">
         <v>2</v>
       </c>
       <c r="J8" s="2">
-        <v>12460</v>
+        <v>22049</v>
       </c>
       <c r="K8" s="2">
-        <v>2615</v>
+        <v>12205</v>
       </c>
       <c r="L8" s="2">
         <v>9846</v>
       </c>
       <c r="M8" s="2">
-        <v>4924</v>
+        <v>4921</v>
       </c>
       <c r="N8" s="2">
-        <v>2763</v>
+        <v>2693</v>
       </c>
       <c r="O8" s="1">
         <v>1456</v>
       </c>
       <c r="P8" s="8">
         <f t="shared" si="0"/>
-        <v>0.53837743275748962</v>
+        <v>0.67679823958190066</v>
       </c>
       <c r="Q8" s="8">
         <f t="shared" si="1"/>
-        <v>0.30933721450962831</v>
+        <v>0.30150022391401704</v>
       </c>
       <c r="R8" s="8">
         <f t="shared" si="2"/>
@@ -1495,30 +1510,30 @@
         <v>0</v>
       </c>
       <c r="T8" s="2">
-        <v>8273</v>
+        <v>17862</v>
       </c>
       <c r="U8" s="2">
-        <v>1501</v>
+        <v>11090</v>
       </c>
       <c r="V8" s="2">
         <v>6772</v>
       </c>
       <c r="W8" s="2">
-        <v>4422</v>
+        <v>4521</v>
       </c>
       <c r="X8" s="2">
-        <v>2497</v>
+        <v>2579</v>
       </c>
       <c r="Y8" s="1">
         <v>1694</v>
       </c>
       <c r="Z8" s="8">
         <f t="shared" si="3"/>
-        <v>0.48349005029521103</v>
+        <v>0.62178517397881994</v>
       </c>
       <c r="AA8" s="9">
         <f t="shared" si="4"/>
-        <v>0.27955665024630544</v>
+        <v>0.28873712494402148</v>
       </c>
       <c r="AB8" s="9">
         <f t="shared" si="5"/>
@@ -3097,51 +3112,51 @@
         <v>0</v>
       </c>
       <c r="C26" s="2">
-        <v>21256</v>
+        <v>0</v>
       </c>
       <c r="D26" s="2">
-        <v>10632</v>
+        <v>0</v>
       </c>
       <c r="E26" s="2">
-        <v>10632</v>
+        <v>0</v>
       </c>
       <c r="F26" s="2">
-        <v>9782</v>
+        <v>5547</v>
       </c>
       <c r="G26" s="2">
-        <v>8505</v>
-      </c>
-      <c r="H26" s="2">
+        <v>5219</v>
+      </c>
+      <c r="H26" s="29">
         <v>7375</v>
       </c>
       <c r="I26" s="2">
         <v>0</v>
       </c>
       <c r="J26" s="2">
-        <v>12164</v>
+        <v>33412</v>
       </c>
       <c r="K26" s="2">
-        <v>6083</v>
+        <v>16707</v>
       </c>
       <c r="L26" s="2">
-        <v>6053</v>
+        <v>16707</v>
       </c>
       <c r="M26" s="2">
-        <v>4959</v>
+        <v>5134</v>
       </c>
       <c r="N26" s="2">
-        <v>1667</v>
+        <v>1740</v>
       </c>
       <c r="O26" s="1">
         <v>803</v>
       </c>
       <c r="P26" s="8">
         <f t="shared" si="0"/>
-        <v>0.506951543651605</v>
+        <v>0.92554533982332787</v>
       </c>
       <c r="Q26" s="8">
         <f t="shared" si="1"/>
-        <v>0.1960023515579071</v>
+        <v>0.33339720252922017</v>
       </c>
       <c r="R26" s="8">
         <f t="shared" si="2"/>
@@ -3151,30 +3166,30 @@
         <v>0</v>
       </c>
       <c r="T26" s="2">
-        <v>2936</v>
+        <v>24184</v>
       </c>
       <c r="U26" s="2">
-        <v>1468</v>
+        <v>12092</v>
       </c>
       <c r="V26" s="2">
-        <v>1468</v>
+        <v>12097</v>
       </c>
       <c r="W26" s="2">
-        <v>5029</v>
+        <v>5190</v>
       </c>
       <c r="X26" s="2">
-        <v>1626</v>
+        <v>1717</v>
       </c>
       <c r="Y26" s="1">
         <v>1170</v>
       </c>
       <c r="Z26" s="8">
         <f t="shared" si="3"/>
-        <v>0.51410754446943363</v>
+        <v>0.93564088696592751</v>
       </c>
       <c r="AA26" s="9">
         <f t="shared" si="4"/>
-        <v>0.19118165784832453</v>
+        <v>0.3289902280130293</v>
       </c>
       <c r="AB26" s="9">
         <f t="shared" si="5"/>
@@ -3921,15 +3936,15 @@
       </c>
       <c r="C35" s="27">
         <f t="shared" ref="C35:E35" si="9">COUNTIF(C6:C33,"=0")/28</f>
-        <v>0.42857142857142855</v>
+        <v>0.4642857142857143</v>
       </c>
       <c r="D35" s="27">
         <f t="shared" si="9"/>
-        <v>0.42857142857142855</v>
+        <v>0.4642857142857143</v>
       </c>
       <c r="E35" s="27">
         <f t="shared" si="9"/>
-        <v>0.42857142857142855</v>
+        <v>0.4642857142857143</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -3955,11 +3970,11 @@
       <c r="O35" s="2"/>
       <c r="P35" s="19">
         <f>AVERAGE(P6:P33)</f>
-        <v>0.50629338411818769</v>
+        <v>0.53183000969737049</v>
       </c>
       <c r="Q35" s="19">
         <f>AVERAGE(Q6:Q33)</f>
-        <v>0.32093137801426624</v>
+        <v>0.32585048252743559</v>
       </c>
       <c r="R35" s="19">
         <f>AVERAGE(R6:R33)</f>
@@ -3986,11 +4001,11 @@
       <c r="Y35" s="2"/>
       <c r="Z35" s="19">
         <f>AVERAGE(Z6:Z33)</f>
-        <v>0.61719541001016953</v>
+        <v>0.6434887278021636</v>
       </c>
       <c r="AA35" s="20">
         <f>AVERAGE(AA6:AA33)</f>
-        <v>0.35344522032829023</v>
+        <v>0.36050214611308667</v>
       </c>
       <c r="AB35" s="20">
         <f>AVERAGE(AB6:AB33)</f>
@@ -4007,15 +4022,15 @@
       </c>
       <c r="C36" s="28">
         <f t="shared" ref="C36:E36" si="12">COUNTIF(C2:C33,"=0")/32</f>
-        <v>0.5</v>
+        <v>0.53125</v>
       </c>
       <c r="D36" s="28">
         <f t="shared" si="12"/>
-        <v>0.5</v>
+        <v>0.53125</v>
       </c>
       <c r="E36" s="28">
         <f t="shared" si="12"/>
-        <v>0.5</v>
+        <v>0.53125</v>
       </c>
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>
@@ -4041,11 +4056,11 @@
       <c r="O36" s="14"/>
       <c r="P36" s="21">
         <f>AVERAGE(P2:P33)</f>
-        <v>0.54166757487432038</v>
+        <v>0.56401212225610542</v>
       </c>
       <c r="Q36" s="21">
         <f>AVERAGE(Q2:Q33)</f>
-        <v>0.3735039304803825</v>
+        <v>0.37780814692940567</v>
       </c>
       <c r="R36" s="21">
         <f>AVERAGE(R2:R33)</f>
@@ -4072,11 +4087,11 @@
       <c r="Y36" s="14"/>
       <c r="Z36" s="21">
         <f>AVERAGE(Z2:Z33)</f>
-        <v>0.71215725143476327</v>
+        <v>0.73516390450275815</v>
       </c>
       <c r="AA36" s="22">
         <f>AVERAGE(AA2:AA33)</f>
-        <v>0.43013453600444429</v>
+        <v>0.43630934606614125</v>
       </c>
       <c r="AB36" s="22">
         <f>AVERAGE(AB2:AB33)</f>

</xml_diff>

<commit_message>
Improved accuracy of asin function.
git-svn-id: https://svn.code.sf.net/p/half/code/branches/clean@369 ba856b29-48f5-46b1-a3e5-b459205bce89
</commit_message>
<xml_diff>
--- a/test/results.xlsx
+++ b/test/results.xlsx
@@ -2560,13 +2560,13 @@
         <v>0</v>
       </c>
       <c r="C20" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D20" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E20" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F20" s="2">
         <v>4060</v>
@@ -3936,15 +3936,15 @@
       </c>
       <c r="C35" s="27">
         <f t="shared" ref="C35:E35" si="9">COUNTIF(C6:C33,"=0")/28</f>
-        <v>0.4642857142857143</v>
+        <v>0.5</v>
       </c>
       <c r="D35" s="27">
         <f t="shared" si="9"/>
-        <v>0.4642857142857143</v>
+        <v>0.5</v>
       </c>
       <c r="E35" s="27">
         <f t="shared" si="9"/>
-        <v>0.4642857142857143</v>
+        <v>0.5</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -4022,15 +4022,15 @@
       </c>
       <c r="C36" s="28">
         <f t="shared" ref="C36:E36" si="12">COUNTIF(C2:C33,"=0")/32</f>
-        <v>0.53125</v>
+        <v>0.5625</v>
       </c>
       <c r="D36" s="28">
         <f t="shared" si="12"/>
-        <v>0.53125</v>
+        <v>0.5625</v>
       </c>
       <c r="E36" s="28">
         <f t="shared" si="12"/>
-        <v>0.53125</v>
+        <v>0.5625</v>
       </c>
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>

</xml_diff>

<commit_message>
Improved accuracy of sinh function.
git-svn-id: https://svn.code.sf.net/p/half/code/branches/clean@370 ba856b29-48f5-46b1-a3e5-b459205bce89
</commit_message>
<xml_diff>
--- a/test/results.xlsx
+++ b/test/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>Nh</t>
   </si>
@@ -180,9 +180,6 @@
     <t>ops</t>
   </si>
   <si>
-    <t>funcs</t>
-  </si>
-  <si>
     <t>all</t>
   </si>
   <si>
@@ -205,6 +202,21 @@
   </si>
   <si>
     <t>F16Cd%</t>
+  </si>
+  <si>
+    <t>fmod</t>
+  </si>
+  <si>
+    <t>remainder</t>
+  </si>
+  <si>
+    <t>fma</t>
+  </si>
+  <si>
+    <t>functions</t>
+  </si>
+  <si>
+    <t>fdim</t>
   </si>
 </sst>
 </file>
@@ -456,7 +468,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -477,7 +489,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -497,16 +508,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFFCC"/>
+      <color rgb="FF99FF99"/>
       <color rgb="FF66FF66"/>
       <color rgb="FFFF5050"/>
       <color rgb="FFFFCC66"/>
       <color rgb="FFFFFF66"/>
       <color rgb="FFCCFF33"/>
       <color rgb="FFFFFF99"/>
-      <color rgb="FF99FF99"/>
       <color rgb="FF66FF33"/>
       <color rgb="FF00FF00"/>
-      <color rgb="FFFFFFCC"/>
     </mruColors>
   </colors>
   <extLst>
@@ -804,11 +815,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB36"/>
+  <dimension ref="A1:AB40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
@@ -833,7 +847,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>6</v>
@@ -854,7 +868,7 @@
         <v>12</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>18</v>
@@ -863,7 +877,7 @@
         <v>19</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S1" s="4" t="s">
         <v>13</v>
@@ -884,7 +898,7 @@
         <v>17</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Z1" s="4" t="s">
         <v>20</v>
@@ -893,7 +907,7 @@
         <v>21</v>
       </c>
       <c r="AB1" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -925,13 +939,13 @@
         <v>0</v>
       </c>
       <c r="J2" s="1">
-        <v>22597</v>
+        <v>92246016</v>
       </c>
       <c r="K2" s="1">
-        <v>22669</v>
+        <v>92258304</v>
       </c>
       <c r="L2" s="1">
-        <v>22532</v>
+        <v>92258304</v>
       </c>
       <c r="M2" s="1">
         <v>3315</v>
@@ -1017,13 +1031,13 @@
         <v>0</v>
       </c>
       <c r="J3" s="2">
-        <v>22545</v>
+        <v>92246016</v>
       </c>
       <c r="K3" s="2">
-        <v>22613</v>
+        <v>92258304</v>
       </c>
       <c r="L3" s="2">
-        <v>22530</v>
+        <v>92258304</v>
       </c>
       <c r="M3" s="2">
         <v>3345</v>
@@ -1035,15 +1049,15 @@
         <v>363</v>
       </c>
       <c r="P3" s="8">
-        <f t="shared" ref="P3:P33" si="0">M3/F3</f>
+        <f t="shared" ref="P3:P37" si="0">M3/F3</f>
         <v>0.48485287722858383</v>
       </c>
       <c r="Q3" s="8">
-        <f t="shared" ref="Q3:Q33" si="1">N3/G3</f>
+        <f t="shared" ref="Q3:Q37" si="1">N3/G3</f>
         <v>0.56266862889379443</v>
       </c>
       <c r="R3" s="8">
-        <f t="shared" ref="R3:R33" si="2">O3/H3</f>
+        <f t="shared" ref="R3:R37" si="2">O3/H3</f>
         <v>9.8081599567684405E-2</v>
       </c>
       <c r="S3" s="2">
@@ -1068,15 +1082,15 @@
         <v>1309</v>
       </c>
       <c r="Z3" s="8">
-        <f t="shared" ref="Z3:Z33" si="3">W3/F3</f>
+        <f t="shared" ref="Z3:Z37" si="3">W3/F3</f>
         <v>0.89897086534280335</v>
       </c>
       <c r="AA3" s="9">
-        <f t="shared" ref="AA3:AA33" si="4">X3/G3</f>
+        <f t="shared" ref="AA3:AA37" si="4">X3/G3</f>
         <v>0.64974245768947758</v>
       </c>
       <c r="AB3" s="9">
-        <f t="shared" ref="AB3:AB33" si="5">Y3/H3</f>
+        <f t="shared" ref="AB3:AB37" si="5">Y3/H3</f>
         <v>0.35368819238043769</v>
       </c>
     </row>
@@ -1266,7 +1280,7 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -1281,84 +1295,78 @@
         <v>0</v>
       </c>
       <c r="F6" s="2">
-        <v>6371</v>
+        <v>1222</v>
       </c>
       <c r="G6" s="2">
-        <v>7131</v>
-      </c>
-      <c r="H6" s="29">
-        <v>6190</v>
-      </c>
+        <v>1179</v>
+      </c>
+      <c r="H6" s="2"/>
       <c r="I6" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J6" s="2">
-        <v>9848</v>
+        <v>0</v>
       </c>
       <c r="K6" s="2">
-        <v>9602</v>
+        <v>0</v>
       </c>
       <c r="L6" s="2">
-        <v>9848</v>
+        <v>0</v>
       </c>
       <c r="M6" s="2">
-        <v>2176</v>
+        <v>2808</v>
       </c>
       <c r="N6" s="2">
-        <v>2255</v>
-      </c>
-      <c r="O6" s="1">
-        <v>1157</v>
-      </c>
+        <v>1568</v>
+      </c>
+      <c r="O6" s="1"/>
       <c r="P6" s="8">
         <f t="shared" si="0"/>
-        <v>0.34154763773347985</v>
+        <v>2.2978723404255321</v>
       </c>
       <c r="Q6" s="8">
         <f t="shared" si="1"/>
-        <v>0.31622493338942642</v>
-      </c>
-      <c r="R6" s="8">
+        <v>1.3299406276505512</v>
+      </c>
+      <c r="R6" s="8" t="e">
         <f t="shared" si="2"/>
-        <v>0.18691437802907915</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="S6" s="2">
         <v>0</v>
       </c>
       <c r="T6" s="2">
-        <v>6772</v>
+        <v>0</v>
       </c>
       <c r="U6" s="2">
-        <v>6701</v>
+        <v>0</v>
       </c>
       <c r="V6" s="2">
-        <v>6772</v>
+        <v>0</v>
       </c>
       <c r="W6" s="2">
-        <v>2709</v>
+        <v>2906</v>
       </c>
       <c r="X6" s="2">
-        <v>2474</v>
-      </c>
-      <c r="Y6" s="1">
-        <v>1514</v>
-      </c>
+        <v>1728</v>
+      </c>
+      <c r="Y6" s="1"/>
       <c r="Z6" s="8">
         <f t="shared" si="3"/>
-        <v>0.42520797363051327</v>
+        <v>2.3780687397708675</v>
       </c>
       <c r="AA6" s="9">
         <f t="shared" si="4"/>
-        <v>0.34693591361660359</v>
-      </c>
-      <c r="AB6" s="9">
+        <v>1.4656488549618321</v>
+      </c>
+      <c r="AB6" s="9" t="e">
         <f t="shared" si="5"/>
-        <v>0.24458804523424879</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
@@ -1373,176 +1381,164 @@
         <v>0</v>
       </c>
       <c r="F7" s="2">
-        <v>4807</v>
+        <v>1573</v>
       </c>
       <c r="G7" s="2">
-        <v>5292</v>
-      </c>
-      <c r="H7" s="29">
-        <v>4740</v>
-      </c>
+        <v>1545</v>
+      </c>
+      <c r="H7" s="2"/>
       <c r="I7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="2">
-        <v>9218</v>
+        <v>0</v>
       </c>
       <c r="K7" s="2">
-        <v>9042</v>
+        <v>0</v>
       </c>
       <c r="L7" s="2">
-        <v>9218</v>
+        <v>0</v>
       </c>
       <c r="M7" s="2">
-        <v>8173</v>
+        <v>7990</v>
       </c>
       <c r="N7" s="2">
-        <v>4664</v>
-      </c>
-      <c r="O7" s="1">
-        <v>3138</v>
-      </c>
+        <v>2042</v>
+      </c>
+      <c r="O7" s="1"/>
       <c r="P7" s="8">
         <f t="shared" si="0"/>
-        <v>1.700228832951945</v>
+        <v>5.0794659885568976</v>
       </c>
       <c r="Q7" s="8">
         <f t="shared" si="1"/>
-        <v>0.88133030990173844</v>
-      </c>
-      <c r="R7" s="8">
+        <v>1.3216828478964402</v>
+      </c>
+      <c r="R7" s="8" t="e">
         <f t="shared" si="2"/>
-        <v>0.66202531645569618</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="S7" s="2">
         <v>0</v>
       </c>
       <c r="T7" s="2">
-        <v>6144</v>
+        <v>0</v>
       </c>
       <c r="U7" s="2">
-        <v>6093</v>
+        <v>0</v>
       </c>
       <c r="V7" s="2">
-        <v>6144</v>
+        <v>0</v>
       </c>
       <c r="W7" s="2">
-        <v>7364</v>
+        <v>8010</v>
       </c>
       <c r="X7" s="2">
-        <v>4589</v>
-      </c>
-      <c r="Y7" s="1">
-        <v>3433</v>
-      </c>
+        <v>2038</v>
+      </c>
+      <c r="Y7" s="1"/>
       <c r="Z7" s="8">
         <f t="shared" si="3"/>
-        <v>1.5319325982941543</v>
+        <v>5.0921805467260013</v>
       </c>
       <c r="AA7" s="9">
         <f t="shared" si="4"/>
-        <v>0.86715797430083141</v>
-      </c>
-      <c r="AB7" s="9">
+        <v>1.3190938511326862</v>
+      </c>
+      <c r="AB7" s="9" t="e">
         <f t="shared" si="5"/>
-        <v>0.72426160337552747</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="B8" s="2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C8" s="2">
-        <v>310</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2">
-        <v>591</v>
+        <v>0</v>
       </c>
       <c r="E8" s="2">
-        <v>310</v>
+        <v>0</v>
       </c>
       <c r="F8" s="2">
-        <v>7271</v>
+        <v>1253</v>
       </c>
       <c r="G8" s="2">
-        <v>8932</v>
-      </c>
-      <c r="H8" s="29">
-        <v>7931</v>
-      </c>
+        <v>830</v>
+      </c>
+      <c r="H8" s="2"/>
       <c r="I8" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J8" s="2">
-        <v>22049</v>
+        <v>11280</v>
       </c>
       <c r="K8" s="2">
-        <v>12205</v>
+        <v>11348</v>
       </c>
       <c r="L8" s="2">
-        <v>9846</v>
+        <v>11280</v>
       </c>
       <c r="M8" s="2">
-        <v>4921</v>
+        <v>1405</v>
       </c>
       <c r="N8" s="2">
-        <v>2693</v>
-      </c>
-      <c r="O8" s="1">
-        <v>1456</v>
-      </c>
+        <v>1166</v>
+      </c>
+      <c r="O8" s="1"/>
       <c r="P8" s="8">
         <f t="shared" si="0"/>
-        <v>0.67679823958190066</v>
+        <v>1.1213088587390263</v>
       </c>
       <c r="Q8" s="8">
         <f t="shared" si="1"/>
-        <v>0.30150022391401704</v>
-      </c>
-      <c r="R8" s="8">
+        <v>1.4048192771084338</v>
+      </c>
+      <c r="R8" s="8" t="e">
         <f t="shared" si="2"/>
-        <v>0.18358340688437777</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="S8" s="2">
         <v>0</v>
       </c>
       <c r="T8" s="2">
-        <v>17862</v>
+        <v>0</v>
       </c>
       <c r="U8" s="2">
-        <v>11090</v>
+        <v>0</v>
       </c>
       <c r="V8" s="2">
-        <v>6772</v>
+        <v>0</v>
       </c>
       <c r="W8" s="2">
-        <v>4521</v>
+        <v>1891</v>
       </c>
       <c r="X8" s="2">
-        <v>2579</v>
-      </c>
-      <c r="Y8" s="1">
-        <v>1694</v>
-      </c>
+        <v>1126</v>
+      </c>
+      <c r="Y8" s="1"/>
       <c r="Z8" s="8">
         <f t="shared" si="3"/>
-        <v>0.62178517397881994</v>
+        <v>1.5091779728651238</v>
       </c>
       <c r="AA8" s="9">
         <f t="shared" si="4"/>
-        <v>0.28873712494402148</v>
-      </c>
-      <c r="AB8" s="9">
+        <v>1.3566265060240963</v>
+      </c>
+      <c r="AB8" s="9" t="e">
         <f t="shared" si="5"/>
-        <v>0.21359223300970873</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="B9" s="2">
         <v>0</v>
@@ -1557,46 +1553,42 @@
         <v>0</v>
       </c>
       <c r="F9" s="2">
-        <v>3491</v>
+        <v>16089</v>
       </c>
       <c r="G9" s="2">
-        <v>3085</v>
-      </c>
-      <c r="H9" s="2">
-        <v>2817</v>
-      </c>
+        <v>13721</v>
+      </c>
+      <c r="H9" s="2"/>
       <c r="I9" s="2">
-        <v>1</v>
+        <v>666</v>
       </c>
       <c r="J9" s="2">
-        <v>4</v>
+        <v>430069</v>
       </c>
       <c r="K9" s="2">
-        <v>4</v>
+        <v>430212</v>
       </c>
       <c r="L9" s="2">
-        <v>4</v>
+        <v>429655</v>
       </c>
       <c r="M9" s="2">
-        <v>806</v>
+        <v>15363</v>
       </c>
       <c r="N9" s="2">
-        <v>598</v>
-      </c>
-      <c r="O9" s="1">
-        <v>155</v>
-      </c>
+        <v>11652</v>
+      </c>
+      <c r="O9" s="1"/>
       <c r="P9" s="8">
         <f t="shared" si="0"/>
-        <v>0.23087940418218275</v>
+        <v>0.95487600223755364</v>
       </c>
       <c r="Q9" s="8">
         <f t="shared" si="1"/>
-        <v>0.19384116693679093</v>
-      </c>
-      <c r="R9" s="8">
+        <v>0.84920924130894249</v>
+      </c>
+      <c r="R9" s="8" t="e">
         <f t="shared" si="2"/>
-        <v>5.5023074192403265E-2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="S9" s="2">
         <v>0</v>
@@ -1611,30 +1603,28 @@
         <v>0</v>
       </c>
       <c r="W9" s="2">
-        <v>1032</v>
+        <v>26370</v>
       </c>
       <c r="X9" s="2">
-        <v>629</v>
-      </c>
-      <c r="Y9" s="1">
-        <v>348</v>
-      </c>
+        <v>13030</v>
+      </c>
+      <c r="Y9" s="1"/>
       <c r="Z9" s="8">
         <f t="shared" si="3"/>
-        <v>0.29561730163277</v>
+        <v>1.6390080179004289</v>
       </c>
       <c r="AA9" s="9">
         <f t="shared" si="4"/>
-        <v>0.20388978930307941</v>
-      </c>
-      <c r="AB9" s="9">
+        <v>0.94963923912251291</v>
+      </c>
+      <c r="AB9" s="9" t="e">
         <f t="shared" si="5"/>
-        <v>0.1235356762513312</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
@@ -1649,268 +1639,268 @@
         <v>0</v>
       </c>
       <c r="F10" s="2">
-        <v>3466</v>
+        <v>6371</v>
       </c>
       <c r="G10" s="2">
-        <v>3197</v>
-      </c>
-      <c r="H10" s="2">
-        <v>2821</v>
+        <v>7131</v>
+      </c>
+      <c r="H10" s="28">
+        <v>6190</v>
       </c>
       <c r="I10" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J10" s="2">
-        <v>1</v>
+        <v>9848</v>
       </c>
       <c r="K10" s="2">
-        <v>4</v>
+        <v>9602</v>
       </c>
       <c r="L10" s="2">
-        <v>1</v>
+        <v>9848</v>
       </c>
       <c r="M10" s="2">
-        <v>808</v>
+        <v>2176</v>
       </c>
       <c r="N10" s="2">
-        <v>653</v>
+        <v>2255</v>
       </c>
       <c r="O10" s="1">
-        <v>164</v>
+        <v>1157</v>
       </c>
       <c r="P10" s="8">
         <f t="shared" si="0"/>
-        <v>0.23312175418349682</v>
+        <v>0.34154763773347985</v>
       </c>
       <c r="Q10" s="8">
         <f t="shared" si="1"/>
-        <v>0.20425398811385673</v>
+        <v>0.31622493338942642</v>
       </c>
       <c r="R10" s="8">
         <f t="shared" si="2"/>
-        <v>5.8135412974122655E-2</v>
+        <v>0.18691437802907915</v>
       </c>
       <c r="S10" s="2">
         <v>0</v>
       </c>
       <c r="T10" s="2">
-        <v>0</v>
+        <v>6772</v>
       </c>
       <c r="U10" s="2">
-        <v>0</v>
+        <v>6701</v>
       </c>
       <c r="V10" s="2">
-        <v>0</v>
+        <v>6772</v>
       </c>
       <c r="W10" s="2">
-        <v>1041</v>
+        <v>2709</v>
       </c>
       <c r="X10" s="2">
-        <v>673</v>
+        <v>2474</v>
       </c>
       <c r="Y10" s="1">
-        <v>361</v>
+        <v>1514</v>
       </c>
       <c r="Z10" s="8">
         <f t="shared" si="3"/>
-        <v>0.30034622042700521</v>
+        <v>0.42520797363051327</v>
       </c>
       <c r="AA10" s="9">
         <f t="shared" si="4"/>
-        <v>0.21050985298717548</v>
+        <v>0.34693591361660359</v>
       </c>
       <c r="AB10" s="9">
         <f t="shared" si="5"/>
-        <v>0.12796880538816022</v>
+        <v>0.24458804523424879</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B11" s="2">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C11" s="2">
-        <v>868</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2">
-        <v>868</v>
+        <v>0</v>
       </c>
       <c r="E11" s="2">
-        <v>868</v>
+        <v>0</v>
       </c>
       <c r="F11" s="2">
-        <v>6364</v>
+        <v>4807</v>
       </c>
       <c r="G11" s="2">
-        <v>5690</v>
-      </c>
-      <c r="H11" s="2">
-        <v>5046</v>
+        <v>5292</v>
+      </c>
+      <c r="H11" s="28">
+        <v>4740</v>
       </c>
       <c r="I11" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J11" s="2">
-        <v>4</v>
+        <v>9218</v>
       </c>
       <c r="K11" s="2">
-        <v>5</v>
+        <v>9042</v>
       </c>
       <c r="L11" s="2">
-        <v>5</v>
+        <v>9218</v>
       </c>
       <c r="M11" s="2">
-        <v>1905</v>
+        <v>8173</v>
       </c>
       <c r="N11" s="2">
-        <v>1339</v>
+        <v>4664</v>
       </c>
       <c r="O11" s="1">
-        <v>557</v>
+        <v>3138</v>
       </c>
       <c r="P11" s="8">
         <f t="shared" si="0"/>
-        <v>0.29934003771213075</v>
+        <v>1.700228832951945</v>
       </c>
       <c r="Q11" s="8">
         <f t="shared" si="1"/>
-        <v>0.23532513181019332</v>
+        <v>0.88133030990173844</v>
       </c>
       <c r="R11" s="8">
         <f t="shared" si="2"/>
-        <v>0.11038446294094333</v>
+        <v>0.66202531645569618</v>
       </c>
       <c r="S11" s="2">
         <v>0</v>
       </c>
       <c r="T11" s="2">
-        <v>0</v>
+        <v>6144</v>
       </c>
       <c r="U11" s="2">
-        <v>0</v>
+        <v>6093</v>
       </c>
       <c r="V11" s="2">
-        <v>0</v>
+        <v>6144</v>
       </c>
       <c r="W11" s="2">
-        <v>2000</v>
+        <v>7364</v>
       </c>
       <c r="X11" s="2">
-        <v>1463</v>
+        <v>4589</v>
       </c>
       <c r="Y11" s="1">
-        <v>880</v>
+        <v>3433</v>
       </c>
       <c r="Z11" s="8">
         <f t="shared" si="3"/>
-        <v>0.31426775612822122</v>
+        <v>1.5319325982941543</v>
       </c>
       <c r="AA11" s="9">
         <f t="shared" si="4"/>
-        <v>0.2571177504393673</v>
+        <v>0.86715797430083141</v>
       </c>
       <c r="AB11" s="9">
         <f t="shared" si="5"/>
-        <v>0.17439556084026953</v>
+        <v>0.72426160337552747</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B12" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C12" s="2">
-        <v>0</v>
+        <v>310</v>
       </c>
       <c r="D12" s="2">
-        <v>0</v>
+        <v>591</v>
       </c>
       <c r="E12" s="2">
-        <v>0</v>
+        <v>310</v>
       </c>
       <c r="F12" s="2">
-        <v>5350</v>
+        <v>7271</v>
       </c>
       <c r="G12" s="2">
-        <v>3121</v>
-      </c>
-      <c r="H12" s="2">
-        <v>2870</v>
+        <v>8932</v>
+      </c>
+      <c r="H12" s="28">
+        <v>7931</v>
       </c>
       <c r="I12" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J12" s="2">
-        <v>0</v>
+        <v>22049</v>
       </c>
       <c r="K12" s="2">
-        <v>0</v>
+        <v>12205</v>
       </c>
       <c r="L12" s="2">
-        <v>0</v>
+        <v>9846</v>
       </c>
       <c r="M12" s="2">
-        <v>1808</v>
+        <v>4921</v>
       </c>
       <c r="N12" s="2">
-        <v>1214</v>
+        <v>2693</v>
       </c>
       <c r="O12" s="1">
-        <v>891</v>
+        <v>1456</v>
       </c>
       <c r="P12" s="8">
         <f t="shared" si="0"/>
-        <v>0.33794392523364486</v>
+        <v>0.67679823958190066</v>
       </c>
       <c r="Q12" s="8">
         <f t="shared" si="1"/>
-        <v>0.38897789170137775</v>
+        <v>0.30150022391401704</v>
       </c>
       <c r="R12" s="8">
         <f t="shared" si="2"/>
-        <v>0.31045296167247388</v>
+        <v>0.18358340688437777</v>
       </c>
       <c r="S12" s="2">
         <v>0</v>
       </c>
       <c r="T12" s="2">
-        <v>0</v>
+        <v>17862</v>
       </c>
       <c r="U12" s="2">
-        <v>0</v>
+        <v>11090</v>
       </c>
       <c r="V12" s="2">
-        <v>0</v>
+        <v>6772</v>
       </c>
       <c r="W12" s="2">
-        <v>1956</v>
+        <v>4521</v>
       </c>
       <c r="X12" s="2">
-        <v>944</v>
+        <v>2579</v>
       </c>
       <c r="Y12" s="1">
-        <v>549</v>
+        <v>1694</v>
       </c>
       <c r="Z12" s="8">
         <f t="shared" si="3"/>
-        <v>0.36560747663551402</v>
+        <v>0.62178517397881994</v>
       </c>
       <c r="AA12" s="9">
         <f t="shared" si="4"/>
-        <v>0.30246715796219159</v>
+        <v>0.28873712494402148</v>
       </c>
       <c r="AB12" s="9">
         <f t="shared" si="5"/>
-        <v>0.19128919860627178</v>
+        <v>0.21359223300970873</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B13" s="2">
         <v>0</v>
@@ -1925,46 +1915,46 @@
         <v>0</v>
       </c>
       <c r="F13" s="2">
-        <v>1418</v>
+        <v>3491</v>
       </c>
       <c r="G13" s="2">
-        <v>1436</v>
+        <v>3085</v>
       </c>
       <c r="H13" s="2">
-        <v>1250</v>
+        <v>2817</v>
       </c>
       <c r="I13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K13" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L13" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M13" s="2">
-        <v>434</v>
+        <v>806</v>
       </c>
       <c r="N13" s="2">
-        <v>403</v>
+        <v>598</v>
       </c>
       <c r="O13" s="1">
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="P13" s="8">
         <f t="shared" si="0"/>
-        <v>0.306064880112835</v>
+        <v>0.23087940418218275</v>
       </c>
       <c r="Q13" s="8">
         <f t="shared" si="1"/>
-        <v>0.28064066852367686</v>
+        <v>0.19384116693679093</v>
       </c>
       <c r="R13" s="8">
         <f t="shared" si="2"/>
-        <v>0.1048</v>
+        <v>5.5023074192403265E-2</v>
       </c>
       <c r="S13" s="2">
         <v>0</v>
@@ -1979,30 +1969,30 @@
         <v>0</v>
       </c>
       <c r="W13" s="2">
-        <v>675</v>
+        <v>1032</v>
       </c>
       <c r="X13" s="2">
-        <v>405</v>
+        <v>629</v>
       </c>
       <c r="Y13" s="1">
-        <v>252</v>
+        <v>348</v>
       </c>
       <c r="Z13" s="8">
         <f t="shared" si="3"/>
-        <v>0.47602256699576867</v>
+        <v>0.29561730163277</v>
       </c>
       <c r="AA13" s="9">
         <f t="shared" si="4"/>
-        <v>0.28203342618384403</v>
+        <v>0.20388978930307941</v>
       </c>
       <c r="AB13" s="9">
         <f t="shared" si="5"/>
-        <v>0.2016</v>
+        <v>0.1235356762513312</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2">
         <v>0</v>
@@ -2017,46 +2007,46 @@
         <v>0</v>
       </c>
       <c r="F14" s="2">
-        <v>12922</v>
+        <v>3466</v>
       </c>
       <c r="G14" s="2">
-        <v>13166</v>
+        <v>3197</v>
       </c>
       <c r="H14" s="2">
-        <v>11881</v>
+        <v>2821</v>
       </c>
       <c r="I14" s="2">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="J14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" s="2">
-        <v>5066</v>
+        <v>808</v>
       </c>
       <c r="N14" s="2">
-        <v>3384</v>
+        <v>653</v>
       </c>
       <c r="O14" s="1">
-        <v>2168</v>
+        <v>164</v>
       </c>
       <c r="P14" s="8">
         <f t="shared" si="0"/>
-        <v>0.39204457514316671</v>
+        <v>0.23312175418349682</v>
       </c>
       <c r="Q14" s="8">
         <f t="shared" si="1"/>
-        <v>0.25702567218593347</v>
+        <v>0.20425398811385673</v>
       </c>
       <c r="R14" s="8">
         <f t="shared" si="2"/>
-        <v>0.18247622254019022</v>
+        <v>5.8135412974122655E-2</v>
       </c>
       <c r="S14" s="2">
         <v>0</v>
@@ -2071,122 +2061,122 @@
         <v>0</v>
       </c>
       <c r="W14" s="2">
-        <v>6197</v>
+        <v>1041</v>
       </c>
       <c r="X14" s="2">
-        <v>4616</v>
+        <v>673</v>
       </c>
       <c r="Y14" s="1">
-        <v>3097</v>
+        <v>361</v>
       </c>
       <c r="Z14" s="8">
         <f t="shared" si="3"/>
-        <v>0.47956972604859927</v>
+        <v>0.30034622042700521</v>
       </c>
       <c r="AA14" s="9">
         <f t="shared" si="4"/>
-        <v>0.35060003038128512</v>
+        <v>0.21050985298717548</v>
       </c>
       <c r="AB14" s="9">
         <f t="shared" si="5"/>
-        <v>0.26066829391465363</v>
+        <v>0.12796880538816022</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B15" s="2">
+        <v>22</v>
+      </c>
+      <c r="C15" s="2">
+        <v>868</v>
+      </c>
+      <c r="D15" s="2">
+        <v>868</v>
+      </c>
+      <c r="E15" s="2">
+        <v>868</v>
+      </c>
+      <c r="F15" s="2">
+        <v>6364</v>
+      </c>
+      <c r="G15" s="2">
+        <v>5690</v>
+      </c>
+      <c r="H15" s="2">
+        <v>5046</v>
+      </c>
+      <c r="I15" s="2">
+        <v>2</v>
+      </c>
+      <c r="J15" s="2">
         <v>4</v>
       </c>
-      <c r="C15" s="2">
-        <v>58</v>
-      </c>
-      <c r="D15" s="2">
-        <v>475</v>
-      </c>
-      <c r="E15" s="2">
-        <v>465</v>
-      </c>
-      <c r="F15" s="2">
-        <v>7552</v>
-      </c>
-      <c r="G15" s="2">
-        <v>7234</v>
-      </c>
-      <c r="H15" s="2">
-        <v>6111</v>
-      </c>
-      <c r="I15" s="2">
-        <v>53</v>
-      </c>
-      <c r="J15" s="2">
-        <v>148538</v>
-      </c>
       <c r="K15" s="2">
-        <v>146678</v>
+        <v>5</v>
       </c>
       <c r="L15" s="2">
-        <v>148569</v>
+        <v>5</v>
       </c>
       <c r="M15" s="2">
-        <v>4256</v>
+        <v>1905</v>
       </c>
       <c r="N15" s="2">
-        <v>4351</v>
+        <v>1339</v>
       </c>
       <c r="O15" s="1">
-        <v>2978</v>
+        <v>557</v>
       </c>
       <c r="P15" s="8">
         <f t="shared" si="0"/>
-        <v>0.56355932203389836</v>
+        <v>0.29934003771213075</v>
       </c>
       <c r="Q15" s="8">
         <f t="shared" si="1"/>
-        <v>0.60146530273707488</v>
+        <v>0.23532513181019332</v>
       </c>
       <c r="R15" s="8">
         <f t="shared" si="2"/>
-        <v>0.487317951235477</v>
+        <v>0.11038446294094333</v>
       </c>
       <c r="S15" s="2">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="T15" s="2">
-        <v>121437</v>
+        <v>0</v>
       </c>
       <c r="U15" s="2">
-        <v>120719</v>
+        <v>0</v>
       </c>
       <c r="V15" s="2">
-        <v>121458</v>
+        <v>0</v>
       </c>
       <c r="W15" s="2">
-        <v>4515</v>
+        <v>2000</v>
       </c>
       <c r="X15" s="2">
-        <v>4857</v>
+        <v>1463</v>
       </c>
       <c r="Y15" s="1">
-        <v>3606</v>
+        <v>880</v>
       </c>
       <c r="Z15" s="8">
         <f t="shared" si="3"/>
-        <v>0.59785487288135597</v>
+        <v>0.31426775612822122</v>
       </c>
       <c r="AA15" s="9">
         <f t="shared" si="4"/>
-        <v>0.67141277301631186</v>
+        <v>0.2571177504393673</v>
       </c>
       <c r="AB15" s="9">
         <f t="shared" si="5"/>
-        <v>0.59008345606283752</v>
+        <v>0.17439556084026953</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B16" s="2">
         <v>0</v>
@@ -2201,138 +2191,138 @@
         <v>0</v>
       </c>
       <c r="F16" s="2">
-        <v>3690</v>
+        <v>5350</v>
       </c>
       <c r="G16" s="2">
-        <v>3646</v>
+        <v>3121</v>
       </c>
       <c r="H16" s="2">
-        <v>3042</v>
+        <v>2870</v>
       </c>
       <c r="I16" s="2">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="J16" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K16" s="2">
-        <v>377364</v>
+        <v>0</v>
       </c>
       <c r="L16" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M16" s="2">
-        <v>1507</v>
+        <v>1808</v>
       </c>
       <c r="N16" s="2">
-        <v>1389</v>
+        <v>1214</v>
       </c>
       <c r="O16" s="1">
-        <v>330</v>
+        <v>891</v>
       </c>
       <c r="P16" s="8">
         <f t="shared" si="0"/>
-        <v>0.40840108401084013</v>
+        <v>0.33794392523364486</v>
       </c>
       <c r="Q16" s="8">
         <f t="shared" si="1"/>
-        <v>0.38096544157981349</v>
+        <v>0.38897789170137775</v>
       </c>
       <c r="R16" s="8">
         <f t="shared" si="2"/>
-        <v>0.10848126232741617</v>
+        <v>0.31045296167247388</v>
       </c>
       <c r="S16" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T16" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="U16" s="2">
-        <v>26458</v>
+        <v>0</v>
       </c>
       <c r="V16" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="W16" s="2">
-        <v>7473</v>
+        <v>1956</v>
       </c>
       <c r="X16" s="2">
-        <v>1342</v>
+        <v>944</v>
       </c>
       <c r="Y16" s="1">
-        <v>710</v>
+        <v>549</v>
       </c>
       <c r="Z16" s="8">
         <f t="shared" si="3"/>
-        <v>2.0252032520325205</v>
+        <v>0.36560747663551402</v>
       </c>
       <c r="AA16" s="9">
         <f t="shared" si="4"/>
-        <v>0.36807460230389466</v>
+        <v>0.30246715796219159</v>
       </c>
       <c r="AB16" s="9">
         <f t="shared" si="5"/>
-        <v>0.23339907955292571</v>
+        <v>0.19128919860627178</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B17" s="2">
         <v>0</v>
       </c>
       <c r="C17" s="2">
-        <v>3596</v>
+        <v>0</v>
       </c>
       <c r="D17" s="2">
-        <v>2694</v>
+        <v>0</v>
       </c>
       <c r="E17" s="2">
-        <v>2694</v>
+        <v>0</v>
       </c>
       <c r="F17" s="2">
-        <v>6442</v>
+        <v>1418</v>
       </c>
       <c r="G17" s="2">
-        <v>5963</v>
+        <v>1436</v>
       </c>
       <c r="H17" s="2">
-        <v>4184</v>
+        <v>1250</v>
       </c>
       <c r="I17" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J17" s="2">
-        <v>8124</v>
+        <v>0</v>
       </c>
       <c r="K17" s="2">
-        <v>4062</v>
+        <v>0</v>
       </c>
       <c r="L17" s="2">
-        <v>4062</v>
+        <v>0</v>
       </c>
       <c r="M17" s="2">
-        <v>1721</v>
+        <v>434</v>
       </c>
       <c r="N17" s="2">
-        <v>1793</v>
+        <v>403</v>
       </c>
       <c r="O17" s="1">
-        <v>839</v>
+        <v>131</v>
       </c>
       <c r="P17" s="8">
         <f t="shared" si="0"/>
-        <v>0.26715305805650419</v>
+        <v>0.306064880112835</v>
       </c>
       <c r="Q17" s="8">
         <f t="shared" si="1"/>
-        <v>0.30068757336910951</v>
+        <v>0.28064066852367686</v>
       </c>
       <c r="R17" s="8">
         <f t="shared" si="2"/>
-        <v>0.20052581261950286</v>
+        <v>0.1048</v>
       </c>
       <c r="S17" s="2">
         <v>0</v>
@@ -2347,84 +2337,84 @@
         <v>0</v>
       </c>
       <c r="W17" s="2">
-        <v>2199</v>
+        <v>675</v>
       </c>
       <c r="X17" s="2">
-        <v>1625</v>
+        <v>405</v>
       </c>
       <c r="Y17" s="1">
-        <v>1062</v>
+        <v>252</v>
       </c>
       <c r="Z17" s="8">
         <f t="shared" si="3"/>
-        <v>0.34135361688916488</v>
+        <v>0.47602256699576867</v>
       </c>
       <c r="AA17" s="9">
         <f t="shared" si="4"/>
-        <v>0.27251383531779305</v>
+        <v>0.28203342618384403</v>
       </c>
       <c r="AB17" s="9">
         <f t="shared" si="5"/>
-        <v>0.2538240917782027</v>
+        <v>0.2016</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B18" s="2">
         <v>0</v>
       </c>
       <c r="C18" s="2">
-        <v>434</v>
+        <v>0</v>
       </c>
       <c r="D18" s="2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E18" s="2">
-        <v>434</v>
+        <v>0</v>
       </c>
       <c r="F18" s="2">
-        <v>6053</v>
+        <v>12922</v>
       </c>
       <c r="G18" s="2">
-        <v>6036</v>
+        <v>13166</v>
       </c>
       <c r="H18" s="2">
-        <v>3943</v>
+        <v>11881</v>
       </c>
       <c r="I18" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="J18" s="2">
-        <v>6160</v>
+        <v>0</v>
       </c>
       <c r="K18" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L18" s="2">
-        <v>6154</v>
+        <v>0</v>
       </c>
       <c r="M18" s="2">
-        <v>1734</v>
+        <v>5066</v>
       </c>
       <c r="N18" s="2">
-        <v>1618</v>
+        <v>3384</v>
       </c>
       <c r="O18" s="1">
-        <v>804</v>
+        <v>2168</v>
       </c>
       <c r="P18" s="8">
         <f t="shared" si="0"/>
-        <v>0.28646951924665454</v>
+        <v>0.39204457514316671</v>
       </c>
       <c r="Q18" s="8">
         <f t="shared" si="1"/>
-        <v>0.26805831676607023</v>
+        <v>0.25702567218593347</v>
       </c>
       <c r="R18" s="8">
         <f t="shared" si="2"/>
-        <v>0.20390565559218868</v>
+        <v>0.18247622254019022</v>
       </c>
       <c r="S18" s="2">
         <v>0</v>
@@ -2439,122 +2429,122 @@
         <v>0</v>
       </c>
       <c r="W18" s="2">
-        <v>2185</v>
+        <v>6197</v>
       </c>
       <c r="X18" s="2">
-        <v>1612</v>
+        <v>4616</v>
       </c>
       <c r="Y18" s="1">
-        <v>1050</v>
+        <v>3097</v>
       </c>
       <c r="Z18" s="8">
         <f t="shared" si="3"/>
-        <v>0.36097802742441765</v>
+        <v>0.47956972604859927</v>
       </c>
       <c r="AA18" s="9">
         <f t="shared" si="4"/>
-        <v>0.267064280980782</v>
+        <v>0.35060003038128512</v>
       </c>
       <c r="AB18" s="9">
         <f t="shared" si="5"/>
-        <v>0.26629469946741058</v>
+        <v>0.26066829391465363</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B19" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C19" s="2">
-        <v>3356</v>
+        <v>58</v>
       </c>
       <c r="D19" s="2">
-        <v>3356</v>
+        <v>475</v>
       </c>
       <c r="E19" s="2">
-        <v>3356</v>
+        <v>465</v>
       </c>
       <c r="F19" s="2">
-        <v>8209</v>
+        <v>7552</v>
       </c>
       <c r="G19" s="2">
-        <v>7661</v>
+        <v>7234</v>
       </c>
       <c r="H19" s="2">
-        <v>5109</v>
+        <v>6111</v>
       </c>
       <c r="I19" s="2">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="J19" s="2">
-        <v>2</v>
+        <v>148538</v>
       </c>
       <c r="K19" s="2">
-        <v>3525</v>
+        <v>146678</v>
       </c>
       <c r="L19" s="2">
-        <v>3525</v>
+        <v>148569</v>
       </c>
       <c r="M19" s="2">
-        <v>2271</v>
+        <v>4256</v>
       </c>
       <c r="N19" s="2">
-        <v>1638</v>
+        <v>4351</v>
       </c>
       <c r="O19" s="1">
-        <v>719</v>
+        <v>2978</v>
       </c>
       <c r="P19" s="8">
         <f t="shared" si="0"/>
-        <v>0.27664758192228045</v>
+        <v>0.56355932203389836</v>
       </c>
       <c r="Q19" s="8">
         <f t="shared" si="1"/>
-        <v>0.21381020754470695</v>
+        <v>0.60146530273707488</v>
       </c>
       <c r="R19" s="8">
         <f t="shared" si="2"/>
-        <v>0.14073204149540028</v>
+        <v>0.487317951235477</v>
       </c>
       <c r="S19" s="2">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="T19" s="2">
-        <v>0</v>
+        <v>121437</v>
       </c>
       <c r="U19" s="2">
-        <v>0</v>
+        <v>120719</v>
       </c>
       <c r="V19" s="2">
-        <v>0</v>
+        <v>121458</v>
       </c>
       <c r="W19" s="2">
-        <v>2792</v>
+        <v>4515</v>
       </c>
       <c r="X19" s="2">
-        <v>2181</v>
+        <v>4857</v>
       </c>
       <c r="Y19" s="1">
-        <v>1164</v>
+        <v>3606</v>
       </c>
       <c r="Z19" s="8">
         <f t="shared" si="3"/>
-        <v>0.34011450846631747</v>
+        <v>0.59785487288135597</v>
       </c>
       <c r="AA19" s="9">
         <f t="shared" si="4"/>
-        <v>0.28468868293956401</v>
+        <v>0.67141277301631186</v>
       </c>
       <c r="AB19" s="9">
         <f t="shared" si="5"/>
-        <v>0.22783323546682324</v>
+        <v>0.59008345606283752</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B20" s="2">
         <v>0</v>
@@ -2569,138 +2559,138 @@
         <v>0</v>
       </c>
       <c r="F20" s="2">
-        <v>4060</v>
+        <v>3690</v>
       </c>
       <c r="G20" s="2">
-        <v>3836</v>
+        <v>3646</v>
       </c>
       <c r="H20" s="2">
-        <v>2830</v>
+        <v>3042</v>
       </c>
       <c r="I20" s="2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J20" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K20" s="2">
-        <v>4057</v>
+        <v>377364</v>
       </c>
       <c r="L20" s="2">
-        <v>4057</v>
+        <v>4</v>
       </c>
       <c r="M20" s="2">
-        <v>768</v>
+        <v>1507</v>
       </c>
       <c r="N20" s="2">
-        <v>749</v>
+        <v>1389</v>
       </c>
       <c r="O20" s="1">
-        <v>302</v>
+        <v>330</v>
       </c>
       <c r="P20" s="8">
         <f t="shared" si="0"/>
-        <v>0.18916256157635469</v>
+        <v>0.40840108401084013</v>
       </c>
       <c r="Q20" s="8">
         <f t="shared" si="1"/>
-        <v>0.19525547445255476</v>
+        <v>0.38096544157981349</v>
       </c>
       <c r="R20" s="8">
         <f t="shared" si="2"/>
-        <v>0.10671378091872792</v>
+        <v>0.10848126232741617</v>
       </c>
       <c r="S20" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T20" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U20" s="2">
-        <v>0</v>
+        <v>26458</v>
       </c>
       <c r="V20" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W20" s="2">
-        <v>953</v>
+        <v>7473</v>
       </c>
       <c r="X20" s="2">
-        <v>845</v>
+        <v>1342</v>
       </c>
       <c r="Y20" s="1">
-        <v>553</v>
+        <v>710</v>
       </c>
       <c r="Z20" s="8">
         <f t="shared" si="3"/>
-        <v>0.23472906403940888</v>
+        <v>2.0252032520325205</v>
       </c>
       <c r="AA20" s="9">
         <f t="shared" si="4"/>
-        <v>0.22028154327424401</v>
+        <v>0.36807460230389466</v>
       </c>
       <c r="AB20" s="9">
         <f t="shared" si="5"/>
-        <v>0.19540636042402826</v>
+        <v>0.23339907955292571</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B21" s="2">
         <v>0</v>
       </c>
       <c r="C21" s="2">
-        <v>0</v>
+        <v>3596</v>
       </c>
       <c r="D21" s="2">
-        <v>0</v>
+        <v>2694</v>
       </c>
       <c r="E21" s="2">
-        <v>0</v>
+        <v>2694</v>
       </c>
       <c r="F21" s="2">
-        <v>3842</v>
+        <v>6442</v>
       </c>
       <c r="G21" s="2">
-        <v>3768</v>
+        <v>5963</v>
       </c>
       <c r="H21" s="2">
-        <v>2651</v>
+        <v>4184</v>
       </c>
       <c r="I21" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J21" s="2">
-        <v>1</v>
+        <v>8124</v>
       </c>
       <c r="K21" s="2">
-        <v>0</v>
+        <v>4062</v>
       </c>
       <c r="L21" s="2">
-        <v>1</v>
+        <v>4062</v>
       </c>
       <c r="M21" s="2">
-        <v>793</v>
+        <v>1721</v>
       </c>
       <c r="N21" s="2">
-        <v>808</v>
+        <v>1793</v>
       </c>
       <c r="O21" s="1">
-        <v>331</v>
+        <v>839</v>
       </c>
       <c r="P21" s="8">
         <f t="shared" si="0"/>
-        <v>0.20640291514836023</v>
+        <v>0.26715305805650419</v>
       </c>
       <c r="Q21" s="8">
         <f t="shared" si="1"/>
-        <v>0.21443736730360935</v>
+        <v>0.30068757336910951</v>
       </c>
       <c r="R21" s="8">
         <f t="shared" si="2"/>
-        <v>0.12485854394568087</v>
+        <v>0.20052581261950286</v>
       </c>
       <c r="S21" s="2">
         <v>0</v>
@@ -2715,84 +2705,84 @@
         <v>0</v>
       </c>
       <c r="W21" s="2">
-        <v>983</v>
+        <v>2199</v>
       </c>
       <c r="X21" s="2">
-        <v>825</v>
+        <v>1625</v>
       </c>
       <c r="Y21" s="1">
-        <v>542</v>
+        <v>1062</v>
       </c>
       <c r="Z21" s="8">
         <f t="shared" si="3"/>
-        <v>0.25585632483081727</v>
+        <v>0.34135361688916488</v>
       </c>
       <c r="AA21" s="9">
         <f t="shared" si="4"/>
-        <v>0.21894904458598727</v>
+        <v>0.27251383531779305</v>
       </c>
       <c r="AB21" s="9">
         <f t="shared" si="5"/>
-        <v>0.20445115050924179</v>
+        <v>0.2538240917782027</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B22" s="2">
         <v>0</v>
       </c>
       <c r="C22" s="2">
-        <v>720</v>
+        <v>434</v>
       </c>
       <c r="D22" s="2">
-        <v>720</v>
+        <v>50</v>
       </c>
       <c r="E22" s="2">
-        <v>720</v>
+        <v>434</v>
       </c>
       <c r="F22" s="2">
-        <v>5624</v>
+        <v>6053</v>
       </c>
       <c r="G22" s="2">
-        <v>5243</v>
+        <v>6036</v>
       </c>
       <c r="H22" s="2">
-        <v>3724</v>
+        <v>3943</v>
       </c>
       <c r="I22" s="2">
+        <v>2</v>
+      </c>
+      <c r="J22" s="2">
+        <v>6160</v>
+      </c>
+      <c r="K22" s="2">
         <v>6</v>
       </c>
-      <c r="J22" s="2">
-        <v>7050</v>
-      </c>
-      <c r="K22" s="2">
-        <v>3525</v>
-      </c>
       <c r="L22" s="2">
-        <v>3525</v>
+        <v>6154</v>
       </c>
       <c r="M22" s="2">
-        <v>2195</v>
+        <v>1734</v>
       </c>
       <c r="N22" s="2">
-        <v>1726</v>
+        <v>1618</v>
       </c>
       <c r="O22" s="1">
-        <v>843</v>
+        <v>804</v>
       </c>
       <c r="P22" s="8">
         <f t="shared" si="0"/>
-        <v>0.39029160739687058</v>
+        <v>0.28646951924665454</v>
       </c>
       <c r="Q22" s="8">
         <f t="shared" si="1"/>
-        <v>0.32920083921419035</v>
+        <v>0.26805831676607023</v>
       </c>
       <c r="R22" s="8">
         <f t="shared" si="2"/>
-        <v>0.22636949516648766</v>
+        <v>0.20390565559218868</v>
       </c>
       <c r="S22" s="2">
         <v>0</v>
@@ -2807,84 +2797,84 @@
         <v>0</v>
       </c>
       <c r="W22" s="2">
-        <v>2694</v>
+        <v>2185</v>
       </c>
       <c r="X22" s="2">
-        <v>1949</v>
+        <v>1612</v>
       </c>
       <c r="Y22" s="1">
-        <v>1271</v>
+        <v>1050</v>
       </c>
       <c r="Z22" s="8">
         <f t="shared" si="3"/>
-        <v>0.47901849217638692</v>
+        <v>0.36097802742441765</v>
       </c>
       <c r="AA22" s="9">
         <f t="shared" si="4"/>
-        <v>0.371733740225062</v>
+        <v>0.267064280980782</v>
       </c>
       <c r="AB22" s="9">
         <f t="shared" si="5"/>
-        <v>0.34129967776584319</v>
+        <v>0.26629469946741058</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B23" s="2">
-        <v>1967</v>
+        <v>0</v>
       </c>
       <c r="C23" s="2">
-        <v>3650</v>
+        <v>3356</v>
       </c>
       <c r="D23" s="2">
-        <v>4118</v>
+        <v>3356</v>
       </c>
       <c r="E23" s="2">
-        <v>4083</v>
+        <v>3356</v>
       </c>
       <c r="F23" s="2">
-        <v>6038</v>
+        <v>8209</v>
       </c>
       <c r="G23" s="2">
-        <v>5882</v>
+        <v>7661</v>
       </c>
       <c r="H23" s="2">
-        <v>3992</v>
+        <v>5109</v>
       </c>
       <c r="I23" s="2">
-        <v>377</v>
+        <v>6</v>
       </c>
       <c r="J23" s="2">
-        <v>2343</v>
+        <v>2</v>
       </c>
       <c r="K23" s="2">
-        <v>1194</v>
+        <v>3525</v>
       </c>
       <c r="L23" s="2">
-        <v>1176</v>
+        <v>3525</v>
       </c>
       <c r="M23" s="2">
-        <v>5296</v>
+        <v>2271</v>
       </c>
       <c r="N23" s="2">
-        <v>2342</v>
+        <v>1638</v>
       </c>
       <c r="O23" s="1">
-        <v>1305</v>
+        <v>719</v>
       </c>
       <c r="P23" s="8">
         <f t="shared" si="0"/>
-        <v>0.87711162636634643</v>
+        <v>0.27664758192228045</v>
       </c>
       <c r="Q23" s="8">
         <f t="shared" si="1"/>
-        <v>0.39816388983339002</v>
+        <v>0.21381020754470695</v>
       </c>
       <c r="R23" s="8">
         <f t="shared" si="2"/>
-        <v>0.32690380761523047</v>
+        <v>0.14073204149540028</v>
       </c>
       <c r="S23" s="2">
         <v>0</v>
@@ -2899,122 +2889,122 @@
         <v>0</v>
       </c>
       <c r="W23" s="2">
-        <v>5387</v>
+        <v>2792</v>
       </c>
       <c r="X23" s="2">
-        <v>3045</v>
+        <v>2181</v>
       </c>
       <c r="Y23" s="1">
-        <v>1830</v>
+        <v>1164</v>
       </c>
       <c r="Z23" s="8">
         <f t="shared" si="3"/>
-        <v>0.89218284200066245</v>
+        <v>0.34011450846631747</v>
       </c>
       <c r="AA23" s="9">
         <f t="shared" si="4"/>
-        <v>0.51768106086365184</v>
+        <v>0.28468868293956401</v>
       </c>
       <c r="AB23" s="9">
         <f t="shared" si="5"/>
-        <v>0.45841683366733466</v>
+        <v>0.22783323546682324</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B24" s="2">
         <v>0</v>
       </c>
       <c r="C24" s="2">
-        <v>10616</v>
+        <v>0</v>
       </c>
       <c r="D24" s="2">
-        <v>11136</v>
+        <v>0</v>
       </c>
       <c r="E24" s="2">
-        <v>11136</v>
+        <v>0</v>
       </c>
       <c r="F24" s="2">
-        <v>8956</v>
+        <v>4060</v>
       </c>
       <c r="G24" s="2">
-        <v>8358</v>
+        <v>3836</v>
       </c>
       <c r="H24" s="2">
-        <v>7182</v>
+        <v>2830</v>
       </c>
       <c r="I24" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J24" s="2">
-        <v>19668</v>
+        <v>0</v>
       </c>
       <c r="K24" s="2">
-        <v>13892</v>
+        <v>4057</v>
       </c>
       <c r="L24" s="2">
-        <v>13892</v>
+        <v>4057</v>
       </c>
       <c r="M24" s="2">
-        <v>10288</v>
+        <v>768</v>
       </c>
       <c r="N24" s="2">
-        <v>3095</v>
+        <v>749</v>
       </c>
       <c r="O24" s="1">
-        <v>1760</v>
+        <v>302</v>
       </c>
       <c r="P24" s="8">
         <f t="shared" si="0"/>
-        <v>1.1487271103171059</v>
+        <v>0.18916256157635469</v>
       </c>
       <c r="Q24" s="8">
         <f t="shared" si="1"/>
-        <v>0.37030390045465422</v>
+        <v>0.19525547445255476</v>
       </c>
       <c r="R24" s="8">
         <f t="shared" si="2"/>
-        <v>0.24505708716235031</v>
+        <v>0.10671378091872792</v>
       </c>
       <c r="S24" s="2">
         <v>0</v>
       </c>
       <c r="T24" s="2">
-        <v>13542</v>
+        <v>0</v>
       </c>
       <c r="U24" s="2">
-        <v>6771</v>
+        <v>0</v>
       </c>
       <c r="V24" s="2">
-        <v>6771</v>
+        <v>0</v>
       </c>
       <c r="W24" s="2">
-        <v>10423</v>
+        <v>953</v>
       </c>
       <c r="X24" s="2">
-        <v>2961</v>
+        <v>845</v>
       </c>
       <c r="Y24" s="1">
-        <v>2086</v>
+        <v>553</v>
       </c>
       <c r="Z24" s="8">
         <f t="shared" si="3"/>
-        <v>1.163800803930326</v>
+        <v>0.23472906403940888</v>
       </c>
       <c r="AA24" s="9">
         <f t="shared" si="4"/>
-        <v>0.35427135678391958</v>
+        <v>0.22028154327424401</v>
       </c>
       <c r="AB24" s="9">
         <f t="shared" si="5"/>
-        <v>0.29044834307992201</v>
+        <v>0.19540636042402826</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B25" s="2">
         <v>0</v>
@@ -3029,230 +3019,230 @@
         <v>0</v>
       </c>
       <c r="F25" s="2">
-        <v>7230</v>
+        <v>3842</v>
       </c>
       <c r="G25" s="2">
-        <v>6475</v>
+        <v>3768</v>
       </c>
       <c r="H25" s="2">
-        <v>5604</v>
+        <v>2651</v>
       </c>
       <c r="I25" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J25" s="2">
-        <v>19670</v>
+        <v>1</v>
       </c>
       <c r="K25" s="2">
-        <v>6992</v>
+        <v>0</v>
       </c>
       <c r="L25" s="2">
-        <v>19670</v>
+        <v>1</v>
       </c>
       <c r="M25" s="2">
-        <v>10276</v>
+        <v>793</v>
       </c>
       <c r="N25" s="2">
-        <v>3171</v>
+        <v>808</v>
       </c>
       <c r="O25" s="1">
-        <v>1765</v>
+        <v>331</v>
       </c>
       <c r="P25" s="8">
         <f t="shared" si="0"/>
-        <v>1.4213001383125865</v>
+        <v>0.20640291514836023</v>
       </c>
       <c r="Q25" s="8">
         <f t="shared" si="1"/>
-        <v>0.48972972972972972</v>
+        <v>0.21443736730360935</v>
       </c>
       <c r="R25" s="8">
         <f t="shared" si="2"/>
-        <v>0.31495360456816557</v>
+        <v>0.12485854394568087</v>
       </c>
       <c r="S25" s="2">
         <v>0</v>
       </c>
       <c r="T25" s="2">
-        <v>13542</v>
+        <v>0</v>
       </c>
       <c r="U25" s="2">
         <v>0</v>
       </c>
       <c r="V25" s="2">
-        <v>13542</v>
+        <v>0</v>
       </c>
       <c r="W25" s="2">
-        <v>10376</v>
+        <v>983</v>
       </c>
       <c r="X25" s="2">
-        <v>2925</v>
+        <v>825</v>
       </c>
       <c r="Y25" s="1">
-        <v>1990</v>
+        <v>542</v>
       </c>
       <c r="Z25" s="8">
         <f t="shared" si="3"/>
-        <v>1.4351313969571231</v>
+        <v>0.25585632483081727</v>
       </c>
       <c r="AA25" s="9">
         <f t="shared" si="4"/>
-        <v>0.45173745173745172</v>
+        <v>0.21894904458598727</v>
       </c>
       <c r="AB25" s="9">
         <f t="shared" si="5"/>
-        <v>0.35510349750178444</v>
+        <v>0.20445115050924179</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B26" s="2">
         <v>0</v>
       </c>
       <c r="C26" s="2">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="D26" s="2">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="E26" s="2">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="F26" s="2">
-        <v>5547</v>
+        <v>5624</v>
       </c>
       <c r="G26" s="2">
-        <v>5219</v>
-      </c>
-      <c r="H26" s="29">
-        <v>7375</v>
+        <v>5243</v>
+      </c>
+      <c r="H26" s="2">
+        <v>3724</v>
       </c>
       <c r="I26" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J26" s="2">
-        <v>33412</v>
+        <v>7050</v>
       </c>
       <c r="K26" s="2">
-        <v>16707</v>
+        <v>3525</v>
       </c>
       <c r="L26" s="2">
-        <v>16707</v>
+        <v>3525</v>
       </c>
       <c r="M26" s="2">
-        <v>5134</v>
+        <v>2195</v>
       </c>
       <c r="N26" s="2">
-        <v>1740</v>
+        <v>1726</v>
       </c>
       <c r="O26" s="1">
-        <v>803</v>
+        <v>843</v>
       </c>
       <c r="P26" s="8">
         <f t="shared" si="0"/>
-        <v>0.92554533982332787</v>
+        <v>0.39029160739687058</v>
       </c>
       <c r="Q26" s="8">
         <f t="shared" si="1"/>
-        <v>0.33339720252922017</v>
+        <v>0.32920083921419035</v>
       </c>
       <c r="R26" s="8">
         <f t="shared" si="2"/>
-        <v>0.10888135593220338</v>
+        <v>0.22636949516648766</v>
       </c>
       <c r="S26" s="2">
         <v>0</v>
       </c>
       <c r="T26" s="2">
-        <v>24184</v>
+        <v>0</v>
       </c>
       <c r="U26" s="2">
-        <v>12092</v>
+        <v>0</v>
       </c>
       <c r="V26" s="2">
-        <v>12097</v>
+        <v>0</v>
       </c>
       <c r="W26" s="2">
-        <v>5190</v>
+        <v>2694</v>
       </c>
       <c r="X26" s="2">
-        <v>1717</v>
+        <v>1949</v>
       </c>
       <c r="Y26" s="1">
-        <v>1170</v>
+        <v>1271</v>
       </c>
       <c r="Z26" s="8">
         <f t="shared" si="3"/>
-        <v>0.93564088696592751</v>
+        <v>0.47901849217638692</v>
       </c>
       <c r="AA26" s="9">
         <f t="shared" si="4"/>
-        <v>0.3289902280130293</v>
+        <v>0.371733740225062</v>
       </c>
       <c r="AB26" s="9">
         <f t="shared" si="5"/>
-        <v>0.15864406779661017</v>
+        <v>0.34129967776584319</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B27" s="2">
-        <v>0</v>
+        <v>1967</v>
       </c>
       <c r="C27" s="2">
-        <v>38</v>
+        <v>3650</v>
       </c>
       <c r="D27" s="2">
-        <v>38</v>
+        <v>4118</v>
       </c>
       <c r="E27" s="2">
-        <v>38</v>
+        <v>4083</v>
       </c>
       <c r="F27" s="2">
-        <v>11175</v>
+        <v>6038</v>
       </c>
       <c r="G27" s="2">
-        <v>10415</v>
+        <v>5882</v>
       </c>
       <c r="H27" s="2">
-        <v>9052</v>
+        <v>3992</v>
       </c>
       <c r="I27" s="2">
-        <v>4</v>
+        <v>377</v>
       </c>
       <c r="J27" s="2">
-        <v>3949</v>
+        <v>2343</v>
       </c>
       <c r="K27" s="2">
-        <v>4490</v>
+        <v>1194</v>
       </c>
       <c r="L27" s="2">
-        <v>4490</v>
+        <v>1176</v>
       </c>
       <c r="M27" s="2">
-        <v>4512</v>
+        <v>5296</v>
       </c>
       <c r="N27" s="2">
-        <v>3076</v>
+        <v>2342</v>
       </c>
       <c r="O27" s="1">
-        <v>1850</v>
+        <v>1305</v>
       </c>
       <c r="P27" s="8">
         <f t="shared" si="0"/>
-        <v>0.40375838926174495</v>
+        <v>0.87711162636634643</v>
       </c>
       <c r="Q27" s="8">
         <f t="shared" si="1"/>
-        <v>0.29534325492078733</v>
+        <v>0.39816388983339002</v>
       </c>
       <c r="R27" s="8">
         <f t="shared" si="2"/>
-        <v>0.20437472381794078</v>
+        <v>0.32690380761523047</v>
       </c>
       <c r="S27" s="2">
         <v>0</v>
@@ -3267,30 +3257,30 @@
         <v>0</v>
       </c>
       <c r="W27" s="2">
-        <v>4160</v>
+        <v>5387</v>
       </c>
       <c r="X27" s="2">
-        <v>3411</v>
+        <v>3045</v>
       </c>
       <c r="Y27" s="1">
-        <v>2186</v>
+        <v>1830</v>
       </c>
       <c r="Z27" s="8">
         <f t="shared" si="3"/>
-        <v>0.37225950782997763</v>
+        <v>0.89218284200066245</v>
       </c>
       <c r="AA27" s="9">
         <f t="shared" si="4"/>
-        <v>0.32750840134421505</v>
+        <v>0.51768106086365184</v>
       </c>
       <c r="AB27" s="9">
         <f t="shared" si="5"/>
-        <v>0.24149359257622624</v>
+        <v>0.45841683366733466</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B28" s="2">
         <v>0</v>
@@ -3305,84 +3295,84 @@
         <v>0</v>
       </c>
       <c r="F28" s="2">
-        <v>3009</v>
+        <v>6184</v>
       </c>
       <c r="G28" s="2">
-        <v>2638</v>
-      </c>
-      <c r="H28" s="2">
-        <v>2418</v>
+        <v>6114</v>
+      </c>
+      <c r="H28" s="28">
+        <v>7182</v>
       </c>
       <c r="I28" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J28" s="2">
-        <v>1</v>
+        <v>19668</v>
       </c>
       <c r="K28" s="2">
-        <v>1</v>
+        <v>13892</v>
       </c>
       <c r="L28" s="2">
-        <v>1</v>
+        <v>13892</v>
       </c>
       <c r="M28" s="2">
-        <v>973</v>
+        <v>10631</v>
       </c>
       <c r="N28" s="2">
-        <v>603</v>
+        <v>3232</v>
       </c>
       <c r="O28" s="1">
-        <v>259</v>
+        <v>1760</v>
       </c>
       <c r="P28" s="8">
         <f t="shared" si="0"/>
-        <v>0.32336324360252577</v>
+        <v>1.7191138421733505</v>
       </c>
       <c r="Q28" s="8">
         <f t="shared" si="1"/>
-        <v>0.22858225928733888</v>
+        <v>0.52862283284265621</v>
       </c>
       <c r="R28" s="8">
         <f t="shared" si="2"/>
-        <v>0.10711331679073614</v>
+        <v>0.24505708716235031</v>
       </c>
       <c r="S28" s="2">
         <v>0</v>
       </c>
       <c r="T28" s="2">
-        <v>0</v>
+        <v>13542</v>
       </c>
       <c r="U28" s="2">
-        <v>0</v>
+        <v>6771</v>
       </c>
       <c r="V28" s="2">
-        <v>0</v>
+        <v>6771</v>
       </c>
       <c r="W28" s="2">
-        <v>903</v>
+        <v>10789</v>
       </c>
       <c r="X28" s="2">
-        <v>659</v>
+        <v>3063</v>
       </c>
       <c r="Y28" s="1">
-        <v>383</v>
+        <v>2086</v>
       </c>
       <c r="Z28" s="8">
         <f t="shared" si="3"/>
-        <v>0.30009970089730809</v>
+        <v>1.7446636481241915</v>
       </c>
       <c r="AA28" s="9">
         <f t="shared" si="4"/>
-        <v>0.24981046247156938</v>
+        <v>0.50098135426889112</v>
       </c>
       <c r="AB28" s="9">
         <f t="shared" si="5"/>
-        <v>0.15839536807278742</v>
+        <v>0.29044834307992201</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B29" s="2">
         <v>0</v>
@@ -3397,710 +3387,1078 @@
         <v>0</v>
       </c>
       <c r="F29" s="2">
-        <v>3975</v>
+        <v>7230</v>
       </c>
       <c r="G29" s="2">
-        <v>3351</v>
+        <v>6475</v>
       </c>
       <c r="H29" s="2">
-        <v>2983</v>
+        <v>5604</v>
       </c>
       <c r="I29" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J29" s="2">
-        <v>162</v>
+        <v>19670</v>
       </c>
       <c r="K29" s="2">
-        <v>3009</v>
+        <v>6992</v>
       </c>
       <c r="L29" s="2">
-        <v>3009</v>
+        <v>19670</v>
       </c>
       <c r="M29" s="2">
-        <v>1893</v>
+        <v>10276</v>
       </c>
       <c r="N29" s="2">
-        <v>1233</v>
+        <v>3171</v>
       </c>
       <c r="O29" s="1">
-        <v>569</v>
+        <v>1765</v>
       </c>
       <c r="P29" s="8">
         <f t="shared" si="0"/>
-        <v>0.47622641509433961</v>
+        <v>1.4213001383125865</v>
       </c>
       <c r="Q29" s="8">
         <f t="shared" si="1"/>
-        <v>0.36794986571172783</v>
+        <v>0.48972972972972972</v>
       </c>
       <c r="R29" s="8">
         <f t="shared" si="2"/>
-        <v>0.19074756956084479</v>
+        <v>0.31495360456816557</v>
       </c>
       <c r="S29" s="2">
         <v>0</v>
       </c>
       <c r="T29" s="2">
-        <v>0</v>
+        <v>13542</v>
       </c>
       <c r="U29" s="2">
         <v>0</v>
       </c>
       <c r="V29" s="2">
-        <v>0</v>
+        <v>13542</v>
       </c>
       <c r="W29" s="2">
-        <v>1916</v>
+        <v>10376</v>
       </c>
       <c r="X29" s="2">
-        <v>1358</v>
+        <v>2925</v>
       </c>
       <c r="Y29" s="1">
-        <v>802</v>
+        <v>1990</v>
       </c>
       <c r="Z29" s="8">
         <f t="shared" si="3"/>
-        <v>0.48201257861635222</v>
+        <v>1.4351313969571231</v>
       </c>
       <c r="AA29" s="9">
         <f t="shared" si="4"/>
-        <v>0.40525216353327365</v>
+        <v>0.45173745173745172</v>
       </c>
       <c r="AB29" s="9">
         <f t="shared" si="5"/>
-        <v>0.26885685551458266</v>
+        <v>0.35510349750178444</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B30" s="2">
-        <v>238</v>
+        <v>0</v>
       </c>
       <c r="C30" s="2">
-        <v>218</v>
+        <v>0</v>
       </c>
       <c r="D30" s="2">
-        <v>203</v>
+        <v>0</v>
       </c>
       <c r="E30" s="2">
-        <v>203</v>
+        <v>0</v>
       </c>
       <c r="F30" s="2">
-        <v>5447</v>
+        <v>5547</v>
       </c>
       <c r="G30" s="2">
-        <v>7387</v>
-      </c>
-      <c r="H30" s="2">
-        <v>5973</v>
+        <v>5219</v>
+      </c>
+      <c r="H30" s="28">
+        <v>7375</v>
       </c>
       <c r="I30" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J30" s="2">
-        <v>28860</v>
+        <v>33412</v>
       </c>
       <c r="K30" s="2">
-        <v>14432</v>
+        <v>16707</v>
       </c>
       <c r="L30" s="2">
-        <v>14432</v>
+        <v>16707</v>
       </c>
       <c r="M30" s="2">
-        <v>2333</v>
+        <v>5134</v>
       </c>
       <c r="N30" s="2">
-        <v>1608</v>
-      </c>
-      <c r="O30" s="2">
-        <v>668</v>
-      </c>
-      <c r="P30" s="15">
+        <v>1740</v>
+      </c>
+      <c r="O30" s="1">
+        <v>803</v>
+      </c>
+      <c r="P30" s="8">
         <f t="shared" si="0"/>
-        <v>0.42830916100605837</v>
-      </c>
-      <c r="Q30" s="15">
+        <v>0.92554533982332787</v>
+      </c>
+      <c r="Q30" s="8">
         <f t="shared" si="1"/>
-        <v>0.21767970759442262</v>
+        <v>0.33339720252922017</v>
       </c>
       <c r="R30" s="8">
         <f t="shared" si="2"/>
-        <v>0.11183659802444333</v>
+        <v>0.10888135593220338</v>
       </c>
       <c r="S30" s="2">
         <v>0</v>
       </c>
       <c r="T30" s="2">
-        <v>27728</v>
+        <v>24184</v>
       </c>
       <c r="U30" s="2">
-        <v>13864</v>
+        <v>12092</v>
       </c>
       <c r="V30" s="2">
-        <v>13864</v>
+        <v>12097</v>
       </c>
       <c r="W30" s="2">
-        <v>2897</v>
+        <v>5190</v>
       </c>
       <c r="X30" s="2">
-        <v>1759</v>
-      </c>
-      <c r="Y30" s="2">
-        <v>1139</v>
-      </c>
-      <c r="Z30" s="15">
+        <v>1717</v>
+      </c>
+      <c r="Y30" s="1">
+        <v>1170</v>
+      </c>
+      <c r="Z30" s="8">
         <f t="shared" si="3"/>
-        <v>0.53185239581420962</v>
-      </c>
-      <c r="AA30" s="16">
+        <v>0.93564088696592751</v>
+      </c>
+      <c r="AA30" s="9">
         <f t="shared" si="4"/>
-        <v>0.23812102341952077</v>
+        <v>0.3289902280130293</v>
       </c>
       <c r="AB30" s="9">
         <f t="shared" si="5"/>
-        <v>0.19069144483509123</v>
+        <v>0.15864406779661017</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B31" s="2">
-        <v>164</v>
+        <v>0</v>
       </c>
       <c r="C31" s="2">
-        <v>185</v>
+        <v>38</v>
       </c>
       <c r="D31" s="2">
-        <v>185</v>
+        <v>38</v>
       </c>
       <c r="E31" s="2">
-        <v>185</v>
+        <v>38</v>
       </c>
       <c r="F31" s="2">
-        <v>5296</v>
+        <v>11175</v>
       </c>
       <c r="G31" s="2">
-        <v>7450</v>
+        <v>10415</v>
       </c>
       <c r="H31" s="2">
-        <v>5905</v>
+        <v>9052</v>
       </c>
       <c r="I31" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J31" s="2">
-        <v>14454</v>
+        <v>3949</v>
       </c>
       <c r="K31" s="2">
-        <v>13053</v>
+        <v>4490</v>
       </c>
       <c r="L31" s="2">
-        <v>14454</v>
+        <v>4490</v>
       </c>
       <c r="M31" s="2">
-        <v>4979</v>
+        <v>4512</v>
       </c>
       <c r="N31" s="2">
-        <v>2652</v>
-      </c>
-      <c r="O31" s="2">
-        <v>1426</v>
-      </c>
-      <c r="P31" s="15">
+        <v>3076</v>
+      </c>
+      <c r="O31" s="1">
+        <v>1850</v>
+      </c>
+      <c r="P31" s="8">
         <f t="shared" si="0"/>
-        <v>0.94014350453172202</v>
-      </c>
-      <c r="Q31" s="15">
+        <v>0.40375838926174495</v>
+      </c>
+      <c r="Q31" s="8">
         <f t="shared" si="1"/>
-        <v>0.35597315436241611</v>
+        <v>0.29534325492078733</v>
       </c>
       <c r="R31" s="8">
         <f t="shared" si="2"/>
-        <v>0.24149026248941574</v>
+        <v>0.20437472381794078</v>
       </c>
       <c r="S31" s="2">
         <v>0</v>
       </c>
       <c r="T31" s="2">
-        <v>13867</v>
+        <v>0</v>
       </c>
       <c r="U31" s="2">
-        <v>11569</v>
+        <v>0</v>
       </c>
       <c r="V31" s="2">
-        <v>13867</v>
+        <v>0</v>
       </c>
       <c r="W31" s="2">
-        <v>5292</v>
+        <v>4160</v>
       </c>
       <c r="X31" s="2">
-        <v>3064</v>
-      </c>
-      <c r="Y31" s="2">
-        <v>1870</v>
-      </c>
-      <c r="Z31" s="15">
+        <v>3411</v>
+      </c>
+      <c r="Y31" s="1">
+        <v>2186</v>
+      </c>
+      <c r="Z31" s="8">
         <f t="shared" si="3"/>
-        <v>0.99924471299093653</v>
-      </c>
-      <c r="AA31" s="16">
+        <v>0.37225950782997763</v>
+      </c>
+      <c r="AA31" s="9">
         <f t="shared" si="4"/>
-        <v>0.41127516778523487</v>
+        <v>0.32750840134421505</v>
       </c>
       <c r="AB31" s="9">
         <f t="shared" si="5"/>
-        <v>0.31668077900084673</v>
+        <v>0.24149359257622624</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B32" s="2">
+        <v>0</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0</v>
+      </c>
+      <c r="F32" s="2">
+        <v>3009</v>
+      </c>
+      <c r="G32" s="2">
+        <v>2638</v>
+      </c>
+      <c r="H32" s="2">
+        <v>2418</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1</v>
+      </c>
+      <c r="J32" s="2">
+        <v>1</v>
+      </c>
+      <c r="K32" s="2">
+        <v>1</v>
+      </c>
+      <c r="L32" s="2">
+        <v>1</v>
+      </c>
+      <c r="M32" s="2">
+        <v>973</v>
+      </c>
+      <c r="N32" s="2">
+        <v>603</v>
+      </c>
+      <c r="O32" s="1">
+        <v>259</v>
+      </c>
+      <c r="P32" s="8">
+        <f t="shared" si="0"/>
+        <v>0.32336324360252577</v>
+      </c>
+      <c r="Q32" s="8">
+        <f t="shared" si="1"/>
+        <v>0.22858225928733888</v>
+      </c>
+      <c r="R32" s="8">
+        <f t="shared" si="2"/>
+        <v>0.10711331679073614</v>
+      </c>
+      <c r="S32" s="2">
+        <v>0</v>
+      </c>
+      <c r="T32" s="2">
+        <v>0</v>
+      </c>
+      <c r="U32" s="2">
+        <v>0</v>
+      </c>
+      <c r="V32" s="2">
+        <v>0</v>
+      </c>
+      <c r="W32" s="2">
+        <v>903</v>
+      </c>
+      <c r="X32" s="2">
+        <v>659</v>
+      </c>
+      <c r="Y32" s="1">
+        <v>383</v>
+      </c>
+      <c r="Z32" s="8">
+        <f t="shared" si="3"/>
+        <v>0.30009970089730809</v>
+      </c>
+      <c r="AA32" s="9">
+        <f t="shared" si="4"/>
+        <v>0.24981046247156938</v>
+      </c>
+      <c r="AB32" s="9">
+        <f t="shared" si="5"/>
+        <v>0.15839536807278742</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2">
+        <v>3975</v>
+      </c>
+      <c r="G33" s="2">
+        <v>3351</v>
+      </c>
+      <c r="H33" s="2">
+        <v>2983</v>
+      </c>
+      <c r="I33" s="2">
+        <v>0</v>
+      </c>
+      <c r="J33" s="2">
+        <v>162</v>
+      </c>
+      <c r="K33" s="2">
+        <v>3009</v>
+      </c>
+      <c r="L33" s="2">
+        <v>3009</v>
+      </c>
+      <c r="M33" s="2">
+        <v>1893</v>
+      </c>
+      <c r="N33" s="2">
+        <v>1233</v>
+      </c>
+      <c r="O33" s="1">
+        <v>569</v>
+      </c>
+      <c r="P33" s="8">
+        <f t="shared" si="0"/>
+        <v>0.47622641509433961</v>
+      </c>
+      <c r="Q33" s="8">
+        <f t="shared" si="1"/>
+        <v>0.36794986571172783</v>
+      </c>
+      <c r="R33" s="8">
+        <f t="shared" si="2"/>
+        <v>0.19074756956084479</v>
+      </c>
+      <c r="S33" s="2">
+        <v>0</v>
+      </c>
+      <c r="T33" s="2">
+        <v>0</v>
+      </c>
+      <c r="U33" s="2">
+        <v>0</v>
+      </c>
+      <c r="V33" s="2">
+        <v>0</v>
+      </c>
+      <c r="W33" s="2">
+        <v>1916</v>
+      </c>
+      <c r="X33" s="2">
+        <v>1358</v>
+      </c>
+      <c r="Y33" s="1">
+        <v>802</v>
+      </c>
+      <c r="Z33" s="8">
+        <f t="shared" si="3"/>
+        <v>0.48201257861635222</v>
+      </c>
+      <c r="AA33" s="9">
+        <f t="shared" si="4"/>
+        <v>0.40525216353327365</v>
+      </c>
+      <c r="AB33" s="9">
+        <f t="shared" si="5"/>
+        <v>0.26885685551458266</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="2">
+        <v>238</v>
+      </c>
+      <c r="C34" s="2">
+        <v>218</v>
+      </c>
+      <c r="D34" s="2">
+        <v>203</v>
+      </c>
+      <c r="E34" s="2">
+        <v>203</v>
+      </c>
+      <c r="F34" s="2">
+        <v>5447</v>
+      </c>
+      <c r="G34" s="2">
+        <v>7387</v>
+      </c>
+      <c r="H34" s="2">
+        <v>5973</v>
+      </c>
+      <c r="I34" s="2">
+        <v>2</v>
+      </c>
+      <c r="J34" s="2">
+        <v>28860</v>
+      </c>
+      <c r="K34" s="2">
+        <v>14432</v>
+      </c>
+      <c r="L34" s="2">
+        <v>14432</v>
+      </c>
+      <c r="M34" s="2">
+        <v>2333</v>
+      </c>
+      <c r="N34" s="2">
+        <v>1608</v>
+      </c>
+      <c r="O34" s="2">
+        <v>668</v>
+      </c>
+      <c r="P34" s="15">
+        <f t="shared" si="0"/>
+        <v>0.42830916100605837</v>
+      </c>
+      <c r="Q34" s="15">
+        <f t="shared" si="1"/>
+        <v>0.21767970759442262</v>
+      </c>
+      <c r="R34" s="8">
+        <f t="shared" si="2"/>
+        <v>0.11183659802444333</v>
+      </c>
+      <c r="S34" s="2">
+        <v>0</v>
+      </c>
+      <c r="T34" s="2">
+        <v>27728</v>
+      </c>
+      <c r="U34" s="2">
+        <v>13864</v>
+      </c>
+      <c r="V34" s="2">
+        <v>13864</v>
+      </c>
+      <c r="W34" s="2">
+        <v>2897</v>
+      </c>
+      <c r="X34" s="2">
+        <v>1759</v>
+      </c>
+      <c r="Y34" s="2">
+        <v>1139</v>
+      </c>
+      <c r="Z34" s="15">
+        <f t="shared" si="3"/>
+        <v>0.53185239581420962</v>
+      </c>
+      <c r="AA34" s="16">
+        <f t="shared" si="4"/>
+        <v>0.23812102341952077</v>
+      </c>
+      <c r="AB34" s="9">
+        <f t="shared" si="5"/>
+        <v>0.19069144483509123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="2">
+        <v>164</v>
+      </c>
+      <c r="C35" s="2">
+        <v>185</v>
+      </c>
+      <c r="D35" s="2">
+        <v>185</v>
+      </c>
+      <c r="E35" s="2">
+        <v>185</v>
+      </c>
+      <c r="F35" s="2">
+        <v>5296</v>
+      </c>
+      <c r="G35" s="2">
+        <v>7450</v>
+      </c>
+      <c r="H35" s="2">
+        <v>5905</v>
+      </c>
+      <c r="I35" s="2">
+        <v>2</v>
+      </c>
+      <c r="J35" s="2">
+        <v>14454</v>
+      </c>
+      <c r="K35" s="2">
+        <v>13053</v>
+      </c>
+      <c r="L35" s="2">
+        <v>14454</v>
+      </c>
+      <c r="M35" s="2">
+        <v>4979</v>
+      </c>
+      <c r="N35" s="2">
+        <v>2652</v>
+      </c>
+      <c r="O35" s="2">
+        <v>1426</v>
+      </c>
+      <c r="P35" s="15">
+        <f t="shared" si="0"/>
+        <v>0.94014350453172202</v>
+      </c>
+      <c r="Q35" s="15">
+        <f t="shared" si="1"/>
+        <v>0.35597315436241611</v>
+      </c>
+      <c r="R35" s="8">
+        <f t="shared" si="2"/>
+        <v>0.24149026248941574</v>
+      </c>
+      <c r="S35" s="2">
+        <v>0</v>
+      </c>
+      <c r="T35" s="2">
+        <v>13867</v>
+      </c>
+      <c r="U35" s="2">
+        <v>11569</v>
+      </c>
+      <c r="V35" s="2">
+        <v>13867</v>
+      </c>
+      <c r="W35" s="2">
+        <v>5292</v>
+      </c>
+      <c r="X35" s="2">
+        <v>3064</v>
+      </c>
+      <c r="Y35" s="2">
+        <v>1870</v>
+      </c>
+      <c r="Z35" s="15">
+        <f t="shared" si="3"/>
+        <v>0.99924471299093653</v>
+      </c>
+      <c r="AA35" s="16">
+        <f t="shared" si="4"/>
+        <v>0.41127516778523487</v>
+      </c>
+      <c r="AB35" s="9">
+        <f t="shared" si="5"/>
+        <v>0.31668077900084673</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" s="2">
         <v>65536</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C36" s="2">
         <v>65536</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D36" s="2">
         <v>65536</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E36" s="2">
         <v>65536</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F36" s="2">
         <v>22222</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G36" s="2">
         <v>22222</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H36" s="2">
         <v>22222</v>
       </c>
-      <c r="I32" s="2">
+      <c r="I36" s="2">
         <v>6</v>
       </c>
-      <c r="J32" s="2">
+      <c r="J36" s="2">
         <v>5</v>
       </c>
-      <c r="K32" s="2">
+      <c r="K36" s="2">
         <v>5</v>
       </c>
-      <c r="L32" s="2">
+      <c r="L36" s="2">
         <v>6</v>
       </c>
-      <c r="M32" s="2">
+      <c r="M36" s="2">
         <v>9084</v>
       </c>
-      <c r="N32" s="2">
+      <c r="N36" s="2">
         <v>5827</v>
       </c>
-      <c r="O32" s="2">
+      <c r="O36" s="2">
         <v>3771</v>
       </c>
-      <c r="P32" s="15">
+      <c r="P36" s="15">
         <f t="shared" si="0"/>
         <v>0.40878408784087839</v>
       </c>
-      <c r="Q32" s="15">
+      <c r="Q36" s="15">
         <f t="shared" si="1"/>
         <v>0.26221762217622174</v>
       </c>
-      <c r="R32" s="8">
+      <c r="R36" s="8">
         <f t="shared" si="2"/>
         <v>0.16969669696696968</v>
       </c>
-      <c r="S32" s="2">
-        <v>0</v>
-      </c>
-      <c r="T32" s="2">
-        <v>0</v>
-      </c>
-      <c r="U32" s="2">
-        <v>0</v>
-      </c>
-      <c r="V32" s="2">
-        <v>0</v>
-      </c>
-      <c r="W32" s="2">
+      <c r="S36" s="2">
+        <v>0</v>
+      </c>
+      <c r="T36" s="2">
+        <v>0</v>
+      </c>
+      <c r="U36" s="2">
+        <v>0</v>
+      </c>
+      <c r="V36" s="2">
+        <v>0</v>
+      </c>
+      <c r="W36" s="2">
         <v>9800</v>
       </c>
-      <c r="X32" s="2">
+      <c r="X36" s="2">
         <v>7285</v>
       </c>
-      <c r="Y32" s="2">
+      <c r="Y36" s="2">
         <v>5126</v>
       </c>
-      <c r="Z32" s="15">
+      <c r="Z36" s="15">
         <f t="shared" si="3"/>
         <v>0.44100441004410046</v>
       </c>
-      <c r="AA32" s="16">
+      <c r="AA36" s="16">
         <f t="shared" si="4"/>
         <v>0.32782827828278283</v>
       </c>
-      <c r="AB32" s="9">
+      <c r="AB36" s="9">
         <f t="shared" si="5"/>
         <v>0.23067230672306724</v>
       </c>
     </row>
-    <row r="33" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B33" s="11">
+    <row r="37" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="11">
         <v>65536</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C37" s="11">
         <v>65536</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D37" s="11">
         <v>65536</v>
       </c>
-      <c r="E33" s="11">
+      <c r="E37" s="11">
         <v>65536</v>
       </c>
-      <c r="F33" s="11">
+      <c r="F37" s="11">
         <v>22222</v>
       </c>
-      <c r="G33" s="11">
+      <c r="G37" s="11">
         <v>22222</v>
       </c>
-      <c r="H33" s="11">
+      <c r="H37" s="11">
         <v>22222</v>
       </c>
-      <c r="I33" s="11">
+      <c r="I37" s="11">
         <v>2</v>
       </c>
-      <c r="J33" s="11">
+      <c r="J37" s="11">
         <v>11169</v>
       </c>
-      <c r="K33" s="11">
+      <c r="K37" s="11">
         <v>1975</v>
       </c>
-      <c r="L33" s="11">
+      <c r="L37" s="11">
         <v>13140</v>
       </c>
-      <c r="M33" s="11">
+      <c r="M37" s="11">
         <v>9598</v>
       </c>
-      <c r="N33" s="11">
+      <c r="N37" s="11">
         <v>5366</v>
       </c>
-      <c r="O33" s="11">
+      <c r="O37" s="11">
         <v>3366</v>
       </c>
-      <c r="P33" s="12">
+      <c r="P37" s="12">
         <f t="shared" si="0"/>
         <v>0.43191431914319145</v>
       </c>
-      <c r="Q33" s="12">
+      <c r="Q37" s="12">
         <f t="shared" si="1"/>
         <v>0.24147241472414724</v>
       </c>
-      <c r="R33" s="12">
+      <c r="R37" s="12">
         <f t="shared" si="2"/>
         <v>0.15147151471514717</v>
       </c>
-      <c r="S33" s="11">
-        <v>0</v>
-      </c>
-      <c r="T33" s="11">
+      <c r="S37" s="11">
+        <v>0</v>
+      </c>
+      <c r="T37" s="11">
         <v>8867</v>
       </c>
-      <c r="U33" s="11">
+      <c r="U37" s="11">
         <v>927</v>
       </c>
-      <c r="V33" s="11">
+      <c r="V37" s="11">
         <v>9794</v>
       </c>
-      <c r="W33" s="11">
+      <c r="W37" s="11">
         <v>22644</v>
       </c>
-      <c r="X33" s="11">
+      <c r="X37" s="11">
         <v>15498</v>
       </c>
-      <c r="Y33" s="11">
+      <c r="Y37" s="11">
         <v>10750</v>
       </c>
-      <c r="Z33" s="12">
+      <c r="Z37" s="12">
         <f t="shared" si="3"/>
         <v>1.0189901899018989</v>
       </c>
-      <c r="AA33" s="13">
+      <c r="AA37" s="13">
         <f t="shared" si="4"/>
         <v>0.69741697416974169</v>
       </c>
-      <c r="AB33" s="13">
+      <c r="AB37" s="13">
         <f t="shared" si="5"/>
         <v>0.4837548375483755</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A34" s="23" t="s">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A38" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="26">
+      <c r="B38" s="25">
         <f>COUNTIF(B2:B5,"=0")/4</f>
         <v>1</v>
       </c>
-      <c r="C34" s="26">
-        <f t="shared" ref="C34:E34" si="6">COUNTIF(C2:C5,"=0")/4</f>
+      <c r="C38" s="25">
+        <f t="shared" ref="C38:E38" si="6">COUNTIF(C2:C5,"=0")/4</f>
         <v>1</v>
       </c>
-      <c r="D34" s="26">
+      <c r="D38" s="25">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="E34" s="26">
+      <c r="E38" s="25">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="26">
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="25">
         <f>COUNTIF(I2:I5,"=0")/4</f>
         <v>1</v>
       </c>
-      <c r="J34" s="26">
-        <f t="shared" ref="J34:L34" si="7">COUNTIF(J2:J5,"=0")/4</f>
+      <c r="J38" s="25">
+        <f t="shared" ref="J38:L38" si="7">COUNTIF(J2:J5,"=0")/4</f>
         <v>0.5</v>
       </c>
-      <c r="K34" s="26">
+      <c r="K38" s="25">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
-      <c r="L34" s="26">
+      <c r="L38" s="25">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="17">
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="17">
         <f>AVERAGE(P2:P5)</f>
         <v>0.78928691016725028</v>
       </c>
-      <c r="Q34" s="17">
+      <c r="Q38" s="17">
         <f>AVERAGE(Q2:Q5)</f>
         <v>0.74151179774319675</v>
       </c>
-      <c r="R34" s="17">
+      <c r="R38" s="17">
         <f>AVERAGE(R2:R5)</f>
         <v>0.14808930291674494</v>
       </c>
-      <c r="S34" s="26">
+      <c r="S38" s="25">
         <f>COUNTIF(S2:S5,"=0")/4</f>
         <v>1</v>
       </c>
-      <c r="T34" s="26">
-        <f t="shared" ref="T34:V34" si="8">COUNTIF(T2:T5,"=0")/4</f>
+      <c r="T38" s="25">
+        <f t="shared" ref="T38:V38" si="8">COUNTIF(T2:T5,"=0")/4</f>
         <v>1</v>
       </c>
-      <c r="U34" s="26">
+      <c r="U38" s="25">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="V34" s="26">
+      <c r="V38" s="25">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="W34" s="1"/>
-      <c r="X34" s="1"/>
-      <c r="Y34" s="1"/>
-      <c r="Z34" s="17">
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+      <c r="Y38" s="1"/>
+      <c r="Z38" s="17">
         <f>AVERAGE(Z2:Z5)</f>
         <v>1.376890141406921</v>
       </c>
-      <c r="AA34" s="18">
+      <c r="AA38" s="18">
         <f>AVERAGE(AA2:AA5)</f>
         <v>0.96695974573752319</v>
       </c>
-      <c r="AB34" s="18">
+      <c r="AB38" s="18">
         <f>AVERAGE(AB2:AB5)</f>
         <v>0.72452141642573398</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A35" s="24" t="s">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A39" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="26">
+        <f>COUNTIF(B6:B37,"=0")/COUNTA(B6:B37)</f>
+        <v>0.75</v>
+      </c>
+      <c r="C39" s="26">
+        <f t="shared" ref="C39:E39" si="9">COUNTIF(C6:C37,"=0")/COUNTA(C6:C37)</f>
+        <v>0.59375</v>
+      </c>
+      <c r="D39" s="26">
+        <f t="shared" si="9"/>
+        <v>0.59375</v>
+      </c>
+      <c r="E39" s="26">
+        <f t="shared" si="9"/>
+        <v>0.59375</v>
+      </c>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="26">
+        <f>COUNTIF(I6:I37,"=0")/COUNTA(I6:I37)</f>
+        <v>0.25</v>
+      </c>
+      <c r="J39" s="26">
+        <f t="shared" ref="J39:L39" si="10">COUNTIF(J6:J37,"=0")/COUNTA(J6:J37)</f>
+        <v>0.1875</v>
+      </c>
+      <c r="K39" s="26">
+        <f t="shared" si="10"/>
+        <v>0.1875</v>
+      </c>
+      <c r="L39" s="26">
+        <f t="shared" si="10"/>
+        <v>0.15625</v>
+      </c>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="19">
+        <f>AVERAGE(P6:P37)</f>
+        <v>0.77859844354192587</v>
+      </c>
+      <c r="Q39" s="19">
+        <f t="shared" ref="Q39:R39" si="11">AVERAGE(Q6:Q37)</f>
+        <v>0.44336826366001769</v>
+      </c>
+      <c r="R39" s="19" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S39" s="26">
+        <f>COUNTIF(S6:S37,"=0")/COUNTA(S6:S37)</f>
+        <v>0.9375</v>
+      </c>
+      <c r="T39" s="26">
+        <f t="shared" ref="T39:V39" si="12">COUNTIF(T6:T37,"=0")/COUNTA(T6:T37)</f>
+        <v>0.65625</v>
+      </c>
+      <c r="U39" s="26">
+        <f t="shared" si="12"/>
+        <v>0.6875</v>
+      </c>
+      <c r="V39" s="26">
+        <f t="shared" si="12"/>
+        <v>0.65625</v>
+      </c>
+      <c r="W39" s="2"/>
+      <c r="X39" s="2"/>
+      <c r="Y39" s="2"/>
+      <c r="Z39" s="19">
+        <f>AVERAGE(Z6:Z37)</f>
+        <v>0.91303070312240198</v>
+      </c>
+      <c r="AA39" s="19">
+        <f t="shared" ref="AA39:AB39" si="13">AVERAGE(AA6:AA37)</f>
+        <v>0.47911807937164141</v>
+      </c>
+      <c r="AB39" s="19" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A40" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="27">
-        <f>COUNTIF(B6:B33,"=0")/28</f>
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="C35" s="27">
-        <f t="shared" ref="C35:E35" si="9">COUNTIF(C6:C33,"=0")/28</f>
-        <v>0.5</v>
-      </c>
-      <c r="D35" s="27">
-        <f t="shared" si="9"/>
-        <v>0.5</v>
-      </c>
-      <c r="E35" s="27">
-        <f t="shared" si="9"/>
-        <v>0.5</v>
-      </c>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="27">
-        <f>COUNTIF(I6:I33,"=0")/28</f>
-        <v>0.17857142857142858</v>
-      </c>
-      <c r="J35" s="27">
-        <f t="shared" ref="J35:L35" si="10">COUNTIF(J6:J33,"=0")/28</f>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="K35" s="27">
-        <f t="shared" si="10"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="L35" s="27">
-        <f t="shared" si="10"/>
-        <v>0.10714285714285714</v>
-      </c>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
-      <c r="P35" s="19">
-        <f>AVERAGE(P6:P33)</f>
-        <v>0.53183000969737049</v>
-      </c>
-      <c r="Q35" s="19">
-        <f>AVERAGE(Q6:Q33)</f>
-        <v>0.32585048252743559</v>
-      </c>
-      <c r="R35" s="19">
-        <f>AVERAGE(R6:R33)</f>
-        <v>0.20090093987977201</v>
-      </c>
-      <c r="S35" s="27">
-        <f>COUNTIF(S6:S33,"=0")/28</f>
-        <v>0.9285714285714286</v>
-      </c>
-      <c r="T35" s="27">
-        <f t="shared" ref="T35:V35" si="11">COUNTIF(T6:T33,"=0")/28</f>
-        <v>0.6071428571428571</v>
-      </c>
-      <c r="U35" s="27">
-        <f t="shared" si="11"/>
-        <v>0.6428571428571429</v>
-      </c>
-      <c r="V35" s="27">
-        <f t="shared" si="11"/>
-        <v>0.6071428571428571</v>
-      </c>
-      <c r="W35" s="2"/>
-      <c r="X35" s="2"/>
-      <c r="Y35" s="2"/>
-      <c r="Z35" s="19">
-        <f>AVERAGE(Z6:Z33)</f>
-        <v>0.6434887278021636</v>
-      </c>
-      <c r="AA35" s="20">
-        <f>AVERAGE(AA6:AA33)</f>
-        <v>0.36050214611308667</v>
-      </c>
-      <c r="AB35" s="20">
-        <f>AVERAGE(AB6:AB33)</f>
-        <v>0.2759874676415755</v>
-      </c>
-    </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A36" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="B36" s="28">
-        <f>COUNTIF(B2:B33,"=0")/32</f>
-        <v>0.75</v>
-      </c>
-      <c r="C36" s="28">
-        <f t="shared" ref="C36:E36" si="12">COUNTIF(C2:C33,"=0")/32</f>
-        <v>0.5625</v>
-      </c>
-      <c r="D36" s="28">
-        <f t="shared" si="12"/>
-        <v>0.5625</v>
-      </c>
-      <c r="E36" s="28">
-        <f t="shared" si="12"/>
-        <v>0.5625</v>
-      </c>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="28">
-        <f>COUNTIF(I2:I33,"=0")/32</f>
-        <v>0.28125</v>
-      </c>
-      <c r="J36" s="28">
-        <f t="shared" ref="J36:L36" si="13">COUNTIF(J2:J33,"=0")/32</f>
-        <v>0.1875</v>
-      </c>
-      <c r="K36" s="28">
-        <f t="shared" si="13"/>
-        <v>0.1875</v>
-      </c>
-      <c r="L36" s="28">
-        <f t="shared" si="13"/>
-        <v>0.15625</v>
-      </c>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
-      <c r="P36" s="21">
-        <f>AVERAGE(P2:P33)</f>
-        <v>0.56401212225610542</v>
-      </c>
-      <c r="Q36" s="21">
-        <f>AVERAGE(Q2:Q33)</f>
-        <v>0.37780814692940567</v>
-      </c>
-      <c r="R36" s="21">
-        <f>AVERAGE(R2:R33)</f>
-        <v>0.19429948525939358</v>
-      </c>
-      <c r="S36" s="28">
-        <f>COUNTIF(S2:S33,"=0")/32</f>
-        <v>0.9375</v>
-      </c>
-      <c r="T36" s="28">
-        <f t="shared" ref="T36:V36" si="14">COUNTIF(T2:T33,"=0")/32</f>
-        <v>0.65625</v>
-      </c>
-      <c r="U36" s="28">
+      <c r="B40" s="27">
+        <f>COUNTIF(B2:B37,"=0")/COUNTA(B2:B37)</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="C40" s="27">
+        <f t="shared" ref="C40:E40" si="14">COUNTIF(C2:C37,"=0")/COUNTA(C2:C37)</f>
+        <v>0.63888888888888884</v>
+      </c>
+      <c r="D40" s="27">
         <f t="shared" si="14"/>
-        <v>0.6875</v>
-      </c>
-      <c r="V36" s="28">
+        <v>0.63888888888888884</v>
+      </c>
+      <c r="E40" s="27">
         <f t="shared" si="14"/>
-        <v>0.65625</v>
-      </c>
-      <c r="W36" s="14"/>
-      <c r="X36" s="14"/>
-      <c r="Y36" s="14"/>
-      <c r="Z36" s="21">
-        <f>AVERAGE(Z2:Z33)</f>
-        <v>0.73516390450275815</v>
-      </c>
-      <c r="AA36" s="22">
-        <f>AVERAGE(AA2:AA33)</f>
-        <v>0.43630934606614125</v>
-      </c>
-      <c r="AB36" s="22">
-        <f>AVERAGE(AB2:AB33)</f>
-        <v>0.33205421123959522</v>
+        <v>0.63888888888888884</v>
+      </c>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="27">
+        <f>COUNTIF(I2:I37,"=0")/COUNTA(I2:I37)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J40" s="27">
+        <f t="shared" ref="J40:L40" si="15">COUNTIF(J2:J37,"=0")/COUNTA(J2:J37)</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="K40" s="27">
+        <f t="shared" si="15"/>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="L40" s="27">
+        <f t="shared" si="15"/>
+        <v>0.19444444444444445</v>
+      </c>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="20">
+        <f>AVERAGE(P2:P37)</f>
+        <v>0.77978605094473963</v>
+      </c>
+      <c r="Q40" s="20">
+        <f>AVERAGE(Q2:Q37)</f>
+        <v>0.47649532300259334</v>
+      </c>
+      <c r="R40" s="20" t="e">
+        <f>AVERAGE(R2:R37)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S40" s="27">
+        <f>COUNTIF(S2:S37,"=0")/COUNTA(S2:S37)</f>
+        <v>0.94444444444444442</v>
+      </c>
+      <c r="T40" s="27">
+        <f t="shared" ref="T40:V40" si="16">COUNTIF(T2:T37,"=0")/COUNTA(T2:T37)</f>
+        <v>0.69444444444444442</v>
+      </c>
+      <c r="U40" s="27">
+        <f t="shared" si="16"/>
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="V40" s="27">
+        <f t="shared" si="16"/>
+        <v>0.69444444444444442</v>
+      </c>
+      <c r="W40" s="14"/>
+      <c r="X40" s="14"/>
+      <c r="Y40" s="14"/>
+      <c r="Z40" s="20">
+        <f>AVERAGE(Z2:Z37)</f>
+        <v>0.96457064070957088</v>
+      </c>
+      <c r="AA40" s="21">
+        <f>AVERAGE(AA2:AA37)</f>
+        <v>0.53332270896785039</v>
+      </c>
+      <c r="AB40" s="21" t="e">
+        <f>AVERAGE(AB2:AB37)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="P2:R36 Z2:AB36">
-    <cfRule type="dataBar" priority="8">
+  <conditionalFormatting sqref="P2:R40 Z2:AB40">
+    <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4114,7 +4472,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:E5 I2:L5 S2:V5">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="4294967296"/>
+        <color rgb="FF99FF99"/>
+        <color rgb="FFFFFFCC"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:E8 B19:E20 B27:E27 I6:L8 I19:L20 I27:L27 S6:V8 S19:V20 S27:V27">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4125,20 +4495,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15:E16 B23:E23 I15:L16 I23:L23 S15:V16 S23:V23">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="1048576"/>
-        <color rgb="FF99FF99"/>
-        <color rgb="FFFFFFCC"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6:E14 I6:L14 S6:V14 B17:E22 I17:L22 S17:V22 I24:L33 S24:V33 B24:E33">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="B10:E18 I10:L18 S10:V18 B21:E26 I21:L26 S21:V26 I28:L37 S28:V37 B28:E37">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4149,8 +4507,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B34:E36 I34:L36 S34:V36">
-    <cfRule type="dataBar" priority="3">
+  <conditionalFormatting sqref="B38:E40 I38:L40 S38:V40">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4163,11 +4521,23 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B9:E9 I9:L9 S9:V9">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="16777216"/>
+        <color rgb="FF99FF99"/>
+        <color rgb="FFFFFFCC"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B34 S34:V34 S35:V36 B35:G36 C34:G34 I35:N36 I34:N34 P35:Q36 P34:Q34" formulaRange="1"/>
-    <ignoredError sqref="R2:R33 AB2:AB33" evalError="1"/>
+    <ignoredError sqref="B38 S38:V38 F40:G40 C38:G38 M40:N40 I38:N38 P40:Q40 P38:Q38 F39:G39 B39:E39 M39:N39 I39:L39 S39:V39" formulaRange="1"/>
+    <ignoredError sqref="R10:R37 AB10:AB37 AB2:AB5 R2:R5" evalError="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -4185,7 +4555,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>P2:R36 Z2:AB36</xm:sqref>
+          <xm:sqref>P2:R40 Z2:AB40</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{D4AEBDF6-16F3-4574-8AF5-06B7A23DFE16}">
@@ -4200,7 +4570,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>B34:E36 I34:L36 S34:V36</xm:sqref>
+          <xm:sqref>B38:E40 I38:L40 S38:V40</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Improved accuracy of asinh function.
git-svn-id: https://svn.code.sf.net/p/half/code/branches/clean@371 ba856b29-48f5-46b1-a3e5-b459205bce89
</commit_message>
<xml_diff>
--- a/test/results.xlsx
+++ b/test/results.xlsx
@@ -3562,19 +3562,19 @@
         <v>0</v>
       </c>
       <c r="C31" s="2">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="D31" s="2">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="E31" s="2">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="F31" s="2">
-        <v>11175</v>
+        <v>8572</v>
       </c>
       <c r="G31" s="2">
-        <v>10415</v>
+        <v>7993</v>
       </c>
       <c r="H31" s="2">
         <v>9052</v>
@@ -3592,21 +3592,21 @@
         <v>4490</v>
       </c>
       <c r="M31" s="2">
-        <v>4512</v>
+        <v>4500</v>
       </c>
       <c r="N31" s="2">
-        <v>3076</v>
+        <v>3138</v>
       </c>
       <c r="O31" s="1">
         <v>1850</v>
       </c>
       <c r="P31" s="8">
         <f t="shared" si="0"/>
-        <v>0.40375838926174495</v>
+        <v>0.52496500233317778</v>
       </c>
       <c r="Q31" s="8">
         <f t="shared" si="1"/>
-        <v>0.29534325492078733</v>
+        <v>0.39259351932941322</v>
       </c>
       <c r="R31" s="8">
         <f t="shared" si="2"/>
@@ -3625,21 +3625,21 @@
         <v>0</v>
       </c>
       <c r="W31" s="2">
-        <v>4160</v>
+        <v>4344</v>
       </c>
       <c r="X31" s="2">
-        <v>3411</v>
+        <v>3540</v>
       </c>
       <c r="Y31" s="1">
         <v>2186</v>
       </c>
       <c r="Z31" s="8">
         <f t="shared" si="3"/>
-        <v>0.37225950782997763</v>
+        <v>0.50676621558562762</v>
       </c>
       <c r="AA31" s="9">
         <f t="shared" si="4"/>
-        <v>0.32750840134421505</v>
+        <v>0.44288752658576253</v>
       </c>
       <c r="AB31" s="9">
         <f t="shared" si="5"/>
@@ -4294,15 +4294,15 @@
       </c>
       <c r="C39" s="26">
         <f t="shared" ref="C39:E39" si="9">COUNTIF(C6:C37,"=0")/COUNTA(C6:C37)</f>
-        <v>0.59375</v>
+        <v>0.625</v>
       </c>
       <c r="D39" s="26">
         <f t="shared" si="9"/>
-        <v>0.59375</v>
+        <v>0.625</v>
       </c>
       <c r="E39" s="26">
         <f t="shared" si="9"/>
-        <v>0.59375</v>
+        <v>0.625</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -4328,11 +4328,11 @@
       <c r="O39" s="2"/>
       <c r="P39" s="19">
         <f>AVERAGE(P6:P37)</f>
-        <v>0.77859844354192587</v>
+        <v>0.78238615020040814</v>
       </c>
       <c r="Q39" s="19">
         <f t="shared" ref="Q39:R39" si="11">AVERAGE(Q6:Q37)</f>
-        <v>0.44336826366001769</v>
+        <v>0.44640733442278724</v>
       </c>
       <c r="R39" s="19" t="e">
         <f t="shared" si="11"/>
@@ -4359,11 +4359,11 @@
       <c r="Y39" s="2"/>
       <c r="Z39" s="19">
         <f>AVERAGE(Z6:Z37)</f>
-        <v>0.91303070312240198</v>
+        <v>0.91723403773976608</v>
       </c>
       <c r="AA39" s="19">
         <f t="shared" ref="AA39:AB39" si="13">AVERAGE(AA6:AA37)</f>
-        <v>0.47911807937164141</v>
+        <v>0.48272367703543984</v>
       </c>
       <c r="AB39" s="19" t="e">
         <f t="shared" si="13"/>
@@ -4380,15 +4380,15 @@
       </c>
       <c r="C40" s="27">
         <f t="shared" ref="C40:E40" si="14">COUNTIF(C2:C37,"=0")/COUNTA(C2:C37)</f>
-        <v>0.63888888888888884</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D40" s="27">
         <f t="shared" si="14"/>
-        <v>0.63888888888888884</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="E40" s="27">
         <f t="shared" si="14"/>
-        <v>0.63888888888888884</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F40" s="14"/>
       <c r="G40" s="14"/>
@@ -4414,11 +4414,11 @@
       <c r="O40" s="14"/>
       <c r="P40" s="20">
         <f>AVERAGE(P2:P37)</f>
-        <v>0.77978605094473963</v>
+        <v>0.78315290130783499</v>
       </c>
       <c r="Q40" s="20">
         <f>AVERAGE(Q2:Q37)</f>
-        <v>0.47649532300259334</v>
+        <v>0.4791967192361663</v>
       </c>
       <c r="R40" s="20" t="e">
         <f>AVERAGE(R2:R37)</f>
@@ -4445,11 +4445,11 @@
       <c r="Y40" s="14"/>
       <c r="Z40" s="20">
         <f>AVERAGE(Z2:Z37)</f>
-        <v>0.96457064070957088</v>
+        <v>0.96830693814722779</v>
       </c>
       <c r="AA40" s="21">
         <f>AVERAGE(AA2:AA37)</f>
-        <v>0.53332270896785039</v>
+        <v>0.53652768466900458</v>
       </c>
       <c r="AB40" s="21" t="e">
         <f>AVERAGE(AB2:AB37)</f>

</xml_diff>

<commit_message>
Improved accuracy of atan function.
git-svn-id: https://svn.code.sf.net/p/half/code/branches/clean@372 ba856b29-48f5-46b1-a3e5-b459205bce89
</commit_message>
<xml_diff>
--- a/test/results.xlsx
+++ b/test/results.xlsx
@@ -1553,10 +1553,10 @@
         <v>0</v>
       </c>
       <c r="F9" s="2">
-        <v>16089</v>
+        <v>21492</v>
       </c>
       <c r="G9" s="2">
-        <v>13721</v>
+        <v>19652</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2">
@@ -1572,19 +1572,19 @@
         <v>429655</v>
       </c>
       <c r="M9" s="2">
-        <v>15363</v>
+        <v>15353</v>
       </c>
       <c r="N9" s="2">
-        <v>11652</v>
+        <v>11599</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="8">
         <f t="shared" si="0"/>
-        <v>0.95487600223755364</v>
+        <v>0.71435883119300203</v>
       </c>
       <c r="Q9" s="8">
         <f t="shared" si="1"/>
-        <v>0.84920924130894249</v>
+        <v>0.59021982495420311</v>
       </c>
       <c r="R9" s="8" t="e">
         <f t="shared" si="2"/>
@@ -1603,19 +1603,19 @@
         <v>0</v>
       </c>
       <c r="W9" s="2">
-        <v>26370</v>
+        <v>28087</v>
       </c>
       <c r="X9" s="2">
-        <v>13030</v>
+        <v>13725</v>
       </c>
       <c r="Y9" s="1"/>
       <c r="Z9" s="8">
         <f t="shared" si="3"/>
-        <v>1.6390080179004289</v>
+        <v>1.3068583659035919</v>
       </c>
       <c r="AA9" s="9">
         <f t="shared" si="4"/>
-        <v>0.94963923912251291</v>
+        <v>0.69840219824954208</v>
       </c>
       <c r="AB9" s="9" t="e">
         <f t="shared" si="5"/>
@@ -3102,19 +3102,19 @@
         <v>0</v>
       </c>
       <c r="C26" s="2">
-        <v>720</v>
+        <v>0</v>
       </c>
       <c r="D26" s="2">
-        <v>720</v>
+        <v>0</v>
       </c>
       <c r="E26" s="2">
-        <v>720</v>
+        <v>0</v>
       </c>
       <c r="F26" s="2">
-        <v>5624</v>
+        <v>3931</v>
       </c>
       <c r="G26" s="2">
-        <v>5243</v>
+        <v>3663</v>
       </c>
       <c r="H26" s="2">
         <v>3724</v>
@@ -3132,21 +3132,21 @@
         <v>3525</v>
       </c>
       <c r="M26" s="2">
-        <v>2195</v>
+        <v>2297</v>
       </c>
       <c r="N26" s="2">
-        <v>1726</v>
+        <v>1782</v>
       </c>
       <c r="O26" s="1">
         <v>843</v>
       </c>
       <c r="P26" s="8">
         <f t="shared" si="0"/>
-        <v>0.39029160739687058</v>
+        <v>0.58432968710251842</v>
       </c>
       <c r="Q26" s="8">
         <f t="shared" si="1"/>
-        <v>0.32920083921419035</v>
+        <v>0.48648648648648651</v>
       </c>
       <c r="R26" s="8">
         <f t="shared" si="2"/>
@@ -3165,21 +3165,21 @@
         <v>0</v>
       </c>
       <c r="W26" s="2">
-        <v>2694</v>
+        <v>2795</v>
       </c>
       <c r="X26" s="2">
-        <v>1949</v>
+        <v>2041</v>
       </c>
       <c r="Y26" s="1">
         <v>1271</v>
       </c>
       <c r="Z26" s="8">
         <f t="shared" si="3"/>
-        <v>0.47901849217638692</v>
+        <v>0.71101500890358682</v>
       </c>
       <c r="AA26" s="9">
         <f t="shared" si="4"/>
-        <v>0.371733740225062</v>
+        <v>0.55719355719355723</v>
       </c>
       <c r="AB26" s="9">
         <f t="shared" si="5"/>
@@ -3576,7 +3576,7 @@
       <c r="G31" s="2">
         <v>7993</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H31" s="28">
         <v>9052</v>
       </c>
       <c r="I31" s="2">
@@ -4294,15 +4294,15 @@
       </c>
       <c r="C39" s="26">
         <f t="shared" ref="C39:E39" si="9">COUNTIF(C6:C37,"=0")/COUNTA(C6:C37)</f>
-        <v>0.625</v>
+        <v>0.65625</v>
       </c>
       <c r="D39" s="26">
         <f t="shared" si="9"/>
-        <v>0.625</v>
+        <v>0.65625</v>
       </c>
       <c r="E39" s="26">
         <f t="shared" si="9"/>
-        <v>0.625</v>
+        <v>0.65625</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -4328,11 +4328,11 @@
       <c r="O39" s="2"/>
       <c r="P39" s="19">
         <f>AVERAGE(P6:P37)</f>
-        <v>0.78238615020040814</v>
+        <v>0.78093367859606733</v>
       </c>
       <c r="Q39" s="19">
         <f t="shared" ref="Q39:R39" si="11">AVERAGE(Q6:Q37)</f>
-        <v>0.44640733442278724</v>
+        <v>0.4432290916389609</v>
       </c>
       <c r="R39" s="19" t="e">
         <f t="shared" si="11"/>
@@ -4359,11 +4359,11 @@
       <c r="Y39" s="2"/>
       <c r="Z39" s="19">
         <f>AVERAGE(Z6:Z37)</f>
-        <v>0.91723403773976608</v>
+        <v>0.91410425226258996</v>
       </c>
       <c r="AA39" s="19">
         <f t="shared" ref="AA39:AB39" si="13">AVERAGE(AA6:AA37)</f>
-        <v>0.48272367703543984</v>
+        <v>0.48066813878842485</v>
       </c>
       <c r="AB39" s="19" t="e">
         <f t="shared" si="13"/>
@@ -4380,15 +4380,15 @@
       </c>
       <c r="C40" s="27">
         <f t="shared" ref="C40:E40" si="14">COUNTIF(C2:C37,"=0")/COUNTA(C2:C37)</f>
-        <v>0.66666666666666663</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="D40" s="27">
         <f t="shared" si="14"/>
-        <v>0.66666666666666663</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="E40" s="27">
         <f t="shared" si="14"/>
-        <v>0.66666666666666663</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="F40" s="14"/>
       <c r="G40" s="14"/>
@@ -4414,11 +4414,11 @@
       <c r="O40" s="14"/>
       <c r="P40" s="20">
         <f>AVERAGE(P2:P37)</f>
-        <v>0.78315290130783499</v>
+        <v>0.78186181543730982</v>
       </c>
       <c r="Q40" s="20">
         <f>AVERAGE(Q2:Q37)</f>
-        <v>0.4791967192361663</v>
+        <v>0.47637161453943172</v>
       </c>
       <c r="R40" s="20" t="e">
         <f>AVERAGE(R2:R37)</f>
@@ -4445,11 +4445,11 @@
       <c r="Y40" s="14"/>
       <c r="Z40" s="20">
         <f>AVERAGE(Z2:Z37)</f>
-        <v>0.96830693814722779</v>
+        <v>0.96552490661196011</v>
       </c>
       <c r="AA40" s="21">
         <f>AVERAGE(AA2:AA37)</f>
-        <v>0.53652768466900458</v>
+        <v>0.53470053956054686</v>
       </c>
       <c r="AB40" s="21" t="e">
         <f>AVERAGE(AB2:AB37)</f>

</xml_diff>

<commit_message>
Improved accuracy of sin function.
git-svn-id: https://svn.code.sf.net/p/half/code/branches/clean@373 ba856b29-48f5-46b1-a3e5-b459205bce89
</commit_message>
<xml_diff>
--- a/test/results.xlsx
+++ b/test/results.xlsx
@@ -2642,21 +2642,21 @@
         <v>0</v>
       </c>
       <c r="C21" s="2">
-        <v>3596</v>
+        <v>0</v>
       </c>
       <c r="D21" s="2">
-        <v>2694</v>
+        <v>0</v>
       </c>
       <c r="E21" s="2">
-        <v>2694</v>
+        <v>0</v>
       </c>
       <c r="F21" s="2">
-        <v>6442</v>
+        <v>6032</v>
       </c>
       <c r="G21" s="2">
-        <v>5963</v>
-      </c>
-      <c r="H21" s="2">
+        <v>4258</v>
+      </c>
+      <c r="H21" s="28">
         <v>4184</v>
       </c>
       <c r="I21" s="2">
@@ -2672,21 +2672,21 @@
         <v>4062</v>
       </c>
       <c r="M21" s="2">
-        <v>1721</v>
+        <v>1790</v>
       </c>
       <c r="N21" s="2">
-        <v>1793</v>
+        <v>1846</v>
       </c>
       <c r="O21" s="1">
         <v>839</v>
       </c>
       <c r="P21" s="8">
         <f t="shared" si="0"/>
-        <v>0.26715305805650419</v>
+        <v>0.2967506631299735</v>
       </c>
       <c r="Q21" s="8">
         <f t="shared" si="1"/>
-        <v>0.30068757336910951</v>
+        <v>0.43353687177078443</v>
       </c>
       <c r="R21" s="8">
         <f t="shared" si="2"/>
@@ -2705,21 +2705,21 @@
         <v>0</v>
       </c>
       <c r="W21" s="2">
-        <v>2199</v>
+        <v>2270</v>
       </c>
       <c r="X21" s="2">
-        <v>1625</v>
+        <v>1706</v>
       </c>
       <c r="Y21" s="1">
         <v>1062</v>
       </c>
       <c r="Z21" s="8">
         <f t="shared" si="3"/>
-        <v>0.34135361688916488</v>
+        <v>0.37632625994694963</v>
       </c>
       <c r="AA21" s="9">
         <f t="shared" si="4"/>
-        <v>0.27251383531779305</v>
+        <v>0.40065758572099575</v>
       </c>
       <c r="AB21" s="9">
         <f t="shared" si="5"/>
@@ -3116,7 +3116,7 @@
       <c r="G26" s="2">
         <v>3663</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="28">
         <v>3724</v>
       </c>
       <c r="I26" s="2">
@@ -4294,15 +4294,15 @@
       </c>
       <c r="C39" s="26">
         <f t="shared" ref="C39:E39" si="9">COUNTIF(C6:C37,"=0")/COUNTA(C6:C37)</f>
-        <v>0.65625</v>
+        <v>0.6875</v>
       </c>
       <c r="D39" s="26">
         <f t="shared" si="9"/>
-        <v>0.65625</v>
+        <v>0.6875</v>
       </c>
       <c r="E39" s="26">
         <f t="shared" si="9"/>
-        <v>0.65625</v>
+        <v>0.6875</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -4328,11 +4328,11 @@
       <c r="O39" s="2"/>
       <c r="P39" s="19">
         <f>AVERAGE(P6:P37)</f>
-        <v>0.78093367859606733</v>
+        <v>0.78185860375461325</v>
       </c>
       <c r="Q39" s="19">
         <f t="shared" ref="Q39:R39" si="11">AVERAGE(Q6:Q37)</f>
-        <v>0.4432290916389609</v>
+        <v>0.4473806322140132</v>
       </c>
       <c r="R39" s="19" t="e">
         <f t="shared" si="11"/>
@@ -4359,11 +4359,11 @@
       <c r="Y39" s="2"/>
       <c r="Z39" s="19">
         <f>AVERAGE(Z6:Z37)</f>
-        <v>0.91410425226258996</v>
+        <v>0.91519714735814572</v>
       </c>
       <c r="AA39" s="19">
         <f t="shared" ref="AA39:AB39" si="13">AVERAGE(AA6:AA37)</f>
-        <v>0.48066813878842485</v>
+        <v>0.48467263098852498</v>
       </c>
       <c r="AB39" s="19" t="e">
         <f t="shared" si="13"/>
@@ -4380,15 +4380,15 @@
       </c>
       <c r="C40" s="27">
         <f t="shared" ref="C40:E40" si="14">COUNTIF(C2:C37,"=0")/COUNTA(C2:C37)</f>
-        <v>0.69444444444444442</v>
+        <v>0.72222222222222221</v>
       </c>
       <c r="D40" s="27">
         <f t="shared" si="14"/>
-        <v>0.69444444444444442</v>
+        <v>0.72222222222222221</v>
       </c>
       <c r="E40" s="27">
         <f t="shared" si="14"/>
-        <v>0.69444444444444442</v>
+        <v>0.72222222222222221</v>
       </c>
       <c r="F40" s="14"/>
       <c r="G40" s="14"/>
@@ -4414,11 +4414,11 @@
       <c r="O40" s="14"/>
       <c r="P40" s="20">
         <f>AVERAGE(P2:P37)</f>
-        <v>0.78186181543730982</v>
+        <v>0.78268397113379506</v>
       </c>
       <c r="Q40" s="20">
         <f>AVERAGE(Q2:Q37)</f>
-        <v>0.47637161453943172</v>
+        <v>0.4800618728283671</v>
       </c>
       <c r="R40" s="20" t="e">
         <f>AVERAGE(R2:R37)</f>
@@ -4445,11 +4445,11 @@
       <c r="Y40" s="14"/>
       <c r="Z40" s="20">
         <f>AVERAGE(Z2:Z37)</f>
-        <v>0.96552490661196011</v>
+        <v>0.96649636891912083</v>
       </c>
       <c r="AA40" s="21">
         <f>AVERAGE(AA2:AA37)</f>
-        <v>0.53470053956054686</v>
+        <v>0.53826008818285809</v>
       </c>
       <c r="AB40" s="21" t="e">
         <f>AVERAGE(AB2:AB37)</f>

</xml_diff>

<commit_message>
Improved accuracy of cos and tan functions.
git-svn-id: https://svn.code.sf.net/p/half/code/branches/clean@374 ba856b29-48f5-46b1-a3e5-b459205bce89
</commit_message>
<xml_diff>
--- a/test/results.xlsx
+++ b/test/results.xlsx
@@ -2734,19 +2734,19 @@
         <v>0</v>
       </c>
       <c r="C22" s="2">
-        <v>434</v>
+        <v>0</v>
       </c>
       <c r="D22" s="2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E22" s="2">
-        <v>434</v>
+        <v>0</v>
       </c>
       <c r="F22" s="2">
-        <v>6053</v>
+        <v>4918</v>
       </c>
       <c r="G22" s="2">
-        <v>6036</v>
+        <v>4441</v>
       </c>
       <c r="H22" s="2">
         <v>3943</v>
@@ -2764,21 +2764,21 @@
         <v>6154</v>
       </c>
       <c r="M22" s="2">
-        <v>1734</v>
+        <v>1803</v>
       </c>
       <c r="N22" s="2">
-        <v>1618</v>
+        <v>1668</v>
       </c>
       <c r="O22" s="1">
         <v>804</v>
       </c>
       <c r="P22" s="8">
         <f t="shared" si="0"/>
-        <v>0.28646951924665454</v>
+        <v>0.36661244408296056</v>
       </c>
       <c r="Q22" s="8">
         <f t="shared" si="1"/>
-        <v>0.26805831676607023</v>
+        <v>0.37559108308939426</v>
       </c>
       <c r="R22" s="8">
         <f t="shared" si="2"/>
@@ -2797,21 +2797,21 @@
         <v>0</v>
       </c>
       <c r="W22" s="2">
-        <v>2185</v>
+        <v>2265</v>
       </c>
       <c r="X22" s="2">
-        <v>1612</v>
+        <v>1679</v>
       </c>
       <c r="Y22" s="1">
         <v>1050</v>
       </c>
       <c r="Z22" s="8">
         <f t="shared" si="3"/>
-        <v>0.36097802742441765</v>
+        <v>0.46055307035380239</v>
       </c>
       <c r="AA22" s="9">
         <f t="shared" si="4"/>
-        <v>0.267064280980782</v>
+        <v>0.37806800270209412</v>
       </c>
       <c r="AB22" s="9">
         <f t="shared" si="5"/>
@@ -2826,19 +2826,19 @@
         <v>0</v>
       </c>
       <c r="C23" s="2">
-        <v>3356</v>
+        <v>0</v>
       </c>
       <c r="D23" s="2">
-        <v>3356</v>
+        <v>0</v>
       </c>
       <c r="E23" s="2">
-        <v>3356</v>
+        <v>0</v>
       </c>
       <c r="F23" s="2">
-        <v>8209</v>
+        <v>6137</v>
       </c>
       <c r="G23" s="2">
-        <v>7661</v>
+        <v>5354</v>
       </c>
       <c r="H23" s="2">
         <v>5109</v>
@@ -2856,21 +2856,21 @@
         <v>3525</v>
       </c>
       <c r="M23" s="2">
-        <v>2271</v>
+        <v>2358</v>
       </c>
       <c r="N23" s="2">
-        <v>1638</v>
+        <v>1673</v>
       </c>
       <c r="O23" s="1">
         <v>719</v>
       </c>
       <c r="P23" s="8">
         <f t="shared" si="0"/>
-        <v>0.27664758192228045</v>
+        <v>0.38422682092227473</v>
       </c>
       <c r="Q23" s="8">
         <f t="shared" si="1"/>
-        <v>0.21381020754470695</v>
+        <v>0.31247665296974225</v>
       </c>
       <c r="R23" s="8">
         <f t="shared" si="2"/>
@@ -2889,21 +2889,21 @@
         <v>0</v>
       </c>
       <c r="W23" s="2">
-        <v>2792</v>
+        <v>2886</v>
       </c>
       <c r="X23" s="2">
-        <v>2181</v>
+        <v>2224</v>
       </c>
       <c r="Y23" s="1">
         <v>1164</v>
       </c>
       <c r="Z23" s="8">
         <f t="shared" si="3"/>
-        <v>0.34011450846631747</v>
+        <v>0.47026234316441257</v>
       </c>
       <c r="AA23" s="9">
         <f t="shared" si="4"/>
-        <v>0.28468868293956401</v>
+        <v>0.41539036234590959</v>
       </c>
       <c r="AB23" s="9">
         <f t="shared" si="5"/>
@@ -4294,15 +4294,15 @@
       </c>
       <c r="C39" s="26">
         <f t="shared" ref="C39:E39" si="9">COUNTIF(C6:C37,"=0")/COUNTA(C6:C37)</f>
-        <v>0.6875</v>
+        <v>0.75</v>
       </c>
       <c r="D39" s="26">
         <f t="shared" si="9"/>
-        <v>0.6875</v>
+        <v>0.75</v>
       </c>
       <c r="E39" s="26">
         <f t="shared" si="9"/>
-        <v>0.6875</v>
+        <v>0.75</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -4328,11 +4328,11 @@
       <c r="O39" s="2"/>
       <c r="P39" s="19">
         <f>AVERAGE(P6:P37)</f>
-        <v>0.78185860375461325</v>
+        <v>0.78772492137449757</v>
       </c>
       <c r="Q39" s="19">
         <f t="shared" ref="Q39:R39" si="11">AVERAGE(Q6:Q37)</f>
-        <v>0.4473806322140132</v>
+        <v>0.45382435758114942</v>
       </c>
       <c r="R39" s="19" t="e">
         <f t="shared" si="11"/>
@@ -4359,11 +4359,11 @@
       <c r="Y39" s="2"/>
       <c r="Z39" s="19">
         <f>AVERAGE(Z6:Z37)</f>
-        <v>0.91519714735814572</v>
+        <v>0.92237598728400461</v>
       </c>
       <c r="AA39" s="19">
         <f t="shared" ref="AA39:AB39" si="13">AVERAGE(AA6:AA37)</f>
-        <v>0.48467263098852498</v>
+        <v>0.49222592477376426</v>
       </c>
       <c r="AB39" s="19" t="e">
         <f t="shared" si="13"/>
@@ -4380,15 +4380,15 @@
       </c>
       <c r="C40" s="27">
         <f t="shared" ref="C40:E40" si="14">COUNTIF(C2:C37,"=0")/COUNTA(C2:C37)</f>
-        <v>0.72222222222222221</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="D40" s="27">
         <f t="shared" si="14"/>
-        <v>0.72222222222222221</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="E40" s="27">
         <f t="shared" si="14"/>
-        <v>0.72222222222222221</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="F40" s="14"/>
       <c r="G40" s="14"/>
@@ -4414,11 +4414,11 @@
       <c r="O40" s="14"/>
       <c r="P40" s="20">
         <f>AVERAGE(P2:P37)</f>
-        <v>0.78268397113379506</v>
+        <v>0.78789847568480342</v>
       </c>
       <c r="Q40" s="20">
         <f>AVERAGE(Q2:Q37)</f>
-        <v>0.4800618728283671</v>
+        <v>0.48578962871026593</v>
       </c>
       <c r="R40" s="20" t="e">
         <f>AVERAGE(R2:R37)</f>
@@ -4445,11 +4445,11 @@
       <c r="Y40" s="14"/>
       <c r="Z40" s="20">
         <f>AVERAGE(Z2:Z37)</f>
-        <v>0.96649636891912083</v>
+        <v>0.97287755996432879</v>
       </c>
       <c r="AA40" s="21">
         <f>AVERAGE(AA2:AA37)</f>
-        <v>0.53826008818285809</v>
+        <v>0.5449741271030708</v>
       </c>
       <c r="AB40" s="21" t="e">
         <f>AVERAGE(AB2:AB37)</f>

</xml_diff>

<commit_message>
Improved accuracy of sincos function.
git-svn-id: https://svn.code.sf.net/p/half/code/branches/clean@375 ba856b29-48f5-46b1-a3e5-b459205bce89
</commit_message>
<xml_diff>
--- a/test/results.xlsx
+++ b/test/results.xlsx
@@ -2748,7 +2748,7 @@
       <c r="G22" s="2">
         <v>4441</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="28">
         <v>3943</v>
       </c>
       <c r="I22" s="2">
@@ -2840,7 +2840,7 @@
       <c r="G23" s="2">
         <v>5354</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="28">
         <v>5109</v>
       </c>
       <c r="I23" s="2">

</xml_diff>

<commit_message>
Improved performance of conversion functions.
git-svn-id: https://svn.code.sf.net/p/half/code/branches/clean@377 ba856b29-48f5-46b1-a3e5-b459205bce89
</commit_message>
<xml_diff>
--- a/test/results.xlsx
+++ b/test/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Nh</t>
   </si>
@@ -202,12 +202,6 @@
   </si>
   <si>
     <t>F16Cd%</t>
-  </si>
-  <si>
-    <t>fmod</t>
-  </si>
-  <si>
-    <t>remainder</t>
   </si>
   <si>
     <t>fma</t>
@@ -223,7 +217,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,25 +240,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="16">
@@ -463,12 +445,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -497,10 +478,10 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="2" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -815,7 +796,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB40"/>
+  <dimension ref="A1:AC38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -927,13 +908,13 @@
         <v>0</v>
       </c>
       <c r="F2" s="1">
-        <v>5574</v>
+        <v>5328</v>
       </c>
       <c r="G2" s="1">
-        <v>4044</v>
+        <v>4017</v>
       </c>
       <c r="H2" s="1">
-        <v>3655</v>
+        <v>3762</v>
       </c>
       <c r="I2" s="1">
         <v>0</v>
@@ -948,25 +929,25 @@
         <v>92258304</v>
       </c>
       <c r="M2" s="1">
-        <v>3315</v>
+        <v>2455</v>
       </c>
       <c r="N2" s="1">
-        <v>2309</v>
+        <v>1995</v>
       </c>
       <c r="O2" s="1">
-        <v>365</v>
+        <v>378</v>
       </c>
       <c r="P2" s="8">
         <f>M2/F2</f>
-        <v>0.59472551130247575</v>
+        <v>0.46077327327327328</v>
       </c>
       <c r="Q2" s="8">
         <f>N2/G2</f>
-        <v>0.57096933728981203</v>
+        <v>0.49663928304705002</v>
       </c>
       <c r="R2" s="8">
         <f>O2/H2</f>
-        <v>9.9863201094391243E-2</v>
+        <v>0.10047846889952153</v>
       </c>
       <c r="S2" s="1">
         <v>0</v>
@@ -981,25 +962,25 @@
         <v>0</v>
       </c>
       <c r="W2" s="1">
-        <v>5218</v>
+        <v>4506</v>
       </c>
       <c r="X2" s="1">
-        <v>2704</v>
+        <v>2442</v>
       </c>
       <c r="Y2" s="1">
-        <v>1306</v>
+        <v>1147</v>
       </c>
       <c r="Z2" s="8">
         <f>W2/F2</f>
-        <v>0.93613204162181562</v>
+        <v>0.84572072072072069</v>
       </c>
       <c r="AA2" s="9">
         <f>X2/G2</f>
-        <v>0.66864490603363003</v>
+        <v>0.607916355489171</v>
       </c>
       <c r="AB2" s="9">
         <f>Y2/H2</f>
-        <v>0.35731874145006842</v>
+        <v>0.30489101541733121</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -1019,13 +1000,13 @@
         <v>0</v>
       </c>
       <c r="F3" s="2">
-        <v>6899</v>
+        <v>6713</v>
       </c>
       <c r="G3" s="2">
-        <v>4077</v>
+        <v>4068</v>
       </c>
       <c r="H3" s="2">
-        <v>3701</v>
+        <v>3791</v>
       </c>
       <c r="I3" s="2">
         <v>0</v>
@@ -1040,25 +1021,25 @@
         <v>92258304</v>
       </c>
       <c r="M3" s="2">
-        <v>3345</v>
+        <v>2454</v>
       </c>
       <c r="N3" s="2">
-        <v>2294</v>
+        <v>2004</v>
       </c>
       <c r="O3" s="1">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="P3" s="8">
-        <f t="shared" ref="P3:P37" si="0">M3/F3</f>
-        <v>0.48485287722858383</v>
+        <f t="shared" ref="P3:P35" si="0">M3/F3</f>
+        <v>0.36555936243110382</v>
       </c>
       <c r="Q3" s="8">
-        <f t="shared" ref="Q3:Q37" si="1">N3/G3</f>
-        <v>0.56266862889379443</v>
+        <f t="shared" ref="Q3:Q35" si="1">N3/G3</f>
+        <v>0.49262536873156343</v>
       </c>
       <c r="R3" s="8">
-        <f t="shared" ref="R3:R37" si="2">O3/H3</f>
-        <v>9.8081599567684405E-2</v>
+        <f t="shared" ref="R3:R35" si="2">O3/H3</f>
+        <v>9.9182273806383545E-2</v>
       </c>
       <c r="S3" s="2">
         <v>0</v>
@@ -1073,25 +1054,25 @@
         <v>0</v>
       </c>
       <c r="W3" s="2">
-        <v>6202</v>
+        <v>5494</v>
       </c>
       <c r="X3" s="2">
-        <v>2649</v>
+        <v>2431</v>
       </c>
       <c r="Y3" s="1">
-        <v>1309</v>
+        <v>1144</v>
       </c>
       <c r="Z3" s="8">
-        <f t="shared" ref="Z3:Z37" si="3">W3/F3</f>
-        <v>0.89897086534280335</v>
+        <f t="shared" ref="Z3:Z35" si="3">W3/F3</f>
+        <v>0.81841203634738569</v>
       </c>
       <c r="AA3" s="9">
-        <f t="shared" ref="AA3:AA37" si="4">X3/G3</f>
-        <v>0.64974245768947758</v>
+        <f t="shared" ref="AA3:AA35" si="4">X3/G3</f>
+        <v>0.59759095378564409</v>
       </c>
       <c r="AB3" s="9">
-        <f t="shared" ref="AB3:AB37" si="5">Y3/H3</f>
-        <v>0.35368819238043769</v>
+        <f t="shared" ref="AB3:AB35" si="5">Y3/H3</f>
+        <v>0.30176734370878394</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -1111,13 +1092,13 @@
         <v>0</v>
       </c>
       <c r="F4" s="2">
-        <v>3112</v>
+        <v>3127</v>
       </c>
       <c r="G4" s="2">
-        <v>2417</v>
+        <v>2427</v>
       </c>
       <c r="H4" s="2">
-        <v>1761</v>
+        <v>1820</v>
       </c>
       <c r="I4" s="2">
         <v>0</v>
@@ -1132,25 +1113,25 @@
         <v>0</v>
       </c>
       <c r="M4" s="2">
-        <v>3381</v>
+        <v>3173</v>
       </c>
       <c r="N4" s="2">
-        <v>2358</v>
+        <v>2697</v>
       </c>
       <c r="O4" s="1">
-        <v>368</v>
+        <v>376</v>
       </c>
       <c r="P4" s="8">
         <f t="shared" si="0"/>
-        <v>1.086439588688946</v>
+        <v>1.0147105852254557</v>
       </c>
       <c r="Q4" s="8">
         <f t="shared" si="1"/>
-        <v>0.9755895738518825</v>
+        <v>1.1112484548825712</v>
       </c>
       <c r="R4" s="8">
         <f t="shared" si="2"/>
-        <v>0.20897217490062464</v>
+        <v>0.20659340659340658</v>
       </c>
       <c r="S4" s="2">
         <v>0</v>
@@ -1165,25 +1146,25 @@
         <v>0</v>
       </c>
       <c r="W4" s="2">
-        <v>5458</v>
+        <v>5197</v>
       </c>
       <c r="X4" s="2">
-        <v>3256</v>
+        <v>3037</v>
       </c>
       <c r="Y4" s="1">
-        <v>1925</v>
+        <v>1775</v>
       </c>
       <c r="Z4" s="8">
         <f t="shared" si="3"/>
-        <v>1.7538560411311055</v>
+        <v>1.6619763351455068</v>
       </c>
       <c r="AA4" s="9">
         <f t="shared" si="4"/>
-        <v>1.3471245345469591</v>
+        <v>1.2513391017717346</v>
       </c>
       <c r="AB4" s="9">
         <f t="shared" si="5"/>
-        <v>1.0931289040318002</v>
+        <v>0.97527472527472525</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -1203,13 +1184,13 @@
         <v>0</v>
       </c>
       <c r="F5" s="2">
-        <v>3833</v>
+        <v>3862</v>
       </c>
       <c r="G5" s="2">
-        <v>3094</v>
+        <v>2902</v>
       </c>
       <c r="H5" s="2">
-        <v>2033</v>
+        <v>2104</v>
       </c>
       <c r="I5" s="2">
         <v>0</v>
@@ -1224,25 +1205,25 @@
         <v>0</v>
       </c>
       <c r="M5" s="2">
-        <v>3799</v>
+        <v>3534</v>
       </c>
       <c r="N5" s="2">
-        <v>2651</v>
+        <v>3028</v>
       </c>
       <c r="O5" s="1">
         <v>377</v>
       </c>
       <c r="P5" s="8">
         <f t="shared" si="0"/>
-        <v>0.99112966344899556</v>
+        <v>0.91506991196271359</v>
       </c>
       <c r="Q5" s="8">
         <f t="shared" si="1"/>
-        <v>0.85681965093729795</v>
+        <v>1.0434183321847001</v>
       </c>
       <c r="R5" s="8">
         <f t="shared" si="2"/>
-        <v>0.1854402361042794</v>
+        <v>0.17918250950570341</v>
       </c>
       <c r="S5" s="2">
         <v>0</v>
@@ -1257,30 +1238,30 @@
         <v>0</v>
       </c>
       <c r="W5" s="2">
-        <v>7354</v>
+        <v>7310</v>
       </c>
       <c r="X5" s="2">
-        <v>3720</v>
+        <v>3528</v>
       </c>
       <c r="Y5" s="1">
-        <v>2224</v>
+        <v>2056</v>
       </c>
       <c r="Z5" s="8">
         <f t="shared" si="3"/>
-        <v>1.9186016175319593</v>
+        <v>1.8928016571724495</v>
       </c>
       <c r="AA5" s="9">
         <f t="shared" si="4"/>
-        <v>1.2023270846800258</v>
+        <v>1.2157133011716057</v>
       </c>
       <c r="AB5" s="9">
         <f t="shared" si="5"/>
-        <v>1.0939498278406297</v>
+        <v>0.97718631178707227</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -1295,42 +1276,46 @@
         <v>0</v>
       </c>
       <c r="F6" s="2">
-        <v>1222</v>
+        <v>1151</v>
       </c>
       <c r="G6" s="2">
-        <v>1179</v>
-      </c>
-      <c r="H6" s="2"/>
+        <v>763</v>
+      </c>
+      <c r="H6" s="2">
+        <v>596</v>
+      </c>
       <c r="I6" s="2">
         <v>0</v>
       </c>
       <c r="J6" s="2">
-        <v>0</v>
+        <v>11280</v>
       </c>
       <c r="K6" s="2">
-        <v>0</v>
+        <v>11348</v>
       </c>
       <c r="L6" s="2">
-        <v>0</v>
+        <v>11280</v>
       </c>
       <c r="M6" s="2">
-        <v>2808</v>
+        <v>720</v>
       </c>
       <c r="N6" s="2">
-        <v>1568</v>
-      </c>
-      <c r="O6" s="1"/>
+        <v>574</v>
+      </c>
+      <c r="O6" s="1">
+        <v>493</v>
+      </c>
       <c r="P6" s="8">
         <f t="shared" si="0"/>
-        <v>2.2978723404255321</v>
+        <v>0.62554300608166813</v>
       </c>
       <c r="Q6" s="8">
         <f t="shared" si="1"/>
-        <v>1.3299406276505512</v>
-      </c>
-      <c r="R6" s="8" t="e">
+        <v>0.75229357798165142</v>
+      </c>
+      <c r="R6" s="8">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0.82718120805369133</v>
       </c>
       <c r="S6" s="2">
         <v>0</v>
@@ -1345,28 +1330,30 @@
         <v>0</v>
       </c>
       <c r="W6" s="2">
-        <v>2906</v>
+        <v>1447</v>
       </c>
       <c r="X6" s="2">
-        <v>1728</v>
-      </c>
-      <c r="Y6" s="1"/>
+        <v>647</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>642</v>
+      </c>
       <c r="Z6" s="8">
         <f t="shared" si="3"/>
-        <v>2.3780687397708675</v>
+        <v>1.2571676802780192</v>
       </c>
       <c r="AA6" s="9">
         <f t="shared" si="4"/>
-        <v>1.4656488549618321</v>
-      </c>
-      <c r="AB6" s="9" t="e">
+        <v>0.84796854521625165</v>
+      </c>
+      <c r="AB6" s="9">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>1.0771812080536913</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
@@ -1381,42 +1368,46 @@
         <v>0</v>
       </c>
       <c r="F7" s="2">
-        <v>1573</v>
+        <v>20775</v>
       </c>
       <c r="G7" s="2">
-        <v>1545</v>
-      </c>
-      <c r="H7" s="2"/>
+        <v>18203</v>
+      </c>
+      <c r="H7" s="2">
+        <v>14420</v>
+      </c>
       <c r="I7" s="2">
-        <v>0</v>
+        <v>666</v>
       </c>
       <c r="J7" s="2">
-        <v>0</v>
+        <v>430069</v>
       </c>
       <c r="K7" s="2">
-        <v>0</v>
+        <v>430212</v>
       </c>
       <c r="L7" s="2">
-        <v>0</v>
+        <v>429655</v>
       </c>
       <c r="M7" s="2">
-        <v>7990</v>
+        <v>11284</v>
       </c>
       <c r="N7" s="2">
-        <v>2042</v>
-      </c>
-      <c r="O7" s="1"/>
+        <v>9027</v>
+      </c>
+      <c r="O7" s="1">
+        <v>1964</v>
+      </c>
       <c r="P7" s="8">
         <f t="shared" si="0"/>
-        <v>5.0794659885568976</v>
+        <v>0.54315282791817088</v>
       </c>
       <c r="Q7" s="8">
         <f t="shared" si="1"/>
-        <v>1.3216828478964402</v>
-      </c>
-      <c r="R7" s="8" t="e">
+        <v>0.49590726803274188</v>
+      </c>
+      <c r="R7" s="8">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0.13619972260748961</v>
       </c>
       <c r="S7" s="2">
         <v>0</v>
@@ -1431,28 +1422,30 @@
         <v>0</v>
       </c>
       <c r="W7" s="2">
-        <v>8010</v>
+        <v>25794</v>
       </c>
       <c r="X7" s="2">
-        <v>2038</v>
-      </c>
-      <c r="Y7" s="1"/>
+        <v>12398</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>5347</v>
+      </c>
       <c r="Z7" s="8">
         <f t="shared" si="3"/>
-        <v>5.0921805467260013</v>
+        <v>1.2415884476534296</v>
       </c>
       <c r="AA7" s="9">
         <f t="shared" si="4"/>
-        <v>1.3190938511326862</v>
-      </c>
-      <c r="AB7" s="9" t="e">
+        <v>0.68109652255122777</v>
+      </c>
+      <c r="AB7" s="9">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.37080443828016646</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="B8" s="2">
         <v>0</v>
@@ -1467,78 +1460,84 @@
         <v>0</v>
       </c>
       <c r="F8" s="2">
-        <v>1253</v>
+        <v>6085</v>
       </c>
       <c r="G8" s="2">
-        <v>830</v>
-      </c>
-      <c r="H8" s="2"/>
+        <v>5622</v>
+      </c>
+      <c r="H8" s="2">
+        <v>5253</v>
+      </c>
       <c r="I8" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J8" s="2">
-        <v>11280</v>
+        <v>9848</v>
       </c>
       <c r="K8" s="2">
-        <v>11348</v>
+        <v>9602</v>
       </c>
       <c r="L8" s="2">
-        <v>11280</v>
+        <v>9848</v>
       </c>
       <c r="M8" s="2">
-        <v>1405</v>
+        <v>2130</v>
       </c>
       <c r="N8" s="2">
-        <v>1166</v>
-      </c>
-      <c r="O8" s="1"/>
+        <v>2153</v>
+      </c>
+      <c r="O8" s="1">
+        <v>1217</v>
+      </c>
       <c r="P8" s="8">
         <f t="shared" si="0"/>
-        <v>1.1213088587390263</v>
+        <v>0.35004108463434674</v>
       </c>
       <c r="Q8" s="8">
         <f t="shared" si="1"/>
-        <v>1.4048192771084338</v>
-      </c>
-      <c r="R8" s="8" t="e">
+        <v>0.38295980078263964</v>
+      </c>
+      <c r="R8" s="8">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0.23167713687416713</v>
       </c>
       <c r="S8" s="2">
         <v>0</v>
       </c>
       <c r="T8" s="2">
-        <v>0</v>
+        <v>6772</v>
       </c>
       <c r="U8" s="2">
-        <v>0</v>
+        <v>6701</v>
       </c>
       <c r="V8" s="2">
-        <v>0</v>
+        <v>6772</v>
       </c>
       <c r="W8" s="2">
-        <v>1891</v>
+        <v>2611</v>
       </c>
       <c r="X8" s="2">
-        <v>1126</v>
-      </c>
-      <c r="Y8" s="1"/>
+        <v>2249</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>1518</v>
+      </c>
       <c r="Z8" s="8">
         <f t="shared" si="3"/>
-        <v>1.5091779728651238</v>
+        <v>0.42908792111750205</v>
       </c>
       <c r="AA8" s="9">
         <f t="shared" si="4"/>
-        <v>1.3566265060240963</v>
-      </c>
-      <c r="AB8" s="9" t="e">
+        <v>0.40003557452863747</v>
+      </c>
+      <c r="AB8" s="9">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.28897772701313534</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="B9" s="2">
         <v>0</v>
@@ -1553,170 +1552,176 @@
         <v>0</v>
       </c>
       <c r="F9" s="2">
-        <v>21492</v>
+        <v>4709</v>
       </c>
       <c r="G9" s="2">
-        <v>19652</v>
-      </c>
-      <c r="H9" s="2"/>
+        <v>4998</v>
+      </c>
+      <c r="H9" s="2">
+        <v>4493</v>
+      </c>
       <c r="I9" s="2">
-        <v>666</v>
+        <v>1</v>
       </c>
       <c r="J9" s="2">
-        <v>430069</v>
+        <v>9218</v>
       </c>
       <c r="K9" s="2">
-        <v>430212</v>
+        <v>9042</v>
       </c>
       <c r="L9" s="2">
-        <v>429655</v>
+        <v>9218</v>
       </c>
       <c r="M9" s="2">
-        <v>15353</v>
+        <v>8049</v>
       </c>
       <c r="N9" s="2">
-        <v>11599</v>
-      </c>
-      <c r="O9" s="1"/>
+        <v>4411</v>
+      </c>
+      <c r="O9" s="1">
+        <v>3258</v>
+      </c>
       <c r="P9" s="8">
         <f t="shared" si="0"/>
-        <v>0.71435883119300203</v>
+        <v>1.7092801019324697</v>
       </c>
       <c r="Q9" s="8">
         <f t="shared" si="1"/>
-        <v>0.59021982495420311</v>
-      </c>
-      <c r="R9" s="8" t="e">
+        <v>0.88255302120848345</v>
+      </c>
+      <c r="R9" s="8">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0.72512797685288222</v>
       </c>
       <c r="S9" s="2">
         <v>0</v>
       </c>
       <c r="T9" s="2">
-        <v>0</v>
+        <v>6144</v>
       </c>
       <c r="U9" s="2">
-        <v>0</v>
+        <v>6093</v>
       </c>
       <c r="V9" s="2">
-        <v>0</v>
+        <v>6144</v>
       </c>
       <c r="W9" s="2">
-        <v>28087</v>
+        <v>7199</v>
       </c>
       <c r="X9" s="2">
-        <v>13725</v>
-      </c>
-      <c r="Y9" s="1"/>
+        <v>4360</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>3525</v>
+      </c>
       <c r="Z9" s="8">
         <f t="shared" si="3"/>
-        <v>1.3068583659035919</v>
+        <v>1.5287746867700149</v>
       </c>
       <c r="AA9" s="9">
         <f t="shared" si="4"/>
-        <v>0.69840219824954208</v>
-      </c>
-      <c r="AB9" s="9" t="e">
+        <v>0.87234893957583037</v>
+      </c>
+      <c r="AB9" s="9">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.7845537502782105</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B10" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C10" s="2">
-        <v>0</v>
+        <v>310</v>
       </c>
       <c r="D10" s="2">
-        <v>0</v>
+        <v>591</v>
       </c>
       <c r="E10" s="2">
-        <v>0</v>
+        <v>310</v>
       </c>
       <c r="F10" s="2">
-        <v>6371</v>
+        <v>7196</v>
       </c>
       <c r="G10" s="2">
-        <v>7131</v>
-      </c>
-      <c r="H10" s="28">
-        <v>6190</v>
+        <v>6922</v>
+      </c>
+      <c r="H10" s="2">
+        <v>6373</v>
       </c>
       <c r="I10" s="2">
         <v>2</v>
       </c>
       <c r="J10" s="2">
-        <v>9848</v>
+        <v>22049</v>
       </c>
       <c r="K10" s="2">
-        <v>9602</v>
+        <v>12205</v>
       </c>
       <c r="L10" s="2">
-        <v>9848</v>
+        <v>9846</v>
       </c>
       <c r="M10" s="2">
-        <v>2176</v>
+        <v>4786</v>
       </c>
       <c r="N10" s="2">
-        <v>2255</v>
+        <v>2419</v>
       </c>
       <c r="O10" s="1">
-        <v>1157</v>
+        <v>1553</v>
       </c>
       <c r="P10" s="8">
         <f t="shared" si="0"/>
-        <v>0.34154763773347985</v>
+        <v>0.66509171762090047</v>
       </c>
       <c r="Q10" s="8">
         <f t="shared" si="1"/>
-        <v>0.31622493338942642</v>
+        <v>0.34946547240681886</v>
       </c>
       <c r="R10" s="8">
         <f t="shared" si="2"/>
-        <v>0.18691437802907915</v>
+        <v>0.24368429311156442</v>
       </c>
       <c r="S10" s="2">
         <v>0</v>
       </c>
       <c r="T10" s="2">
-        <v>6772</v>
+        <v>17862</v>
       </c>
       <c r="U10" s="2">
-        <v>6701</v>
+        <v>11090</v>
       </c>
       <c r="V10" s="2">
         <v>6772</v>
       </c>
       <c r="W10" s="2">
-        <v>2709</v>
+        <v>4397</v>
       </c>
       <c r="X10" s="2">
-        <v>2474</v>
+        <v>2408</v>
       </c>
       <c r="Y10" s="1">
-        <v>1514</v>
+        <v>1724</v>
       </c>
       <c r="Z10" s="8">
         <f t="shared" si="3"/>
-        <v>0.42520797363051327</v>
+        <v>0.61103390772651478</v>
       </c>
       <c r="AA10" s="9">
         <f t="shared" si="4"/>
-        <v>0.34693591361660359</v>
+        <v>0.34787633631898296</v>
       </c>
       <c r="AB10" s="9">
         <f t="shared" si="5"/>
-        <v>0.24458804523424879</v>
+        <v>0.27051624038914168</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2">
         <v>0</v>
@@ -1731,230 +1736,230 @@
         <v>0</v>
       </c>
       <c r="F11" s="2">
-        <v>4807</v>
+        <v>3380</v>
       </c>
       <c r="G11" s="2">
-        <v>5292</v>
-      </c>
-      <c r="H11" s="28">
-        <v>4740</v>
+        <v>3324</v>
+      </c>
+      <c r="H11" s="2">
+        <v>2914</v>
       </c>
       <c r="I11" s="2">
         <v>1</v>
       </c>
       <c r="J11" s="2">
-        <v>9218</v>
+        <v>4</v>
       </c>
       <c r="K11" s="2">
-        <v>9042</v>
+        <v>4</v>
       </c>
       <c r="L11" s="2">
-        <v>9218</v>
+        <v>4</v>
       </c>
       <c r="M11" s="2">
-        <v>8173</v>
+        <v>735</v>
       </c>
       <c r="N11" s="2">
-        <v>4664</v>
+        <v>553</v>
       </c>
       <c r="O11" s="1">
-        <v>3138</v>
+        <v>157</v>
       </c>
       <c r="P11" s="8">
         <f t="shared" si="0"/>
-        <v>1.700228832951945</v>
+        <v>0.21745562130177515</v>
       </c>
       <c r="Q11" s="8">
         <f t="shared" si="1"/>
-        <v>0.88133030990173844</v>
+        <v>0.16636582430806257</v>
       </c>
       <c r="R11" s="8">
         <f t="shared" si="2"/>
-        <v>0.66202531645569618</v>
+        <v>5.3877831159917636E-2</v>
       </c>
       <c r="S11" s="2">
         <v>0</v>
       </c>
       <c r="T11" s="2">
-        <v>6144</v>
+        <v>0</v>
       </c>
       <c r="U11" s="2">
-        <v>6093</v>
+        <v>0</v>
       </c>
       <c r="V11" s="2">
-        <v>6144</v>
+        <v>0</v>
       </c>
       <c r="W11" s="2">
-        <v>7364</v>
+        <v>1029</v>
       </c>
       <c r="X11" s="2">
-        <v>4589</v>
+        <v>617</v>
       </c>
       <c r="Y11" s="1">
-        <v>3433</v>
+        <v>348</v>
       </c>
       <c r="Z11" s="8">
         <f t="shared" si="3"/>
-        <v>1.5319325982941543</v>
+        <v>0.30443786982248522</v>
       </c>
       <c r="AA11" s="9">
         <f t="shared" si="4"/>
-        <v>0.86715797430083141</v>
+        <v>0.18561973525872444</v>
       </c>
       <c r="AB11" s="9">
         <f t="shared" si="5"/>
-        <v>0.72426160337552747</v>
+        <v>0.11942347288949898</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C12" s="2">
-        <v>310</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>3467</v>
+      </c>
+      <c r="G12" s="2">
+        <v>3169</v>
+      </c>
+      <c r="H12" s="2">
+        <v>2896</v>
+      </c>
+      <c r="I12" s="2">
+        <v>5</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2">
+        <v>4</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1</v>
+      </c>
+      <c r="M12" s="2">
+        <v>741</v>
+      </c>
+      <c r="N12" s="2">
         <v>591</v>
       </c>
-      <c r="E12" s="2">
-        <v>310</v>
-      </c>
-      <c r="F12" s="2">
-        <v>7271</v>
-      </c>
-      <c r="G12" s="2">
-        <v>8932</v>
-      </c>
-      <c r="H12" s="28">
-        <v>7931</v>
-      </c>
-      <c r="I12" s="2">
-        <v>2</v>
-      </c>
-      <c r="J12" s="2">
-        <v>22049</v>
-      </c>
-      <c r="K12" s="2">
-        <v>12205</v>
-      </c>
-      <c r="L12" s="2">
-        <v>9846</v>
-      </c>
-      <c r="M12" s="2">
-        <v>4921</v>
-      </c>
-      <c r="N12" s="2">
-        <v>2693</v>
-      </c>
       <c r="O12" s="1">
-        <v>1456</v>
+        <v>168</v>
       </c>
       <c r="P12" s="8">
         <f t="shared" si="0"/>
-        <v>0.67679823958190066</v>
+        <v>0.21372944909143352</v>
       </c>
       <c r="Q12" s="8">
         <f t="shared" si="1"/>
-        <v>0.30150022391401704</v>
+        <v>0.18649416219627643</v>
       </c>
       <c r="R12" s="8">
         <f t="shared" si="2"/>
-        <v>0.18358340688437777</v>
+        <v>5.8011049723756904E-2</v>
       </c>
       <c r="S12" s="2">
         <v>0</v>
       </c>
       <c r="T12" s="2">
-        <v>17862</v>
+        <v>0</v>
       </c>
       <c r="U12" s="2">
-        <v>11090</v>
+        <v>0</v>
       </c>
       <c r="V12" s="2">
-        <v>6772</v>
+        <v>0</v>
       </c>
       <c r="W12" s="2">
-        <v>4521</v>
+        <v>1048</v>
       </c>
       <c r="X12" s="2">
-        <v>2579</v>
+        <v>667</v>
       </c>
       <c r="Y12" s="1">
-        <v>1694</v>
+        <v>360</v>
       </c>
       <c r="Z12" s="8">
         <f t="shared" si="3"/>
-        <v>0.62178517397881994</v>
+        <v>0.30227862705509084</v>
       </c>
       <c r="AA12" s="9">
         <f t="shared" si="4"/>
-        <v>0.28873712494402148</v>
+        <v>0.21047649100662669</v>
       </c>
       <c r="AB12" s="9">
         <f t="shared" si="5"/>
-        <v>0.21359223300970873</v>
+        <v>0.12430939226519337</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C13" s="2">
-        <v>0</v>
+        <v>868</v>
       </c>
       <c r="D13" s="2">
-        <v>0</v>
+        <v>868</v>
       </c>
       <c r="E13" s="2">
-        <v>0</v>
+        <v>868</v>
       </c>
       <c r="F13" s="2">
-        <v>3491</v>
+        <v>6377</v>
       </c>
       <c r="G13" s="2">
-        <v>3085</v>
+        <v>5779</v>
       </c>
       <c r="H13" s="2">
-        <v>2817</v>
+        <v>5210</v>
       </c>
       <c r="I13" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J13" s="2">
         <v>4</v>
       </c>
       <c r="K13" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L13" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M13" s="2">
-        <v>806</v>
+        <v>1746</v>
       </c>
       <c r="N13" s="2">
-        <v>598</v>
+        <v>1262</v>
       </c>
       <c r="O13" s="1">
-        <v>155</v>
+        <v>576</v>
       </c>
       <c r="P13" s="8">
         <f t="shared" si="0"/>
-        <v>0.23087940418218275</v>
+        <v>0.27379645601379959</v>
       </c>
       <c r="Q13" s="8">
         <f t="shared" si="1"/>
-        <v>0.19384116693679093</v>
+        <v>0.21837688181346254</v>
       </c>
       <c r="R13" s="8">
         <f t="shared" si="2"/>
-        <v>5.5023074192403265E-2</v>
+        <v>0.11055662188099807</v>
       </c>
       <c r="S13" s="2">
         <v>0</v>
@@ -1969,30 +1974,30 @@
         <v>0</v>
       </c>
       <c r="W13" s="2">
-        <v>1032</v>
+        <v>2019</v>
       </c>
       <c r="X13" s="2">
-        <v>629</v>
+        <v>1439</v>
       </c>
       <c r="Y13" s="1">
-        <v>348</v>
+        <v>885</v>
       </c>
       <c r="Z13" s="8">
         <f t="shared" si="3"/>
-        <v>0.29561730163277</v>
+        <v>0.31660655480633526</v>
       </c>
       <c r="AA13" s="9">
         <f t="shared" si="4"/>
-        <v>0.20388978930307941</v>
+        <v>0.24900501816923343</v>
       </c>
       <c r="AB13" s="9">
         <f t="shared" si="5"/>
-        <v>0.1235356762513312</v>
+        <v>0.16986564299424184</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2">
         <v>0</v>
@@ -2007,46 +2012,46 @@
         <v>0</v>
       </c>
       <c r="F14" s="2">
-        <v>3466</v>
+        <v>5375</v>
       </c>
       <c r="G14" s="2">
-        <v>3197</v>
+        <v>3106</v>
       </c>
       <c r="H14" s="2">
-        <v>2821</v>
+        <v>2915</v>
       </c>
       <c r="I14" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="2">
-        <v>808</v>
+        <v>1716</v>
       </c>
       <c r="N14" s="2">
-        <v>653</v>
+        <v>1154</v>
       </c>
       <c r="O14" s="1">
-        <v>164</v>
+        <v>923</v>
       </c>
       <c r="P14" s="8">
         <f t="shared" si="0"/>
-        <v>0.23312175418349682</v>
+        <v>0.3192558139534884</v>
       </c>
       <c r="Q14" s="8">
         <f t="shared" si="1"/>
-        <v>0.20425398811385673</v>
+        <v>0.37153895685769478</v>
       </c>
       <c r="R14" s="8">
         <f t="shared" si="2"/>
-        <v>5.8135412974122655E-2</v>
+        <v>0.31663807890222984</v>
       </c>
       <c r="S14" s="2">
         <v>0</v>
@@ -2061,84 +2066,84 @@
         <v>0</v>
       </c>
       <c r="W14" s="2">
-        <v>1041</v>
+        <v>1957</v>
       </c>
       <c r="X14" s="2">
-        <v>673</v>
+        <v>909</v>
       </c>
       <c r="Y14" s="1">
-        <v>361</v>
+        <v>564</v>
       </c>
       <c r="Z14" s="8">
         <f t="shared" si="3"/>
-        <v>0.30034622042700521</v>
+        <v>0.36409302325581394</v>
       </c>
       <c r="AA14" s="9">
         <f t="shared" si="4"/>
-        <v>0.21050985298717548</v>
+        <v>0.29265936896329686</v>
       </c>
       <c r="AB14" s="9">
         <f t="shared" si="5"/>
-        <v>0.12796880538816022</v>
+        <v>0.1934819897084048</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B15" s="2">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C15" s="2">
-        <v>868</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2">
-        <v>868</v>
+        <v>0</v>
       </c>
       <c r="E15" s="2">
-        <v>868</v>
+        <v>0</v>
       </c>
       <c r="F15" s="2">
-        <v>6364</v>
+        <v>1424</v>
       </c>
       <c r="G15" s="2">
-        <v>5690</v>
+        <v>1428</v>
       </c>
       <c r="H15" s="2">
-        <v>5046</v>
+        <v>1272</v>
       </c>
       <c r="I15" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J15" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K15" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L15" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M15" s="2">
-        <v>1905</v>
+        <v>412</v>
       </c>
       <c r="N15" s="2">
-        <v>1339</v>
+        <v>355</v>
       </c>
       <c r="O15" s="1">
-        <v>557</v>
+        <v>90</v>
       </c>
       <c r="P15" s="8">
         <f t="shared" si="0"/>
-        <v>0.29934003771213075</v>
+        <v>0.2893258426966292</v>
       </c>
       <c r="Q15" s="8">
         <f t="shared" si="1"/>
-        <v>0.23532513181019332</v>
+        <v>0.24859943977591037</v>
       </c>
       <c r="R15" s="8">
         <f t="shared" si="2"/>
-        <v>0.11038446294094333</v>
+        <v>7.0754716981132074E-2</v>
       </c>
       <c r="S15" s="2">
         <v>0</v>
@@ -2153,30 +2158,30 @@
         <v>0</v>
       </c>
       <c r="W15" s="2">
-        <v>2000</v>
+        <v>681</v>
       </c>
       <c r="X15" s="2">
-        <v>1463</v>
+        <v>383</v>
       </c>
       <c r="Y15" s="1">
-        <v>880</v>
+        <v>248</v>
       </c>
       <c r="Z15" s="8">
         <f t="shared" si="3"/>
-        <v>0.31426775612822122</v>
+        <v>0.4782303370786517</v>
       </c>
       <c r="AA15" s="9">
         <f t="shared" si="4"/>
-        <v>0.2571177504393673</v>
+        <v>0.26820728291316526</v>
       </c>
       <c r="AB15" s="9">
         <f t="shared" si="5"/>
-        <v>0.17439556084026953</v>
+        <v>0.19496855345911951</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B16" s="2">
         <v>0</v>
@@ -2191,16 +2196,16 @@
         <v>0</v>
       </c>
       <c r="F16" s="2">
-        <v>5350</v>
+        <v>13103</v>
       </c>
       <c r="G16" s="2">
-        <v>3121</v>
+        <v>13126</v>
       </c>
       <c r="H16" s="2">
-        <v>2870</v>
+        <v>12476</v>
       </c>
       <c r="I16" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J16" s="2">
         <v>0</v>
@@ -2212,25 +2217,25 @@
         <v>0</v>
       </c>
       <c r="M16" s="2">
-        <v>1808</v>
+        <v>4684</v>
       </c>
       <c r="N16" s="2">
-        <v>1214</v>
+        <v>3089</v>
       </c>
       <c r="O16" s="1">
-        <v>891</v>
+        <v>2242</v>
       </c>
       <c r="P16" s="8">
         <f t="shared" si="0"/>
-        <v>0.33794392523364486</v>
+        <v>0.35747538731588185</v>
       </c>
       <c r="Q16" s="8">
         <f t="shared" si="1"/>
-        <v>0.38897789170137775</v>
+        <v>0.23533445070851744</v>
       </c>
       <c r="R16" s="8">
         <f t="shared" si="2"/>
-        <v>0.31045296167247388</v>
+        <v>0.17970503366463611</v>
       </c>
       <c r="S16" s="2">
         <v>0</v>
@@ -2245,122 +2250,122 @@
         <v>0</v>
       </c>
       <c r="W16" s="2">
-        <v>1956</v>
+        <v>6201</v>
       </c>
       <c r="X16" s="2">
-        <v>944</v>
+        <v>4531</v>
       </c>
       <c r="Y16" s="1">
-        <v>549</v>
+        <v>3190</v>
       </c>
       <c r="Z16" s="8">
         <f t="shared" si="3"/>
-        <v>0.36560747663551402</v>
+        <v>0.4732504006716019</v>
       </c>
       <c r="AA16" s="9">
         <f t="shared" si="4"/>
-        <v>0.30246715796219159</v>
+        <v>0.34519274721925947</v>
       </c>
       <c r="AB16" s="9">
         <f t="shared" si="5"/>
-        <v>0.19128919860627178</v>
+        <v>0.25569092657903175</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B17" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C17" s="2">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="D17" s="2">
-        <v>0</v>
+        <v>475</v>
       </c>
       <c r="E17" s="2">
-        <v>0</v>
+        <v>465</v>
       </c>
       <c r="F17" s="2">
-        <v>1418</v>
+        <v>7477</v>
       </c>
       <c r="G17" s="2">
-        <v>1436</v>
+        <v>7225</v>
       </c>
       <c r="H17" s="2">
-        <v>1250</v>
+        <v>6296</v>
       </c>
       <c r="I17" s="2">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="J17" s="2">
-        <v>0</v>
+        <v>148538</v>
       </c>
       <c r="K17" s="2">
-        <v>0</v>
+        <v>146678</v>
       </c>
       <c r="L17" s="2">
-        <v>0</v>
+        <v>148569</v>
       </c>
       <c r="M17" s="2">
-        <v>434</v>
+        <v>4037</v>
       </c>
       <c r="N17" s="2">
-        <v>403</v>
+        <v>4134</v>
       </c>
       <c r="O17" s="1">
-        <v>131</v>
+        <v>3072</v>
       </c>
       <c r="P17" s="8">
         <f t="shared" si="0"/>
-        <v>0.306064880112835</v>
+        <v>0.53992242878159691</v>
       </c>
       <c r="Q17" s="8">
         <f t="shared" si="1"/>
-        <v>0.28064066852367686</v>
+        <v>0.57217993079584772</v>
       </c>
       <c r="R17" s="8">
         <f t="shared" si="2"/>
-        <v>0.1048</v>
+        <v>0.48792884371029227</v>
       </c>
       <c r="S17" s="2">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="T17" s="2">
-        <v>0</v>
+        <v>121437</v>
       </c>
       <c r="U17" s="2">
-        <v>0</v>
+        <v>120719</v>
       </c>
       <c r="V17" s="2">
-        <v>0</v>
+        <v>121458</v>
       </c>
       <c r="W17" s="2">
-        <v>675</v>
+        <v>4475</v>
       </c>
       <c r="X17" s="2">
-        <v>405</v>
+        <v>4787</v>
       </c>
       <c r="Y17" s="1">
-        <v>252</v>
+        <v>3663</v>
       </c>
       <c r="Z17" s="8">
         <f t="shared" si="3"/>
-        <v>0.47602256699576867</v>
+        <v>0.5985020730239401</v>
       </c>
       <c r="AA17" s="9">
         <f t="shared" si="4"/>
-        <v>0.28203342618384403</v>
+        <v>0.66256055363321797</v>
       </c>
       <c r="AB17" s="9">
         <f t="shared" si="5"/>
-        <v>0.2016</v>
+        <v>0.58179796696315123</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B18" s="2">
         <v>0</v>
@@ -2375,176 +2380,176 @@
         <v>0</v>
       </c>
       <c r="F18" s="2">
-        <v>12922</v>
+        <v>3777</v>
       </c>
       <c r="G18" s="2">
-        <v>13166</v>
+        <v>3633</v>
       </c>
       <c r="H18" s="2">
-        <v>11881</v>
+        <v>3257</v>
       </c>
       <c r="I18" s="2">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="J18" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K18" s="2">
-        <v>0</v>
+        <v>377364</v>
       </c>
       <c r="L18" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M18" s="2">
-        <v>5066</v>
+        <v>1322</v>
       </c>
       <c r="N18" s="2">
-        <v>3384</v>
+        <v>1031</v>
       </c>
       <c r="O18" s="1">
-        <v>2168</v>
+        <v>341</v>
       </c>
       <c r="P18" s="8">
         <f t="shared" si="0"/>
-        <v>0.39204457514316671</v>
+        <v>0.35001323801959228</v>
       </c>
       <c r="Q18" s="8">
         <f t="shared" si="1"/>
-        <v>0.25702567218593347</v>
+        <v>0.28378750344068265</v>
       </c>
       <c r="R18" s="8">
         <f t="shared" si="2"/>
-        <v>0.18247622254019022</v>
+        <v>0.10469757445501995</v>
       </c>
       <c r="S18" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T18" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U18" s="2">
-        <v>0</v>
+        <v>26458</v>
       </c>
       <c r="V18" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W18" s="2">
-        <v>6197</v>
+        <v>7488</v>
       </c>
       <c r="X18" s="2">
-        <v>4616</v>
+        <v>1252</v>
       </c>
       <c r="Y18" s="1">
-        <v>3097</v>
+        <v>716</v>
       </c>
       <c r="Z18" s="8">
         <f t="shared" si="3"/>
-        <v>0.47956972604859927</v>
+        <v>1.9825258141382049</v>
       </c>
       <c r="AA18" s="9">
         <f t="shared" si="4"/>
-        <v>0.35060003038128512</v>
+        <v>0.34461877236443711</v>
       </c>
       <c r="AB18" s="9">
         <f t="shared" si="5"/>
-        <v>0.26066829391465363</v>
+        <v>0.21983420325452871</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B19" s="2">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>4573</v>
+      </c>
+      <c r="G19" s="2">
+        <v>4098</v>
+      </c>
+      <c r="H19" s="2">
+        <v>2919</v>
+      </c>
+      <c r="I19" s="2">
         <v>4</v>
       </c>
-      <c r="C19" s="2">
-        <v>58</v>
-      </c>
-      <c r="D19" s="2">
-        <v>475</v>
-      </c>
-      <c r="E19" s="2">
-        <v>465</v>
-      </c>
-      <c r="F19" s="2">
-        <v>7552</v>
-      </c>
-      <c r="G19" s="2">
-        <v>7234</v>
-      </c>
-      <c r="H19" s="2">
-        <v>6111</v>
-      </c>
-      <c r="I19" s="2">
-        <v>53</v>
-      </c>
       <c r="J19" s="2">
-        <v>148538</v>
+        <v>8124</v>
       </c>
       <c r="K19" s="2">
-        <v>146678</v>
+        <v>4062</v>
       </c>
       <c r="L19" s="2">
-        <v>148569</v>
+        <v>4062</v>
       </c>
       <c r="M19" s="2">
-        <v>4256</v>
+        <v>1621</v>
       </c>
       <c r="N19" s="2">
-        <v>4351</v>
+        <v>1746</v>
       </c>
       <c r="O19" s="1">
-        <v>2978</v>
+        <v>855</v>
       </c>
       <c r="P19" s="8">
         <f t="shared" si="0"/>
-        <v>0.56355932203389836</v>
+        <v>0.35447190028427727</v>
       </c>
       <c r="Q19" s="8">
         <f t="shared" si="1"/>
-        <v>0.60146530273707488</v>
+        <v>0.42606149341142019</v>
       </c>
       <c r="R19" s="8">
         <f t="shared" si="2"/>
-        <v>0.487317951235477</v>
+        <v>0.29290853031860226</v>
       </c>
       <c r="S19" s="2">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="T19" s="2">
-        <v>121437</v>
+        <v>0</v>
       </c>
       <c r="U19" s="2">
-        <v>120719</v>
+        <v>0</v>
       </c>
       <c r="V19" s="2">
-        <v>121458</v>
+        <v>0</v>
       </c>
       <c r="W19" s="2">
-        <v>4515</v>
+        <v>2173</v>
       </c>
       <c r="X19" s="2">
-        <v>4857</v>
+        <v>1593</v>
       </c>
       <c r="Y19" s="1">
-        <v>3606</v>
+        <v>1061</v>
       </c>
       <c r="Z19" s="8">
         <f t="shared" si="3"/>
-        <v>0.59785487288135597</v>
+        <v>0.4751804067351848</v>
       </c>
       <c r="AA19" s="9">
         <f t="shared" si="4"/>
-        <v>0.67141277301631186</v>
+        <v>0.38872620790629575</v>
       </c>
       <c r="AB19" s="9">
         <f t="shared" si="5"/>
-        <v>0.59008345606283752</v>
+        <v>0.36348064405618363</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B20" s="2">
         <v>0</v>
@@ -2559,84 +2564,84 @@
         <v>0</v>
       </c>
       <c r="F20" s="2">
-        <v>3690</v>
+        <v>4734</v>
       </c>
       <c r="G20" s="2">
-        <v>3646</v>
+        <v>4270</v>
       </c>
       <c r="H20" s="2">
-        <v>3042</v>
+        <v>3035</v>
       </c>
       <c r="I20" s="2">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="J20" s="2">
-        <v>4</v>
+        <v>6160</v>
       </c>
       <c r="K20" s="2">
-        <v>377364</v>
+        <v>6</v>
       </c>
       <c r="L20" s="2">
-        <v>4</v>
+        <v>6154</v>
       </c>
       <c r="M20" s="2">
-        <v>1507</v>
+        <v>1590</v>
       </c>
       <c r="N20" s="2">
-        <v>1389</v>
+        <v>1527</v>
       </c>
       <c r="O20" s="1">
-        <v>330</v>
+        <v>827</v>
       </c>
       <c r="P20" s="8">
         <f t="shared" si="0"/>
-        <v>0.40840108401084013</v>
+        <v>0.33586818757921422</v>
       </c>
       <c r="Q20" s="8">
         <f t="shared" si="1"/>
-        <v>0.38096544157981349</v>
+        <v>0.35761124121779858</v>
       </c>
       <c r="R20" s="8">
         <f t="shared" si="2"/>
-        <v>0.10848126232741617</v>
+        <v>0.27248764415156507</v>
       </c>
       <c r="S20" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T20" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="U20" s="2">
-        <v>26458</v>
+        <v>0</v>
       </c>
       <c r="V20" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="W20" s="2">
-        <v>7473</v>
+        <v>2167</v>
       </c>
       <c r="X20" s="2">
-        <v>1342</v>
+        <v>1577</v>
       </c>
       <c r="Y20" s="1">
-        <v>710</v>
+        <v>1043</v>
       </c>
       <c r="Z20" s="8">
         <f t="shared" si="3"/>
-        <v>2.0252032520325205</v>
+        <v>0.45775242923531895</v>
       </c>
       <c r="AA20" s="9">
         <f t="shared" si="4"/>
-        <v>0.36807460230389466</v>
+        <v>0.36932084309133489</v>
       </c>
       <c r="AB20" s="9">
         <f t="shared" si="5"/>
-        <v>0.23339907955292571</v>
+        <v>0.34365733113673808</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B21" s="2">
         <v>0</v>
@@ -2651,46 +2656,46 @@
         <v>0</v>
       </c>
       <c r="F21" s="2">
-        <v>6032</v>
+        <v>5900</v>
       </c>
       <c r="G21" s="2">
-        <v>4258</v>
-      </c>
-      <c r="H21" s="28">
-        <v>4184</v>
+        <v>5178</v>
+      </c>
+      <c r="H21" s="2">
+        <v>3712</v>
       </c>
       <c r="I21" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J21" s="2">
-        <v>8124</v>
+        <v>2</v>
       </c>
       <c r="K21" s="2">
-        <v>4062</v>
+        <v>3525</v>
       </c>
       <c r="L21" s="2">
-        <v>4062</v>
+        <v>3525</v>
       </c>
       <c r="M21" s="2">
-        <v>1790</v>
+        <v>2183</v>
       </c>
       <c r="N21" s="2">
-        <v>1846</v>
+        <v>1502</v>
       </c>
       <c r="O21" s="1">
-        <v>839</v>
+        <v>744</v>
       </c>
       <c r="P21" s="8">
         <f t="shared" si="0"/>
-        <v>0.2967506631299735</v>
+        <v>0.37</v>
       </c>
       <c r="Q21" s="8">
         <f t="shared" si="1"/>
-        <v>0.43353687177078443</v>
+        <v>0.29007338740826571</v>
       </c>
       <c r="R21" s="8">
         <f t="shared" si="2"/>
-        <v>0.20052581261950286</v>
+        <v>0.20043103448275862</v>
       </c>
       <c r="S21" s="2">
         <v>0</v>
@@ -2705,30 +2710,30 @@
         <v>0</v>
       </c>
       <c r="W21" s="2">
-        <v>2270</v>
+        <v>2758</v>
       </c>
       <c r="X21" s="2">
-        <v>1706</v>
+        <v>2088</v>
       </c>
       <c r="Y21" s="1">
-        <v>1062</v>
+        <v>1162</v>
       </c>
       <c r="Z21" s="8">
         <f t="shared" si="3"/>
-        <v>0.37632625994694963</v>
+        <v>0.46745762711864408</v>
       </c>
       <c r="AA21" s="9">
         <f t="shared" si="4"/>
-        <v>0.40065758572099575</v>
+        <v>0.40324449594438005</v>
       </c>
       <c r="AB21" s="9">
         <f t="shared" si="5"/>
-        <v>0.2538240917782027</v>
+        <v>0.31303879310344829</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B22" s="2">
         <v>0</v>
@@ -2743,46 +2748,46 @@
         <v>0</v>
       </c>
       <c r="F22" s="2">
-        <v>4918</v>
+        <v>3965</v>
       </c>
       <c r="G22" s="2">
-        <v>4441</v>
-      </c>
-      <c r="H22" s="28">
-        <v>3943</v>
+        <v>3808</v>
+      </c>
+      <c r="H22" s="2">
+        <v>2940</v>
       </c>
       <c r="I22" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J22" s="2">
-        <v>6160</v>
+        <v>0</v>
       </c>
       <c r="K22" s="2">
-        <v>6</v>
+        <v>4057</v>
       </c>
       <c r="L22" s="2">
-        <v>6154</v>
+        <v>4057</v>
       </c>
       <c r="M22" s="2">
-        <v>1803</v>
+        <v>699</v>
       </c>
       <c r="N22" s="2">
-        <v>1668</v>
+        <v>678</v>
       </c>
       <c r="O22" s="1">
-        <v>804</v>
+        <v>310</v>
       </c>
       <c r="P22" s="8">
         <f t="shared" si="0"/>
-        <v>0.36661244408296056</v>
+        <v>0.17629255989911727</v>
       </c>
       <c r="Q22" s="8">
         <f t="shared" si="1"/>
-        <v>0.37559108308939426</v>
+        <v>0.17804621848739496</v>
       </c>
       <c r="R22" s="8">
         <f t="shared" si="2"/>
-        <v>0.20390565559218868</v>
+        <v>0.10544217687074831</v>
       </c>
       <c r="S22" s="2">
         <v>0</v>
@@ -2797,30 +2802,30 @@
         <v>0</v>
       </c>
       <c r="W22" s="2">
-        <v>2265</v>
+        <v>942</v>
       </c>
       <c r="X22" s="2">
-        <v>1679</v>
+        <v>785</v>
       </c>
       <c r="Y22" s="1">
-        <v>1050</v>
+        <v>557</v>
       </c>
       <c r="Z22" s="8">
         <f t="shared" si="3"/>
-        <v>0.46055307035380239</v>
+        <v>0.23757881462799496</v>
       </c>
       <c r="AA22" s="9">
         <f t="shared" si="4"/>
-        <v>0.37806800270209412</v>
+        <v>0.20614495798319327</v>
       </c>
       <c r="AB22" s="9">
         <f t="shared" si="5"/>
-        <v>0.26629469946741058</v>
+        <v>0.18945578231292518</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B23" s="2">
         <v>0</v>
@@ -2835,46 +2840,46 @@
         <v>0</v>
       </c>
       <c r="F23" s="2">
-        <v>6137</v>
+        <v>3747</v>
       </c>
       <c r="G23" s="2">
-        <v>5354</v>
-      </c>
-      <c r="H23" s="28">
-        <v>5109</v>
+        <v>3759</v>
+      </c>
+      <c r="H23" s="2">
+        <v>2753</v>
       </c>
       <c r="I23" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J23" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K23" s="2">
-        <v>3525</v>
+        <v>0</v>
       </c>
       <c r="L23" s="2">
-        <v>3525</v>
+        <v>1</v>
       </c>
       <c r="M23" s="2">
-        <v>2358</v>
+        <v>692</v>
       </c>
       <c r="N23" s="2">
-        <v>1673</v>
+        <v>693</v>
       </c>
       <c r="O23" s="1">
-        <v>719</v>
+        <v>340</v>
       </c>
       <c r="P23" s="8">
         <f t="shared" si="0"/>
-        <v>0.38422682092227473</v>
+        <v>0.18468107819589005</v>
       </c>
       <c r="Q23" s="8">
         <f t="shared" si="1"/>
-        <v>0.31247665296974225</v>
+        <v>0.18435754189944134</v>
       </c>
       <c r="R23" s="8">
         <f t="shared" si="2"/>
-        <v>0.14073204149540028</v>
+        <v>0.12350163458045768</v>
       </c>
       <c r="S23" s="2">
         <v>0</v>
@@ -2889,30 +2894,30 @@
         <v>0</v>
       </c>
       <c r="W23" s="2">
-        <v>2886</v>
+        <v>966</v>
       </c>
       <c r="X23" s="2">
-        <v>2224</v>
+        <v>775</v>
       </c>
       <c r="Y23" s="1">
-        <v>1164</v>
+        <v>536</v>
       </c>
       <c r="Z23" s="8">
         <f t="shared" si="3"/>
-        <v>0.47026234316441257</v>
+        <v>0.2578062449959968</v>
       </c>
       <c r="AA23" s="9">
         <f t="shared" si="4"/>
-        <v>0.41539036234590959</v>
+        <v>0.20617185421654696</v>
       </c>
       <c r="AB23" s="9">
         <f t="shared" si="5"/>
-        <v>0.22783323546682324</v>
+        <v>0.19469669451507446</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B24" s="2">
         <v>0</v>
@@ -2927,46 +2932,46 @@
         <v>0</v>
       </c>
       <c r="F24" s="2">
-        <v>4060</v>
+        <v>3848</v>
       </c>
       <c r="G24" s="2">
-        <v>3836</v>
+        <v>3527</v>
       </c>
       <c r="H24" s="2">
-        <v>2830</v>
+        <v>2654</v>
       </c>
       <c r="I24" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J24" s="2">
-        <v>0</v>
+        <v>7050</v>
       </c>
       <c r="K24" s="2">
-        <v>4057</v>
+        <v>3525</v>
       </c>
       <c r="L24" s="2">
-        <v>4057</v>
+        <v>3525</v>
       </c>
       <c r="M24" s="2">
-        <v>768</v>
+        <v>1937</v>
       </c>
       <c r="N24" s="2">
-        <v>749</v>
+        <v>1605</v>
       </c>
       <c r="O24" s="1">
-        <v>302</v>
+        <v>865</v>
       </c>
       <c r="P24" s="8">
         <f t="shared" si="0"/>
-        <v>0.18916256157635469</v>
+        <v>0.5033783783783784</v>
       </c>
       <c r="Q24" s="8">
         <f t="shared" si="1"/>
-        <v>0.19525547445255476</v>
+        <v>0.45506095832151972</v>
       </c>
       <c r="R24" s="8">
         <f t="shared" si="2"/>
-        <v>0.10671378091872792</v>
+        <v>0.32592313489073099</v>
       </c>
       <c r="S24" s="2">
         <v>0</v>
@@ -2981,84 +2986,84 @@
         <v>0</v>
       </c>
       <c r="W24" s="2">
-        <v>953</v>
+        <v>2702</v>
       </c>
       <c r="X24" s="2">
-        <v>845</v>
+        <v>1842</v>
       </c>
       <c r="Y24" s="1">
-        <v>553</v>
+        <v>1281</v>
       </c>
       <c r="Z24" s="8">
         <f t="shared" si="3"/>
-        <v>0.23472906403940888</v>
+        <v>0.70218295218295224</v>
       </c>
       <c r="AA24" s="9">
         <f t="shared" si="4"/>
-        <v>0.22028154327424401</v>
+        <v>0.52225687553161326</v>
       </c>
       <c r="AB24" s="9">
         <f t="shared" si="5"/>
-        <v>0.19540636042402826</v>
+        <v>0.48266767143933687</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B25" s="2">
-        <v>0</v>
+        <v>1967</v>
       </c>
       <c r="C25" s="2">
-        <v>0</v>
+        <v>3650</v>
       </c>
       <c r="D25" s="2">
-        <v>0</v>
+        <v>4118</v>
       </c>
       <c r="E25" s="2">
-        <v>0</v>
+        <v>4083</v>
       </c>
       <c r="F25" s="2">
-        <v>3842</v>
+        <v>6815</v>
       </c>
       <c r="G25" s="2">
-        <v>3768</v>
+        <v>5864</v>
       </c>
       <c r="H25" s="2">
-        <v>2651</v>
+        <v>4136</v>
       </c>
       <c r="I25" s="2">
-        <v>3</v>
+        <v>377</v>
       </c>
       <c r="J25" s="2">
-        <v>1</v>
+        <v>2343</v>
       </c>
       <c r="K25" s="2">
-        <v>0</v>
+        <v>1194</v>
       </c>
       <c r="L25" s="2">
-        <v>1</v>
+        <v>1176</v>
       </c>
       <c r="M25" s="2">
-        <v>793</v>
+        <v>5097</v>
       </c>
       <c r="N25" s="2">
-        <v>808</v>
+        <v>2161</v>
       </c>
       <c r="O25" s="1">
-        <v>331</v>
+        <v>1358</v>
       </c>
       <c r="P25" s="8">
         <f t="shared" si="0"/>
-        <v>0.20640291514836023</v>
+        <v>0.74790902421129857</v>
       </c>
       <c r="Q25" s="8">
         <f t="shared" si="1"/>
-        <v>0.21443736730360935</v>
+        <v>0.36851978171896316</v>
       </c>
       <c r="R25" s="8">
         <f t="shared" si="2"/>
-        <v>0.12485854394568087</v>
+        <v>0.32833655705996134</v>
       </c>
       <c r="S25" s="2">
         <v>0</v>
@@ -3073,30 +3078,30 @@
         <v>0</v>
       </c>
       <c r="W25" s="2">
-        <v>983</v>
+        <v>5357</v>
       </c>
       <c r="X25" s="2">
-        <v>825</v>
+        <v>2968</v>
       </c>
       <c r="Y25" s="1">
-        <v>542</v>
+        <v>1832</v>
       </c>
       <c r="Z25" s="8">
         <f t="shared" si="3"/>
-        <v>0.25585632483081727</v>
+        <v>0.78606016140865742</v>
       </c>
       <c r="AA25" s="9">
         <f t="shared" si="4"/>
-        <v>0.21894904458598727</v>
+        <v>0.50613915416098232</v>
       </c>
       <c r="AB25" s="9">
         <f t="shared" si="5"/>
-        <v>0.20445115050924179</v>
+        <v>0.44294003868471954</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B26" s="2">
         <v>0</v>
@@ -3111,176 +3116,176 @@
         <v>0</v>
       </c>
       <c r="F26" s="2">
-        <v>3931</v>
+        <v>6250</v>
       </c>
       <c r="G26" s="2">
-        <v>3663</v>
-      </c>
-      <c r="H26" s="28">
-        <v>3724</v>
+        <v>5784</v>
+      </c>
+      <c r="H26" s="2">
+        <v>5251</v>
       </c>
       <c r="I26" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J26" s="2">
-        <v>7050</v>
+        <v>19668</v>
       </c>
       <c r="K26" s="2">
-        <v>3525</v>
+        <v>13892</v>
       </c>
       <c r="L26" s="2">
-        <v>3525</v>
+        <v>13892</v>
       </c>
       <c r="M26" s="2">
-        <v>2297</v>
+        <v>10260</v>
       </c>
       <c r="N26" s="2">
-        <v>1782</v>
+        <v>2863</v>
       </c>
       <c r="O26" s="1">
-        <v>843</v>
+        <v>1824</v>
       </c>
       <c r="P26" s="8">
         <f t="shared" si="0"/>
-        <v>0.58432968710251842</v>
+        <v>1.6415999999999999</v>
       </c>
       <c r="Q26" s="8">
         <f t="shared" si="1"/>
-        <v>0.48648648648648651</v>
+        <v>0.49498616874135548</v>
       </c>
       <c r="R26" s="8">
         <f t="shared" si="2"/>
-        <v>0.22636949516648766</v>
+        <v>0.34736240716054084</v>
       </c>
       <c r="S26" s="2">
         <v>0</v>
       </c>
       <c r="T26" s="2">
-        <v>0</v>
+        <v>13542</v>
       </c>
       <c r="U26" s="2">
-        <v>0</v>
+        <v>6771</v>
       </c>
       <c r="V26" s="2">
-        <v>0</v>
+        <v>6771</v>
       </c>
       <c r="W26" s="2">
-        <v>2795</v>
+        <v>10385</v>
       </c>
       <c r="X26" s="2">
-        <v>2041</v>
+        <v>2868</v>
       </c>
       <c r="Y26" s="1">
-        <v>1271</v>
+        <v>2112</v>
       </c>
       <c r="Z26" s="8">
         <f t="shared" si="3"/>
-        <v>0.71101500890358682</v>
+        <v>1.6616</v>
       </c>
       <c r="AA26" s="9">
         <f t="shared" si="4"/>
-        <v>0.55719355719355723</v>
+        <v>0.49585062240663902</v>
       </c>
       <c r="AB26" s="9">
         <f t="shared" si="5"/>
-        <v>0.34129967776584319</v>
+        <v>0.40220910302799467</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B27" s="2">
-        <v>1967</v>
+        <v>0</v>
       </c>
       <c r="C27" s="2">
-        <v>3650</v>
+        <v>0</v>
       </c>
       <c r="D27" s="2">
-        <v>4118</v>
+        <v>0</v>
       </c>
       <c r="E27" s="2">
-        <v>4083</v>
+        <v>0</v>
       </c>
       <c r="F27" s="2">
-        <v>6038</v>
+        <v>7137</v>
       </c>
       <c r="G27" s="2">
-        <v>5882</v>
+        <v>6704</v>
       </c>
       <c r="H27" s="2">
-        <v>3992</v>
+        <v>5789</v>
       </c>
       <c r="I27" s="2">
-        <v>377</v>
+        <v>2</v>
       </c>
       <c r="J27" s="2">
-        <v>2343</v>
+        <v>19670</v>
       </c>
       <c r="K27" s="2">
-        <v>1194</v>
+        <v>6992</v>
       </c>
       <c r="L27" s="2">
-        <v>1176</v>
+        <v>19670</v>
       </c>
       <c r="M27" s="2">
-        <v>5296</v>
+        <v>10219</v>
       </c>
       <c r="N27" s="2">
-        <v>2342</v>
+        <v>2825</v>
       </c>
       <c r="O27" s="1">
-        <v>1305</v>
+        <v>1852</v>
       </c>
       <c r="P27" s="8">
         <f t="shared" si="0"/>
-        <v>0.87711162636634643</v>
+        <v>1.4318341039652516</v>
       </c>
       <c r="Q27" s="8">
         <f t="shared" si="1"/>
-        <v>0.39816388983339002</v>
+        <v>0.42139021479713606</v>
       </c>
       <c r="R27" s="8">
         <f t="shared" si="2"/>
-        <v>0.32690380761523047</v>
+        <v>0.31991708412506475</v>
       </c>
       <c r="S27" s="2">
         <v>0</v>
       </c>
       <c r="T27" s="2">
-        <v>0</v>
+        <v>13542</v>
       </c>
       <c r="U27" s="2">
         <v>0</v>
       </c>
       <c r="V27" s="2">
-        <v>0</v>
+        <v>13542</v>
       </c>
       <c r="W27" s="2">
-        <v>5387</v>
+        <v>10410</v>
       </c>
       <c r="X27" s="2">
-        <v>3045</v>
+        <v>2835</v>
       </c>
       <c r="Y27" s="1">
-        <v>1830</v>
+        <v>2003</v>
       </c>
       <c r="Z27" s="8">
         <f t="shared" si="3"/>
-        <v>0.89218284200066245</v>
+        <v>1.4585960487599832</v>
       </c>
       <c r="AA27" s="9">
         <f t="shared" si="4"/>
-        <v>0.51768106086365184</v>
+        <v>0.42288186157517899</v>
       </c>
       <c r="AB27" s="9">
         <f t="shared" si="5"/>
-        <v>0.45841683366733466</v>
+        <v>0.34600103644843672</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B28" s="2">
         <v>0</v>
@@ -3295,84 +3300,84 @@
         <v>0</v>
       </c>
       <c r="F28" s="2">
-        <v>6184</v>
+        <v>5503</v>
       </c>
       <c r="G28" s="2">
-        <v>6114</v>
-      </c>
-      <c r="H28" s="28">
-        <v>7182</v>
+        <v>4854</v>
+      </c>
+      <c r="H28" s="2">
+        <v>4356</v>
       </c>
       <c r="I28" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J28" s="2">
-        <v>19668</v>
+        <v>33412</v>
       </c>
       <c r="K28" s="2">
-        <v>13892</v>
+        <v>16707</v>
       </c>
       <c r="L28" s="2">
-        <v>13892</v>
+        <v>16707</v>
       </c>
       <c r="M28" s="2">
-        <v>10631</v>
+        <v>4807</v>
       </c>
       <c r="N28" s="2">
-        <v>3232</v>
+        <v>1572</v>
       </c>
       <c r="O28" s="1">
-        <v>1760</v>
+        <v>829</v>
       </c>
       <c r="P28" s="8">
         <f t="shared" si="0"/>
-        <v>1.7191138421733505</v>
+        <v>0.87352353261857174</v>
       </c>
       <c r="Q28" s="8">
         <f t="shared" si="1"/>
-        <v>0.52862283284265621</v>
+        <v>0.32385661310259578</v>
       </c>
       <c r="R28" s="8">
         <f t="shared" si="2"/>
-        <v>0.24505708716235031</v>
+        <v>0.19031221303948576</v>
       </c>
       <c r="S28" s="2">
         <v>0</v>
       </c>
       <c r="T28" s="2">
-        <v>13542</v>
+        <v>24184</v>
       </c>
       <c r="U28" s="2">
-        <v>6771</v>
+        <v>12092</v>
       </c>
       <c r="V28" s="2">
-        <v>6771</v>
+        <v>12097</v>
       </c>
       <c r="W28" s="2">
-        <v>10789</v>
+        <v>5023</v>
       </c>
       <c r="X28" s="2">
-        <v>3063</v>
+        <v>1584</v>
       </c>
       <c r="Y28" s="1">
-        <v>2086</v>
+        <v>1187</v>
       </c>
       <c r="Z28" s="8">
         <f t="shared" si="3"/>
-        <v>1.7446636481241915</v>
+        <v>0.91277485008177361</v>
       </c>
       <c r="AA28" s="9">
         <f t="shared" si="4"/>
-        <v>0.50098135426889112</v>
+        <v>0.32632880098887518</v>
       </c>
       <c r="AB28" s="9">
         <f t="shared" si="5"/>
-        <v>0.29044834307992201</v>
+        <v>0.27249770431588616</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B29" s="2">
         <v>0</v>
@@ -3387,84 +3392,84 @@
         <v>0</v>
       </c>
       <c r="F29" s="2">
-        <v>7230</v>
+        <v>8211</v>
       </c>
       <c r="G29" s="2">
-        <v>6475</v>
+        <v>7729</v>
       </c>
       <c r="H29" s="2">
-        <v>5604</v>
+        <v>6956</v>
       </c>
       <c r="I29" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J29" s="2">
-        <v>19670</v>
+        <v>3949</v>
       </c>
       <c r="K29" s="2">
-        <v>6992</v>
+        <v>4490</v>
       </c>
       <c r="L29" s="2">
-        <v>19670</v>
+        <v>4490</v>
       </c>
       <c r="M29" s="2">
-        <v>10276</v>
+        <v>4081</v>
       </c>
       <c r="N29" s="2">
-        <v>3171</v>
+        <v>2940</v>
       </c>
       <c r="O29" s="1">
-        <v>1765</v>
+        <v>1892</v>
       </c>
       <c r="P29" s="8">
         <f t="shared" si="0"/>
-        <v>1.4213001383125865</v>
+        <v>0.49701619778346123</v>
       </c>
       <c r="Q29" s="8">
         <f t="shared" si="1"/>
-        <v>0.48972972972972972</v>
+        <v>0.38038556087462805</v>
       </c>
       <c r="R29" s="8">
         <f t="shared" si="2"/>
-        <v>0.31495360456816557</v>
+        <v>0.2719953996549741</v>
       </c>
       <c r="S29" s="2">
         <v>0</v>
       </c>
       <c r="T29" s="2">
-        <v>13542</v>
+        <v>0</v>
       </c>
       <c r="U29" s="2">
         <v>0</v>
       </c>
       <c r="V29" s="2">
-        <v>13542</v>
+        <v>0</v>
       </c>
       <c r="W29" s="2">
-        <v>10376</v>
+        <v>4175</v>
       </c>
       <c r="X29" s="2">
-        <v>2925</v>
+        <v>3336</v>
       </c>
       <c r="Y29" s="1">
-        <v>1990</v>
+        <v>2212</v>
       </c>
       <c r="Z29" s="8">
         <f t="shared" si="3"/>
-        <v>1.4351313969571231</v>
+        <v>0.50846425526732431</v>
       </c>
       <c r="AA29" s="9">
         <f t="shared" si="4"/>
-        <v>0.45173745173745172</v>
+        <v>0.43162116703325137</v>
       </c>
       <c r="AB29" s="9">
         <f t="shared" si="5"/>
-        <v>0.35510349750178444</v>
+        <v>0.31799884991374355</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B30" s="2">
         <v>0</v>
@@ -3479,84 +3484,84 @@
         <v>0</v>
       </c>
       <c r="F30" s="2">
-        <v>5547</v>
+        <v>3124</v>
       </c>
       <c r="G30" s="2">
-        <v>5219</v>
-      </c>
-      <c r="H30" s="28">
-        <v>7375</v>
+        <v>2635</v>
+      </c>
+      <c r="H30" s="2">
+        <v>2478</v>
       </c>
       <c r="I30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" s="2">
-        <v>33412</v>
+        <v>1</v>
       </c>
       <c r="K30" s="2">
-        <v>16707</v>
+        <v>1</v>
       </c>
       <c r="L30" s="2">
-        <v>16707</v>
+        <v>1</v>
       </c>
       <c r="M30" s="2">
-        <v>5134</v>
+        <v>912</v>
       </c>
       <c r="N30" s="2">
-        <v>1740</v>
+        <v>578</v>
       </c>
       <c r="O30" s="1">
-        <v>803</v>
+        <v>266</v>
       </c>
       <c r="P30" s="8">
         <f t="shared" si="0"/>
-        <v>0.92554533982332787</v>
+        <v>0.29193341869398209</v>
       </c>
       <c r="Q30" s="8">
         <f t="shared" si="1"/>
-        <v>0.33339720252922017</v>
+        <v>0.21935483870967742</v>
       </c>
       <c r="R30" s="8">
         <f t="shared" si="2"/>
-        <v>0.10888135593220338</v>
+        <v>0.10734463276836158</v>
       </c>
       <c r="S30" s="2">
         <v>0</v>
       </c>
       <c r="T30" s="2">
-        <v>24184</v>
+        <v>0</v>
       </c>
       <c r="U30" s="2">
-        <v>12092</v>
+        <v>0</v>
       </c>
       <c r="V30" s="2">
-        <v>12097</v>
+        <v>0</v>
       </c>
       <c r="W30" s="2">
-        <v>5190</v>
+        <v>905</v>
       </c>
       <c r="X30" s="2">
-        <v>1717</v>
+        <v>652</v>
       </c>
       <c r="Y30" s="1">
-        <v>1170</v>
+        <v>379</v>
       </c>
       <c r="Z30" s="8">
         <f t="shared" si="3"/>
-        <v>0.93564088696592751</v>
+        <v>0.28969270166453265</v>
       </c>
       <c r="AA30" s="9">
         <f t="shared" si="4"/>
-        <v>0.3289902280130293</v>
+        <v>0.24743833017077799</v>
       </c>
       <c r="AB30" s="9">
         <f t="shared" si="5"/>
-        <v>0.15864406779661017</v>
+        <v>0.1529459241323648</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B31" s="2">
         <v>0</v>
@@ -3571,46 +3576,46 @@
         <v>0</v>
       </c>
       <c r="F31" s="2">
-        <v>8572</v>
+        <v>3895</v>
       </c>
       <c r="G31" s="2">
-        <v>7993</v>
-      </c>
-      <c r="H31" s="28">
-        <v>9052</v>
+        <v>3357</v>
+      </c>
+      <c r="H31" s="2">
+        <v>3044</v>
       </c>
       <c r="I31" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J31" s="2">
-        <v>3949</v>
+        <v>162</v>
       </c>
       <c r="K31" s="2">
-        <v>4490</v>
+        <v>3009</v>
       </c>
       <c r="L31" s="2">
-        <v>4490</v>
+        <v>3009</v>
       </c>
       <c r="M31" s="2">
-        <v>4500</v>
+        <v>1674</v>
       </c>
       <c r="N31" s="2">
-        <v>3138</v>
+        <v>1130</v>
       </c>
       <c r="O31" s="1">
-        <v>1850</v>
+        <v>585</v>
       </c>
       <c r="P31" s="8">
         <f t="shared" si="0"/>
-        <v>0.52496500233317778</v>
+        <v>0.42978177150192554</v>
       </c>
       <c r="Q31" s="8">
         <f t="shared" si="1"/>
-        <v>0.39259351932941322</v>
+        <v>0.3366100685135538</v>
       </c>
       <c r="R31" s="8">
         <f t="shared" si="2"/>
-        <v>0.20437472381794078</v>
+        <v>0.19218134034165571</v>
       </c>
       <c r="S31" s="2">
         <v>0</v>
@@ -3625,839 +3630,656 @@
         <v>0</v>
       </c>
       <c r="W31" s="2">
-        <v>4344</v>
+        <v>1832</v>
       </c>
       <c r="X31" s="2">
-        <v>3540</v>
+        <v>1309</v>
       </c>
       <c r="Y31" s="1">
-        <v>2186</v>
+        <v>811</v>
       </c>
       <c r="Z31" s="8">
         <f t="shared" si="3"/>
-        <v>0.50676621558562762</v>
+        <v>0.47034659820282415</v>
       </c>
       <c r="AA31" s="9">
         <f t="shared" si="4"/>
-        <v>0.44288752658576253</v>
+        <v>0.38993148644623177</v>
       </c>
       <c r="AB31" s="9">
         <f t="shared" si="5"/>
-        <v>0.24149359257622624</v>
+        <v>0.2664257555847569</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B32" s="2">
-        <v>0</v>
+        <v>238</v>
       </c>
       <c r="C32" s="2">
-        <v>0</v>
+        <v>218</v>
       </c>
       <c r="D32" s="2">
-        <v>0</v>
+        <v>203</v>
       </c>
       <c r="E32" s="2">
-        <v>0</v>
+        <v>203</v>
       </c>
       <c r="F32" s="2">
-        <v>3009</v>
+        <v>5526</v>
       </c>
       <c r="G32" s="2">
-        <v>2638</v>
+        <v>7380</v>
       </c>
       <c r="H32" s="2">
-        <v>2418</v>
+        <v>6171</v>
       </c>
       <c r="I32" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J32" s="2">
-        <v>1</v>
+        <v>28860</v>
       </c>
       <c r="K32" s="2">
-        <v>1</v>
+        <v>14432</v>
       </c>
       <c r="L32" s="2">
-        <v>1</v>
+        <v>14432</v>
       </c>
       <c r="M32" s="2">
-        <v>973</v>
+        <v>2060</v>
       </c>
       <c r="N32" s="2">
-        <v>603</v>
-      </c>
-      <c r="O32" s="1">
-        <v>259</v>
-      </c>
-      <c r="P32" s="8">
+        <v>1513</v>
+      </c>
+      <c r="O32" s="2">
+        <v>689</v>
+      </c>
+      <c r="P32" s="15">
         <f t="shared" si="0"/>
-        <v>0.32336324360252577</v>
-      </c>
-      <c r="Q32" s="8">
+        <v>0.37278320665942816</v>
+      </c>
+      <c r="Q32" s="15">
         <f t="shared" si="1"/>
-        <v>0.22858225928733888</v>
+        <v>0.20501355013550135</v>
       </c>
       <c r="R32" s="8">
         <f t="shared" si="2"/>
-        <v>0.10711331679073614</v>
+        <v>0.11165127207907957</v>
       </c>
       <c r="S32" s="2">
         <v>0</v>
       </c>
       <c r="T32" s="2">
-        <v>0</v>
+        <v>27728</v>
       </c>
       <c r="U32" s="2">
-        <v>0</v>
+        <v>13864</v>
       </c>
       <c r="V32" s="2">
-        <v>0</v>
+        <v>13864</v>
       </c>
       <c r="W32" s="2">
-        <v>903</v>
+        <v>2879</v>
       </c>
       <c r="X32" s="2">
-        <v>659</v>
-      </c>
-      <c r="Y32" s="1">
-        <v>383</v>
-      </c>
-      <c r="Z32" s="8">
+        <v>1730</v>
+      </c>
+      <c r="Y32" s="2">
+        <v>1152</v>
+      </c>
+      <c r="Z32" s="15">
         <f t="shared" si="3"/>
-        <v>0.30009970089730809</v>
-      </c>
-      <c r="AA32" s="9">
+        <v>0.52099167571480276</v>
+      </c>
+      <c r="AA32" s="16">
         <f t="shared" si="4"/>
-        <v>0.24981046247156938</v>
+        <v>0.23441734417344173</v>
       </c>
       <c r="AB32" s="9">
         <f t="shared" si="5"/>
-        <v>0.15839536807278742</v>
+        <v>0.18667963052989792</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B33" s="2">
-        <v>0</v>
+        <v>164</v>
       </c>
       <c r="C33" s="2">
-        <v>0</v>
+        <v>185</v>
       </c>
       <c r="D33" s="2">
-        <v>0</v>
+        <v>185</v>
       </c>
       <c r="E33" s="2">
-        <v>0</v>
+        <v>185</v>
       </c>
       <c r="F33" s="2">
-        <v>3975</v>
+        <v>5367</v>
       </c>
       <c r="G33" s="2">
-        <v>3351</v>
+        <v>7423</v>
       </c>
       <c r="H33" s="2">
-        <v>2983</v>
+        <v>6082</v>
       </c>
       <c r="I33" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J33" s="2">
-        <v>162</v>
+        <v>14454</v>
       </c>
       <c r="K33" s="2">
-        <v>3009</v>
+        <v>13053</v>
       </c>
       <c r="L33" s="2">
-        <v>3009</v>
+        <v>14454</v>
       </c>
       <c r="M33" s="2">
-        <v>1893</v>
+        <v>4775</v>
       </c>
       <c r="N33" s="2">
-        <v>1233</v>
-      </c>
-      <c r="O33" s="1">
-        <v>569</v>
-      </c>
-      <c r="P33" s="8">
+        <v>2549</v>
+      </c>
+      <c r="O33" s="2">
+        <v>1477</v>
+      </c>
+      <c r="P33" s="15">
         <f t="shared" si="0"/>
-        <v>0.47622641509433961</v>
-      </c>
-      <c r="Q33" s="8">
+        <v>0.88969629215576673</v>
+      </c>
+      <c r="Q33" s="15">
         <f t="shared" si="1"/>
-        <v>0.36794986571172783</v>
+        <v>0.34339215950424357</v>
       </c>
       <c r="R33" s="8">
         <f t="shared" si="2"/>
-        <v>0.19074756956084479</v>
+        <v>0.24284774745149623</v>
       </c>
       <c r="S33" s="2">
         <v>0</v>
       </c>
       <c r="T33" s="2">
-        <v>0</v>
+        <v>13867</v>
       </c>
       <c r="U33" s="2">
-        <v>0</v>
+        <v>11569</v>
       </c>
       <c r="V33" s="2">
-        <v>0</v>
+        <v>13867</v>
       </c>
       <c r="W33" s="2">
-        <v>1916</v>
+        <v>5244</v>
       </c>
       <c r="X33" s="2">
-        <v>1358</v>
-      </c>
-      <c r="Y33" s="1">
-        <v>802</v>
-      </c>
-      <c r="Z33" s="8">
+        <v>2865</v>
+      </c>
+      <c r="Y33" s="2">
+        <v>1907</v>
+      </c>
+      <c r="Z33" s="15">
         <f t="shared" si="3"/>
-        <v>0.48201257861635222</v>
-      </c>
-      <c r="AA33" s="9">
+        <v>0.97708216880939069</v>
+      </c>
+      <c r="AA33" s="16">
         <f t="shared" si="4"/>
-        <v>0.40525216353327365</v>
+        <v>0.38596254883470293</v>
       </c>
       <c r="AB33" s="9">
         <f t="shared" si="5"/>
-        <v>0.26885685551458266</v>
+        <v>0.31354817494245313</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B34" s="2">
-        <v>238</v>
+        <v>65536</v>
       </c>
       <c r="C34" s="2">
-        <v>218</v>
+        <v>65536</v>
       </c>
       <c r="D34" s="2">
-        <v>203</v>
+        <v>65536</v>
       </c>
       <c r="E34" s="2">
-        <v>203</v>
+        <v>65536</v>
       </c>
       <c r="F34" s="2">
-        <v>5447</v>
+        <v>22222</v>
       </c>
       <c r="G34" s="2">
-        <v>7387</v>
+        <v>22222</v>
       </c>
       <c r="H34" s="2">
-        <v>5973</v>
+        <v>22222</v>
       </c>
       <c r="I34" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J34" s="2">
-        <v>28860</v>
+        <v>5</v>
       </c>
       <c r="K34" s="2">
-        <v>14432</v>
+        <v>5</v>
       </c>
       <c r="L34" s="2">
-        <v>14432</v>
+        <v>6</v>
       </c>
       <c r="M34" s="2">
-        <v>2333</v>
+        <v>8838</v>
       </c>
       <c r="N34" s="2">
-        <v>1608</v>
+        <v>5658</v>
       </c>
       <c r="O34" s="2">
-        <v>668</v>
+        <v>3916</v>
       </c>
       <c r="P34" s="15">
         <f t="shared" si="0"/>
-        <v>0.42830916100605837</v>
+        <v>0.39771397713977141</v>
       </c>
       <c r="Q34" s="15">
         <f t="shared" si="1"/>
-        <v>0.21767970759442262</v>
+        <v>0.25461254612546125</v>
       </c>
       <c r="R34" s="8">
         <f t="shared" si="2"/>
-        <v>0.11183659802444333</v>
+        <v>0.17622176221762217</v>
       </c>
       <c r="S34" s="2">
         <v>0</v>
       </c>
       <c r="T34" s="2">
-        <v>27728</v>
+        <v>0</v>
       </c>
       <c r="U34" s="2">
-        <v>13864</v>
+        <v>0</v>
       </c>
       <c r="V34" s="2">
-        <v>13864</v>
+        <v>0</v>
       </c>
       <c r="W34" s="2">
-        <v>2897</v>
+        <v>9880</v>
       </c>
       <c r="X34" s="2">
-        <v>1759</v>
+        <v>7167</v>
       </c>
       <c r="Y34" s="2">
-        <v>1139</v>
+        <v>5196</v>
       </c>
       <c r="Z34" s="15">
         <f t="shared" si="3"/>
-        <v>0.53185239581420962</v>
+        <v>0.44460444604446042</v>
       </c>
       <c r="AA34" s="16">
         <f t="shared" si="4"/>
-        <v>0.23812102341952077</v>
+        <v>0.32251822518225182</v>
       </c>
       <c r="AB34" s="9">
         <f t="shared" si="5"/>
-        <v>0.19069144483509123</v>
+        <v>0.23382233822338222</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B35" s="2">
-        <v>164</v>
-      </c>
-      <c r="C35" s="2">
-        <v>185</v>
-      </c>
-      <c r="D35" s="2">
-        <v>185</v>
-      </c>
-      <c r="E35" s="2">
-        <v>185</v>
-      </c>
-      <c r="F35" s="2">
-        <v>5296</v>
-      </c>
-      <c r="G35" s="2">
-        <v>7450</v>
-      </c>
-      <c r="H35" s="2">
-        <v>5905</v>
-      </c>
-      <c r="I35" s="2">
+    <row r="35" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="11">
+        <v>65536</v>
+      </c>
+      <c r="C35" s="11">
+        <v>65536</v>
+      </c>
+      <c r="D35" s="11">
+        <v>65536</v>
+      </c>
+      <c r="E35" s="11">
+        <v>65536</v>
+      </c>
+      <c r="F35" s="11">
+        <v>22222</v>
+      </c>
+      <c r="G35" s="11">
+        <v>22222</v>
+      </c>
+      <c r="H35" s="11">
+        <v>22222</v>
+      </c>
+      <c r="I35" s="11">
         <v>2</v>
       </c>
-      <c r="J35" s="2">
-        <v>14454</v>
-      </c>
-      <c r="K35" s="2">
-        <v>13053</v>
-      </c>
-      <c r="L35" s="2">
-        <v>14454</v>
-      </c>
-      <c r="M35" s="2">
-        <v>4979</v>
-      </c>
-      <c r="N35" s="2">
-        <v>2652</v>
-      </c>
-      <c r="O35" s="2">
-        <v>1426</v>
-      </c>
-      <c r="P35" s="15">
+      <c r="J35" s="11">
+        <v>11169</v>
+      </c>
+      <c r="K35" s="11">
+        <v>1975</v>
+      </c>
+      <c r="L35" s="11">
+        <v>13140</v>
+      </c>
+      <c r="M35" s="11">
+        <v>9272</v>
+      </c>
+      <c r="N35" s="11">
+        <v>5035</v>
+      </c>
+      <c r="O35" s="11">
+        <v>3489</v>
+      </c>
+      <c r="P35" s="12">
         <f t="shared" si="0"/>
-        <v>0.94014350453172202</v>
-      </c>
-      <c r="Q35" s="15">
+        <v>0.4172441724417244</v>
+      </c>
+      <c r="Q35" s="12">
         <f t="shared" si="1"/>
-        <v>0.35597315436241611</v>
-      </c>
-      <c r="R35" s="8">
+        <v>0.22657726577265772</v>
+      </c>
+      <c r="R35" s="12">
         <f t="shared" si="2"/>
-        <v>0.24149026248941574</v>
-      </c>
-      <c r="S35" s="2">
-        <v>0</v>
-      </c>
-      <c r="T35" s="2">
-        <v>13867</v>
-      </c>
-      <c r="U35" s="2">
-        <v>11569</v>
-      </c>
-      <c r="V35" s="2">
-        <v>13867</v>
-      </c>
-      <c r="W35" s="2">
-        <v>5292</v>
-      </c>
-      <c r="X35" s="2">
-        <v>3064</v>
-      </c>
-      <c r="Y35" s="2">
-        <v>1870</v>
-      </c>
-      <c r="Z35" s="15">
+        <v>0.15700657006570065</v>
+      </c>
+      <c r="S35" s="11">
+        <v>0</v>
+      </c>
+      <c r="T35" s="11">
+        <v>8867</v>
+      </c>
+      <c r="U35" s="11">
+        <v>927</v>
+      </c>
+      <c r="V35" s="11">
+        <v>9794</v>
+      </c>
+      <c r="W35" s="11">
+        <v>22618</v>
+      </c>
+      <c r="X35" s="11">
+        <v>15505</v>
+      </c>
+      <c r="Y35" s="11">
+        <v>11068</v>
+      </c>
+      <c r="Z35" s="12">
         <f t="shared" si="3"/>
-        <v>0.99924471299093653</v>
-      </c>
-      <c r="AA35" s="16">
+        <v>1.0178201782017819</v>
+      </c>
+      <c r="AA35" s="13">
         <f t="shared" si="4"/>
-        <v>0.41127516778523487</v>
-      </c>
-      <c r="AB35" s="9">
+        <v>0.69773197731977321</v>
+      </c>
+      <c r="AB35" s="13">
         <f t="shared" si="5"/>
-        <v>0.31668077900084673</v>
+        <v>0.49806498064980648</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B36" s="2">
-        <v>65536</v>
-      </c>
-      <c r="C36" s="2">
-        <v>65536</v>
-      </c>
-      <c r="D36" s="2">
-        <v>65536</v>
-      </c>
-      <c r="E36" s="2">
-        <v>65536</v>
-      </c>
-      <c r="F36" s="2">
-        <v>22222</v>
-      </c>
-      <c r="G36" s="2">
-        <v>22222</v>
-      </c>
-      <c r="H36" s="2">
-        <v>22222</v>
-      </c>
-      <c r="I36" s="2">
-        <v>6</v>
-      </c>
-      <c r="J36" s="2">
-        <v>5</v>
-      </c>
-      <c r="K36" s="2">
-        <v>5</v>
-      </c>
-      <c r="L36" s="2">
-        <v>6</v>
-      </c>
-      <c r="M36" s="2">
-        <v>9084</v>
-      </c>
-      <c r="N36" s="2">
-        <v>5827</v>
-      </c>
-      <c r="O36" s="2">
-        <v>3771</v>
-      </c>
-      <c r="P36" s="15">
-        <f t="shared" si="0"/>
-        <v>0.40878408784087839</v>
-      </c>
-      <c r="Q36" s="15">
-        <f t="shared" si="1"/>
-        <v>0.26221762217622174</v>
-      </c>
-      <c r="R36" s="8">
-        <f t="shared" si="2"/>
-        <v>0.16969669696696968</v>
-      </c>
-      <c r="S36" s="2">
-        <v>0</v>
-      </c>
-      <c r="T36" s="2">
-        <v>0</v>
-      </c>
-      <c r="U36" s="2">
-        <v>0</v>
-      </c>
-      <c r="V36" s="2">
-        <v>0</v>
-      </c>
-      <c r="W36" s="2">
-        <v>9800</v>
-      </c>
-      <c r="X36" s="2">
-        <v>7285</v>
-      </c>
-      <c r="Y36" s="2">
-        <v>5126</v>
-      </c>
-      <c r="Z36" s="15">
-        <f t="shared" si="3"/>
-        <v>0.44100441004410046</v>
-      </c>
-      <c r="AA36" s="16">
-        <f t="shared" si="4"/>
-        <v>0.32782827828278283</v>
-      </c>
-      <c r="AB36" s="9">
-        <f t="shared" si="5"/>
-        <v>0.23067230672306724</v>
-      </c>
-    </row>
-    <row r="37" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B37" s="11">
-        <v>65536</v>
-      </c>
-      <c r="C37" s="11">
-        <v>65536</v>
-      </c>
-      <c r="D37" s="11">
-        <v>65536</v>
-      </c>
-      <c r="E37" s="11">
-        <v>65536</v>
-      </c>
-      <c r="F37" s="11">
-        <v>22222</v>
-      </c>
-      <c r="G37" s="11">
-        <v>22222</v>
-      </c>
-      <c r="H37" s="11">
-        <v>22222</v>
-      </c>
-      <c r="I37" s="11">
-        <v>2</v>
-      </c>
-      <c r="J37" s="11">
-        <v>11169</v>
-      </c>
-      <c r="K37" s="11">
-        <v>1975</v>
-      </c>
-      <c r="L37" s="11">
-        <v>13140</v>
-      </c>
-      <c r="M37" s="11">
-        <v>9598</v>
-      </c>
-      <c r="N37" s="11">
-        <v>5366</v>
-      </c>
-      <c r="O37" s="11">
-        <v>3366</v>
-      </c>
-      <c r="P37" s="12">
-        <f t="shared" si="0"/>
-        <v>0.43191431914319145</v>
-      </c>
-      <c r="Q37" s="12">
-        <f t="shared" si="1"/>
-        <v>0.24147241472414724</v>
-      </c>
-      <c r="R37" s="12">
-        <f t="shared" si="2"/>
-        <v>0.15147151471514717</v>
-      </c>
-      <c r="S37" s="11">
-        <v>0</v>
-      </c>
-      <c r="T37" s="11">
-        <v>8867</v>
-      </c>
-      <c r="U37" s="11">
-        <v>927</v>
-      </c>
-      <c r="V37" s="11">
-        <v>9794</v>
-      </c>
-      <c r="W37" s="11">
-        <v>22644</v>
-      </c>
-      <c r="X37" s="11">
-        <v>15498</v>
-      </c>
-      <c r="Y37" s="11">
-        <v>10750</v>
-      </c>
-      <c r="Z37" s="12">
-        <f t="shared" si="3"/>
-        <v>1.0189901899018989</v>
-      </c>
-      <c r="AA37" s="13">
-        <f t="shared" si="4"/>
-        <v>0.69741697416974169</v>
-      </c>
-      <c r="AB37" s="13">
-        <f t="shared" si="5"/>
-        <v>0.4837548375483755</v>
-      </c>
-    </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A38" s="22" t="s">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A36" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="25">
+      <c r="B36" s="25">
         <f>COUNTIF(B2:B5,"=0")/4</f>
         <v>1</v>
       </c>
-      <c r="C38" s="25">
-        <f t="shared" ref="C38:E38" si="6">COUNTIF(C2:C5,"=0")/4</f>
+      <c r="C36" s="25">
+        <f>COUNTIF(C2:C5,"=0")/4</f>
         <v>1</v>
       </c>
-      <c r="D38" s="25">
-        <f t="shared" si="6"/>
+      <c r="D36" s="25">
+        <f>COUNTIF(D2:D5,"=0")/4</f>
         <v>1</v>
       </c>
-      <c r="E38" s="25">
-        <f t="shared" si="6"/>
+      <c r="E36" s="25">
+        <f>COUNTIF(E2:E5,"=0")/4</f>
         <v>1</v>
       </c>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="25">
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="25">
         <f>COUNTIF(I2:I5,"=0")/4</f>
         <v>1</v>
       </c>
-      <c r="J38" s="25">
-        <f t="shared" ref="J38:L38" si="7">COUNTIF(J2:J5,"=0")/4</f>
+      <c r="J36" s="25">
+        <f>COUNTIF(J2:J5,"=0")/4</f>
         <v>0.5</v>
       </c>
-      <c r="K38" s="25">
-        <f t="shared" si="7"/>
+      <c r="K36" s="25">
+        <f>COUNTIF(K2:K5,"=0")/4</f>
         <v>0.5</v>
       </c>
-      <c r="L38" s="25">
-        <f t="shared" si="7"/>
+      <c r="L36" s="25">
+        <f>COUNTIF(L2:L5,"=0")/4</f>
         <v>0.5</v>
       </c>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="17">
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="17">
         <f>AVERAGE(P2:P5)</f>
-        <v>0.78928691016725028</v>
-      </c>
-      <c r="Q38" s="17">
+        <v>0.68902828322313658</v>
+      </c>
+      <c r="Q36" s="17">
         <f>AVERAGE(Q2:Q5)</f>
-        <v>0.74151179774319675</v>
-      </c>
-      <c r="R38" s="17">
+        <v>0.78598285971147119</v>
+      </c>
+      <c r="R36" s="17">
         <f>AVERAGE(R2:R5)</f>
-        <v>0.14808930291674494</v>
-      </c>
-      <c r="S38" s="25">
+        <v>0.14635916470125376</v>
+      </c>
+      <c r="S36" s="25">
         <f>COUNTIF(S2:S5,"=0")/4</f>
         <v>1</v>
       </c>
-      <c r="T38" s="25">
-        <f t="shared" ref="T38:V38" si="8">COUNTIF(T2:T5,"=0")/4</f>
+      <c r="T36" s="25">
+        <f>COUNTIF(T2:T5,"=0")/4</f>
         <v>1</v>
       </c>
-      <c r="U38" s="25">
-        <f t="shared" si="8"/>
+      <c r="U36" s="25">
+        <f>COUNTIF(U2:U5,"=0")/4</f>
         <v>1</v>
       </c>
-      <c r="V38" s="25">
-        <f t="shared" si="8"/>
+      <c r="V36" s="25">
+        <f>COUNTIF(V2:V5,"=0")/4</f>
         <v>1</v>
       </c>
-      <c r="W38" s="1"/>
-      <c r="X38" s="1"/>
-      <c r="Y38" s="1"/>
-      <c r="Z38" s="17">
+      <c r="W36" s="1"/>
+      <c r="X36" s="1"/>
+      <c r="Y36" s="1"/>
+      <c r="Z36" s="17">
         <f>AVERAGE(Z2:Z5)</f>
-        <v>1.376890141406921</v>
-      </c>
-      <c r="AA38" s="18">
+        <v>1.3047276873465157</v>
+      </c>
+      <c r="AA36" s="18">
         <f>AVERAGE(AA2:AA5)</f>
-        <v>0.96695974573752319</v>
-      </c>
-      <c r="AB38" s="18">
+        <v>0.91813992805453881</v>
+      </c>
+      <c r="AB36" s="18">
         <f>AVERAGE(AB2:AB5)</f>
-        <v>0.72452141642573398</v>
+        <v>0.63977984904697816</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A39" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="B39" s="26">
-        <f>COUNTIF(B6:B37,"=0")/COUNTA(B6:B37)</f>
-        <v>0.75</v>
-      </c>
-      <c r="C39" s="26">
-        <f t="shared" ref="C39:E39" si="9">COUNTIF(C6:C37,"=0")/COUNTA(C6:C37)</f>
-        <v>0.75</v>
-      </c>
-      <c r="D39" s="26">
-        <f t="shared" si="9"/>
-        <v>0.75</v>
-      </c>
-      <c r="E39" s="26">
-        <f t="shared" si="9"/>
-        <v>0.75</v>
-      </c>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="26">
-        <f>COUNTIF(I6:I37,"=0")/COUNTA(I6:I37)</f>
-        <v>0.25</v>
-      </c>
-      <c r="J39" s="26">
-        <f t="shared" ref="J39:L39" si="10">COUNTIF(J6:J37,"=0")/COUNTA(J6:J37)</f>
-        <v>0.1875</v>
-      </c>
-      <c r="K39" s="26">
-        <f t="shared" si="10"/>
-        <v>0.1875</v>
-      </c>
-      <c r="L39" s="26">
-        <f t="shared" si="10"/>
-        <v>0.15625</v>
-      </c>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="19">
-        <f>AVERAGE(P6:P37)</f>
-        <v>0.78772492137449757</v>
-      </c>
-      <c r="Q39" s="19">
-        <f t="shared" ref="Q39:R39" si="11">AVERAGE(Q6:Q37)</f>
-        <v>0.45382435758114942</v>
-      </c>
-      <c r="R39" s="19" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S39" s="26">
-        <f>COUNTIF(S6:S37,"=0")/COUNTA(S6:S37)</f>
-        <v>0.9375</v>
-      </c>
-      <c r="T39" s="26">
-        <f t="shared" ref="T39:V39" si="12">COUNTIF(T6:T37,"=0")/COUNTA(T6:T37)</f>
-        <v>0.65625</v>
-      </c>
-      <c r="U39" s="26">
-        <f t="shared" si="12"/>
-        <v>0.6875</v>
-      </c>
-      <c r="V39" s="26">
-        <f t="shared" si="12"/>
-        <v>0.65625</v>
-      </c>
-      <c r="W39" s="2"/>
-      <c r="X39" s="2"/>
-      <c r="Y39" s="2"/>
-      <c r="Z39" s="19">
-        <f>AVERAGE(Z6:Z37)</f>
-        <v>0.92237598728400461</v>
-      </c>
-      <c r="AA39" s="19">
-        <f t="shared" ref="AA39:AB39" si="13">AVERAGE(AA6:AA37)</f>
-        <v>0.49222592477376426</v>
-      </c>
-      <c r="AB39" s="19" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A37" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="26">
+        <f>COUNTIF(B6:B35,"=0")/COUNTA(B6:B35)</f>
+        <v>0.73333333333333328</v>
+      </c>
+      <c r="C37" s="26">
+        <f>COUNTIF(C6:C35,"=0")/COUNTA(C6:C35)</f>
+        <v>0.73333333333333328</v>
+      </c>
+      <c r="D37" s="26">
+        <f>COUNTIF(D6:D35,"=0")/COUNTA(D6:D35)</f>
+        <v>0.73333333333333328</v>
+      </c>
+      <c r="E37" s="26">
+        <f>COUNTIF(E6:E35,"=0")/COUNTA(E6:E35)</f>
+        <v>0.73333333333333328</v>
+      </c>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="26">
+        <f>COUNTIF(I6:I35,"=0")/COUNTA(I6:I35)</f>
+        <v>0.2</v>
+      </c>
+      <c r="J37" s="26">
+        <f>COUNTIF(J6:J35,"=0")/COUNTA(J6:J35)</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="K37" s="26">
+        <f>COUNTIF(K6:K35,"=0")/COUNTA(K6:K35)</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="L37" s="26">
+        <f>COUNTIF(L6:L35,"=0")/COUNTA(L6:L35)</f>
+        <v>0.1</v>
+      </c>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="19">
+        <f>AVERAGE(P6:P35)</f>
+        <v>0.5456603592289937</v>
+      </c>
+      <c r="Q37" s="19">
+        <f>AVERAGE(Q6:Q35)</f>
+        <v>0.35372552996834677</v>
+      </c>
+      <c r="R37" s="19">
+        <f>AVERAGE(R6:R35)</f>
+        <v>0.24373037430788613</v>
+      </c>
+      <c r="S37" s="26">
+        <f>COUNTIF(S6:S35,"=0")/COUNTA(S6:S35)</f>
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="T37" s="26">
+        <f>COUNTIF(T6:T35,"=0")/COUNTA(T6:T35)</f>
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="U37" s="26">
+        <f>COUNTIF(U6:U35,"=0")/COUNTA(U6:U35)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="V37" s="26">
+        <f>COUNTIF(V6:V35,"=0")/COUNTA(V6:V35)</f>
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="W37" s="2"/>
+      <c r="X37" s="2"/>
+      <c r="Y37" s="2"/>
+      <c r="Z37" s="19">
+        <f>AVERAGE(Z6:Z35)</f>
+        <v>0.71778563008164098</v>
+      </c>
+      <c r="AA37" s="19">
+        <f>AVERAGE(AA6:AA35)</f>
+        <v>0.40881175468947878</v>
+      </c>
+      <c r="AB37" s="28">
+        <f>AVERAGE(AB6:AB35)</f>
+        <v>0.33238453217148878</v>
+      </c>
+      <c r="AC37" s="29"/>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A40" s="24" t="s">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A38" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="B40" s="27">
-        <f>COUNTIF(B2:B37,"=0")/COUNTA(B2:B37)</f>
-        <v>0.77777777777777779</v>
-      </c>
-      <c r="C40" s="27">
-        <f t="shared" ref="C40:E40" si="14">COUNTIF(C2:C37,"=0")/COUNTA(C2:C37)</f>
-        <v>0.77777777777777779</v>
-      </c>
-      <c r="D40" s="27">
-        <f t="shared" si="14"/>
-        <v>0.77777777777777779</v>
-      </c>
-      <c r="E40" s="27">
-        <f t="shared" si="14"/>
-        <v>0.77777777777777779</v>
-      </c>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="27">
-        <f>COUNTIF(I2:I37,"=0")/COUNTA(I2:I37)</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="J40" s="27">
-        <f t="shared" ref="J40:L40" si="15">COUNTIF(J2:J37,"=0")/COUNTA(J2:J37)</f>
-        <v>0.22222222222222221</v>
-      </c>
-      <c r="K40" s="27">
-        <f t="shared" si="15"/>
-        <v>0.22222222222222221</v>
-      </c>
-      <c r="L40" s="27">
-        <f t="shared" si="15"/>
-        <v>0.19444444444444445</v>
-      </c>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
-      <c r="P40" s="20">
-        <f>AVERAGE(P2:P37)</f>
-        <v>0.78789847568480342</v>
-      </c>
-      <c r="Q40" s="20">
-        <f>AVERAGE(Q2:Q37)</f>
-        <v>0.48578962871026593</v>
-      </c>
-      <c r="R40" s="20" t="e">
-        <f>AVERAGE(R2:R37)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S40" s="27">
-        <f>COUNTIF(S2:S37,"=0")/COUNTA(S2:S37)</f>
-        <v>0.94444444444444442</v>
-      </c>
-      <c r="T40" s="27">
-        <f t="shared" ref="T40:V40" si="16">COUNTIF(T2:T37,"=0")/COUNTA(T2:T37)</f>
-        <v>0.69444444444444442</v>
-      </c>
-      <c r="U40" s="27">
-        <f t="shared" si="16"/>
-        <v>0.72222222222222221</v>
-      </c>
-      <c r="V40" s="27">
-        <f t="shared" si="16"/>
-        <v>0.69444444444444442</v>
-      </c>
-      <c r="W40" s="14"/>
-      <c r="X40" s="14"/>
-      <c r="Y40" s="14"/>
-      <c r="Z40" s="20">
-        <f>AVERAGE(Z2:Z37)</f>
-        <v>0.97287755996432879</v>
-      </c>
-      <c r="AA40" s="21">
-        <f>AVERAGE(AA2:AA37)</f>
-        <v>0.5449741271030708</v>
-      </c>
-      <c r="AB40" s="21" t="e">
-        <f>AVERAGE(AB2:AB37)</f>
-        <v>#DIV/0!</v>
+      <c r="B38" s="27">
+        <f>COUNTIF(B2:B35,"=0")/COUNTA(B2:B35)</f>
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="C38" s="27">
+        <f>COUNTIF(C2:C35,"=0")/COUNTA(C2:C35)</f>
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="D38" s="27">
+        <f>COUNTIF(D2:D35,"=0")/COUNTA(D2:D35)</f>
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="E38" s="27">
+        <f>COUNTIF(E2:E35,"=0")/COUNTA(E2:E35)</f>
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="27">
+        <f>COUNTIF(I2:I35,"=0")/COUNTA(I2:I35)</f>
+        <v>0.29411764705882354</v>
+      </c>
+      <c r="J38" s="27">
+        <f>COUNTIF(J2:J35,"=0")/COUNTA(J2:J35)</f>
+        <v>0.17647058823529413</v>
+      </c>
+      <c r="K38" s="27">
+        <f>COUNTIF(K2:K35,"=0")/COUNTA(K2:K35)</f>
+        <v>0.17647058823529413</v>
+      </c>
+      <c r="L38" s="27">
+        <f>COUNTIF(L2:L35,"=0")/COUNTA(L2:L35)</f>
+        <v>0.14705882352941177</v>
+      </c>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="20">
+        <f>AVERAGE(P2:P35)</f>
+        <v>0.56252717381653994</v>
+      </c>
+      <c r="Q38" s="20">
+        <f>AVERAGE(Q2:Q35)</f>
+        <v>0.40457933346753783</v>
+      </c>
+      <c r="R38" s="20">
+        <f>AVERAGE(R2:R35)</f>
+        <v>0.23227493788357645</v>
+      </c>
+      <c r="S38" s="27">
+        <f>COUNTIF(S2:S35,"=0")/COUNTA(S2:S35)</f>
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="T38" s="27">
+        <f>COUNTIF(T2:T35,"=0")/COUNTA(T2:T35)</f>
+        <v>0.67647058823529416</v>
+      </c>
+      <c r="U38" s="27">
+        <f>COUNTIF(U2:U35,"=0")/COUNTA(U2:U35)</f>
+        <v>0.70588235294117652</v>
+      </c>
+      <c r="V38" s="27">
+        <f>COUNTIF(V2:V35,"=0")/COUNTA(V2:V35)</f>
+        <v>0.67647058823529416</v>
+      </c>
+      <c r="W38" s="14"/>
+      <c r="X38" s="14"/>
+      <c r="Y38" s="14"/>
+      <c r="Z38" s="20">
+        <f>AVERAGE(Z2:Z35)</f>
+        <v>0.78683763681868479</v>
+      </c>
+      <c r="AA38" s="21">
+        <f>AVERAGE(AA2:AA35)</f>
+        <v>0.46873271626183882</v>
+      </c>
+      <c r="AB38" s="21">
+        <f>AVERAGE(AB2:AB35)</f>
+        <v>0.36854868709801691</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="P2:R40 Z2:AB40">
+  <conditionalFormatting sqref="P2:R38 Z2:AB38">
     <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4483,7 +4305,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:E8 B19:E20 B27:E27 I6:L8 I19:L20 I27:L27 S6:V8 S19:V20 S27:V27">
+  <conditionalFormatting sqref="B17:E18 B25:E25 I17:L18 I25:L25 S17:V18 S25:V25 B6:E6 I6:L6 S6:V6">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -4495,7 +4317,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B10:E18 I10:L18 S10:V18 B21:E26 I21:L26 S21:V26 I28:L37 S28:V37 B28:E37">
+  <conditionalFormatting sqref="B8:E16 I8:L16 S8:V16 B19:E24 I19:L24 S19:V24 I26:L35 S26:V35 B26:E35">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -4507,7 +4329,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B38:E40 I38:L40 S38:V40">
+  <conditionalFormatting sqref="B36:E38 I36:L38 S36:V38">
     <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4521,7 +4343,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9:E9 I9:L9 S9:V9">
+  <conditionalFormatting sqref="B7:E7 I7:L7 S7:V7">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -4536,8 +4358,8 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B38 S38:V38 F40:G40 C38:G38 M40:N40 I38:N38 P40:Q40 P38:Q38 F39:G39 B39:E39 M39:N39 I39:L39 S39:V39" formulaRange="1"/>
-    <ignoredError sqref="R10:R37 AB10:AB37 AB2:AB5 R2:R5" evalError="1"/>
+    <ignoredError sqref="B36 S36:V36 F38:G38 C36:G36 M38:N38 I36:N36 P38:Q38 P36:Q36 F37:G37 B37:E37 M37:N37 I37:L37 S37:V37" formulaRange="1"/>
+    <ignoredError sqref="R8:R35 AB8:AB35 AB2:AB5 R2:R5" evalError="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -4555,7 +4377,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>P2:R40 Z2:AB40</xm:sqref>
+          <xm:sqref>P2:R38 Z2:AB38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{D4AEBDF6-16F3-4574-8AF5-06B7A23DFE16}">
@@ -4570,7 +4392,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>B38:E40 I38:L40 S38:V40</xm:sqref>
+          <xm:sqref>B36:E38 I36:L38 S36:V38</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Extended constexpr support to comparison and classification functions.
git-svn-id: https://svn.code.sf.net/p/half/code/branches/clean@378 ba856b29-48f5-46b1-a3e5-b459205bce89
</commit_message>
<xml_diff>
--- a/test/results.xlsx
+++ b/test/results.xlsx
@@ -1282,7 +1282,7 @@
         <v>763</v>
       </c>
       <c r="H6" s="2">
-        <v>596</v>
+        <v>589</v>
       </c>
       <c r="I6" s="2">
         <v>0</v>
@@ -1303,7 +1303,7 @@
         <v>574</v>
       </c>
       <c r="O6" s="1">
-        <v>493</v>
+        <v>262</v>
       </c>
       <c r="P6" s="8">
         <f t="shared" si="0"/>
@@ -1315,7 +1315,7 @@
       </c>
       <c r="R6" s="8">
         <f t="shared" si="2"/>
-        <v>0.82718120805369133</v>
+        <v>0.44482173174872663</v>
       </c>
       <c r="S6" s="2">
         <v>0</v>
@@ -1336,7 +1336,7 @@
         <v>647</v>
       </c>
       <c r="Y6" s="1">
-        <v>642</v>
+        <v>372</v>
       </c>
       <c r="Z6" s="8">
         <f t="shared" si="3"/>
@@ -1348,7 +1348,7 @@
       </c>
       <c r="AB6" s="9">
         <f t="shared" si="5"/>
-        <v>1.0771812080536913</v>
+        <v>0.63157894736842102</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -4157,7 +4157,7 @@
       </c>
       <c r="R37" s="19">
         <f>AVERAGE(R6:R35)</f>
-        <v>0.24373037430788613</v>
+        <v>0.23098505843105394</v>
       </c>
       <c r="S37" s="26">
         <f>COUNTIF(S6:S35,"=0")/COUNTA(S6:S35)</f>
@@ -4188,7 +4188,7 @@
       </c>
       <c r="AB37" s="28">
         <f>AVERAGE(AB6:AB35)</f>
-        <v>0.33238453217148878</v>
+        <v>0.31753112348197976</v>
       </c>
       <c r="AC37" s="29"/>
     </row>
@@ -4244,7 +4244,7 @@
       </c>
       <c r="R38" s="20">
         <f>AVERAGE(R2:R35)</f>
-        <v>0.23227493788357645</v>
+        <v>0.22102907093343044</v>
       </c>
       <c r="S38" s="27">
         <f>COUNTIF(S2:S35,"=0")/COUNTA(S2:S35)</f>
@@ -4275,7 +4275,7 @@
       </c>
       <c r="AB38" s="21">
         <f>AVERAGE(AB2:AB35)</f>
-        <v>0.36854868709801691</v>
+        <v>0.35544273825433254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved performance of asin, tanh and atanh functions.
git-svn-id: https://svn.code.sf.net/p/half/code/branches/clean@379 ba856b29-48f5-46b1-a3e5-b459205bce89
</commit_message>
<xml_diff>
--- a/test/results.xlsx
+++ b/test/results.xlsx
@@ -217,7 +217,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,13 +240,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="16">
@@ -445,11 +457,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -480,8 +493,10 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -2748,12 +2763,12 @@
         <v>0</v>
       </c>
       <c r="F22" s="2">
-        <v>3965</v>
+        <v>1531</v>
       </c>
       <c r="G22" s="2">
-        <v>3808</v>
-      </c>
-      <c r="H22" s="2">
+        <v>1468</v>
+      </c>
+      <c r="H22" s="30">
         <v>2940</v>
       </c>
       <c r="I22" s="2">
@@ -2769,21 +2784,21 @@
         <v>4057</v>
       </c>
       <c r="M22" s="2">
-        <v>699</v>
+        <v>704</v>
       </c>
       <c r="N22" s="2">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="O22" s="1">
         <v>310</v>
       </c>
       <c r="P22" s="8">
         <f t="shared" si="0"/>
-        <v>0.17629255989911727</v>
+        <v>0.45983017635532331</v>
       </c>
       <c r="Q22" s="8">
         <f t="shared" si="1"/>
-        <v>0.17804621848739496</v>
+        <v>0.46253405994550406</v>
       </c>
       <c r="R22" s="8">
         <f t="shared" si="2"/>
@@ -2802,21 +2817,21 @@
         <v>0</v>
       </c>
       <c r="W22" s="2">
-        <v>942</v>
+        <v>1025</v>
       </c>
       <c r="X22" s="2">
-        <v>785</v>
+        <v>837</v>
       </c>
       <c r="Y22" s="1">
         <v>557</v>
       </c>
       <c r="Z22" s="8">
         <f t="shared" si="3"/>
-        <v>0.23757881462799496</v>
+        <v>0.66949706074461135</v>
       </c>
       <c r="AA22" s="9">
         <f t="shared" si="4"/>
-        <v>0.20614495798319327</v>
+        <v>0.57016348773841963</v>
       </c>
       <c r="AB22" s="9">
         <f t="shared" si="5"/>
@@ -3300,12 +3315,12 @@
         <v>0</v>
       </c>
       <c r="F28" s="2">
-        <v>5503</v>
+        <v>2833</v>
       </c>
       <c r="G28" s="2">
-        <v>4854</v>
-      </c>
-      <c r="H28" s="2">
+        <v>2602</v>
+      </c>
+      <c r="H28" s="30">
         <v>4356</v>
       </c>
       <c r="I28" s="2">
@@ -3321,21 +3336,21 @@
         <v>16707</v>
       </c>
       <c r="M28" s="2">
-        <v>4807</v>
+        <v>4762</v>
       </c>
       <c r="N28" s="2">
-        <v>1572</v>
+        <v>1585</v>
       </c>
       <c r="O28" s="1">
         <v>829</v>
       </c>
       <c r="P28" s="8">
         <f t="shared" si="0"/>
-        <v>0.87352353261857174</v>
+        <v>1.6809036357218496</v>
       </c>
       <c r="Q28" s="8">
         <f t="shared" si="1"/>
-        <v>0.32385661310259578</v>
+        <v>0.60914681014604155</v>
       </c>
       <c r="R28" s="8">
         <f t="shared" si="2"/>
@@ -3354,21 +3369,21 @@
         <v>12097</v>
       </c>
       <c r="W28" s="2">
-        <v>5023</v>
+        <v>5005</v>
       </c>
       <c r="X28" s="2">
-        <v>1584</v>
+        <v>1648</v>
       </c>
       <c r="Y28" s="1">
         <v>1187</v>
       </c>
       <c r="Z28" s="8">
         <f t="shared" si="3"/>
-        <v>0.91277485008177361</v>
+        <v>1.7666784327567948</v>
       </c>
       <c r="AA28" s="9">
         <f t="shared" si="4"/>
-        <v>0.32632880098887518</v>
+        <v>0.63335895465026903</v>
       </c>
       <c r="AB28" s="9">
         <f t="shared" si="5"/>
@@ -3576,12 +3591,12 @@
         <v>0</v>
       </c>
       <c r="F31" s="2">
-        <v>3895</v>
+        <v>1632</v>
       </c>
       <c r="G31" s="2">
-        <v>3357</v>
-      </c>
-      <c r="H31" s="2">
+        <v>1428</v>
+      </c>
+      <c r="H31" s="30">
         <v>3044</v>
       </c>
       <c r="I31" s="2">
@@ -3597,21 +3612,21 @@
         <v>3009</v>
       </c>
       <c r="M31" s="2">
-        <v>1674</v>
+        <v>1679</v>
       </c>
       <c r="N31" s="2">
-        <v>1130</v>
+        <v>1147</v>
       </c>
       <c r="O31" s="1">
         <v>585</v>
       </c>
       <c r="P31" s="8">
         <f t="shared" si="0"/>
-        <v>0.42978177150192554</v>
+        <v>1.0287990196078431</v>
       </c>
       <c r="Q31" s="8">
         <f t="shared" si="1"/>
-        <v>0.3366100685135538</v>
+        <v>0.8032212885154062</v>
       </c>
       <c r="R31" s="8">
         <f t="shared" si="2"/>
@@ -3630,21 +3645,21 @@
         <v>0</v>
       </c>
       <c r="W31" s="2">
-        <v>1832</v>
+        <v>1830</v>
       </c>
       <c r="X31" s="2">
-        <v>1309</v>
+        <v>1318</v>
       </c>
       <c r="Y31" s="1">
         <v>811</v>
       </c>
       <c r="Z31" s="8">
         <f t="shared" si="3"/>
-        <v>0.47034659820282415</v>
+        <v>1.1213235294117647</v>
       </c>
       <c r="AA31" s="9">
         <f t="shared" si="4"/>
-        <v>0.38993148644623177</v>
+        <v>0.92296918767507008</v>
       </c>
       <c r="AB31" s="9">
         <f t="shared" si="5"/>
@@ -4149,11 +4164,11 @@
       <c r="O37" s="2"/>
       <c r="P37" s="19">
         <f>AVERAGE(P6:P35)</f>
-        <v>0.5456603592289937</v>
+        <v>0.60199152481784046</v>
       </c>
       <c r="Q37" s="19">
         <f>AVERAGE(Q6:Q35)</f>
-        <v>0.35372552996834677</v>
+        <v>0.38827183858512698</v>
       </c>
       <c r="R37" s="19">
         <f>AVERAGE(R6:R35)</f>
@@ -4180,11 +4195,11 @@
       <c r="Y37" s="2"/>
       <c r="Z37" s="19">
         <f>AVERAGE(Z6:Z35)</f>
-        <v>0.71778563008164098</v>
+        <v>0.78234558874832694</v>
       </c>
       <c r="AA37" s="19">
         <f>AVERAGE(AA6:AA35)</f>
-        <v>0.40881175468947878</v>
+        <v>0.44894796751099408</v>
       </c>
       <c r="AB37" s="28">
         <f>AVERAGE(AB6:AB35)</f>
@@ -4236,11 +4251,11 @@
       <c r="O38" s="14"/>
       <c r="P38" s="20">
         <f>AVERAGE(P2:P35)</f>
-        <v>0.56252717381653994</v>
+        <v>0.61223114345375762</v>
       </c>
       <c r="Q38" s="20">
         <f>AVERAGE(Q2:Q35)</f>
-        <v>0.40457933346753783</v>
+        <v>0.435061370482344</v>
       </c>
       <c r="R38" s="20">
         <f>AVERAGE(R2:R35)</f>
@@ -4267,11 +4282,11 @@
       <c r="Y38" s="14"/>
       <c r="Z38" s="20">
         <f>AVERAGE(Z2:Z35)</f>
-        <v>0.78683763681868479</v>
+        <v>0.84380230623046648</v>
       </c>
       <c r="AA38" s="21">
         <f>AVERAGE(AA2:AA35)</f>
-        <v>0.46873271626183882</v>
+        <v>0.50414702169258752</v>
       </c>
       <c r="AB38" s="21">
         <f>AVERAGE(AB2:AB35)</f>

</xml_diff>

<commit_message>
Improved performance of exponential functions.
git-svn-id: https://svn.code.sf.net/p/half/code/branches/clean@380 ba856b29-48f5-46b1-a3e5-b459205bce89
</commit_message>
<xml_diff>
--- a/test/results.xlsx
+++ b/test/results.xlsx
@@ -177,9 +177,6 @@
     <t>func</t>
   </si>
   <si>
-    <t>ops</t>
-  </si>
-  <si>
     <t>all</t>
   </si>
   <si>
@@ -211,13 +208,16 @@
   </si>
   <si>
     <t>fdim</t>
+  </si>
+  <si>
+    <t>operators</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,25 +240,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="16">
@@ -457,12 +445,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -493,10 +480,8 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -843,7 +828,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>6</v>
@@ -864,7 +849,7 @@
         <v>12</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>18</v>
@@ -873,7 +858,7 @@
         <v>19</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S1" s="4" t="s">
         <v>13</v>
@@ -894,7 +879,7 @@
         <v>17</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z1" s="4" t="s">
         <v>20</v>
@@ -903,7 +888,7 @@
         <v>21</v>
       </c>
       <c r="AB1" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -1276,7 +1261,7 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -1368,7 +1353,7 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
@@ -1475,13 +1460,13 @@
         <v>0</v>
       </c>
       <c r="F8" s="2">
-        <v>6085</v>
+        <v>4689</v>
       </c>
       <c r="G8" s="2">
-        <v>5622</v>
+        <v>4338</v>
       </c>
       <c r="H8" s="2">
-        <v>5253</v>
+        <v>3788</v>
       </c>
       <c r="I8" s="2">
         <v>2</v>
@@ -1496,25 +1481,25 @@
         <v>9848</v>
       </c>
       <c r="M8" s="2">
-        <v>2130</v>
+        <v>2105</v>
       </c>
       <c r="N8" s="2">
-        <v>2153</v>
+        <v>2178</v>
       </c>
       <c r="O8" s="1">
-        <v>1217</v>
+        <v>1192</v>
       </c>
       <c r="P8" s="8">
         <f t="shared" si="0"/>
-        <v>0.35004108463434674</v>
+        <v>0.44892301130304968</v>
       </c>
       <c r="Q8" s="8">
         <f t="shared" si="1"/>
-        <v>0.38295980078263964</v>
+        <v>0.50207468879668049</v>
       </c>
       <c r="R8" s="8">
         <f t="shared" si="2"/>
-        <v>0.23167713687416713</v>
+        <v>0.3146779303062302</v>
       </c>
       <c r="S8" s="2">
         <v>0</v>
@@ -1529,25 +1514,25 @@
         <v>6772</v>
       </c>
       <c r="W8" s="2">
-        <v>2611</v>
+        <v>2733</v>
       </c>
       <c r="X8" s="2">
-        <v>2249</v>
+        <v>2222</v>
       </c>
       <c r="Y8" s="1">
-        <v>1518</v>
+        <v>1483</v>
       </c>
       <c r="Z8" s="8">
         <f t="shared" si="3"/>
-        <v>0.42908792111750205</v>
+        <v>0.58285348688419703</v>
       </c>
       <c r="AA8" s="9">
         <f t="shared" si="4"/>
-        <v>0.40003557452863747</v>
+        <v>0.512217611802674</v>
       </c>
       <c r="AB8" s="9">
         <f t="shared" si="5"/>
-        <v>0.28897772701313534</v>
+        <v>0.39149947201689544</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -1567,13 +1552,13 @@
         <v>0</v>
       </c>
       <c r="F9" s="2">
-        <v>4709</v>
+        <v>4481</v>
       </c>
       <c r="G9" s="2">
-        <v>4998</v>
+        <v>4688</v>
       </c>
       <c r="H9" s="2">
-        <v>4493</v>
+        <v>4074</v>
       </c>
       <c r="I9" s="2">
         <v>1</v>
@@ -1588,25 +1573,25 @@
         <v>9218</v>
       </c>
       <c r="M9" s="2">
-        <v>8049</v>
+        <v>8026</v>
       </c>
       <c r="N9" s="2">
-        <v>4411</v>
+        <v>4416</v>
       </c>
       <c r="O9" s="1">
-        <v>3258</v>
+        <v>3160</v>
       </c>
       <c r="P9" s="8">
         <f t="shared" si="0"/>
-        <v>1.7092801019324697</v>
+        <v>1.7911180540058023</v>
       </c>
       <c r="Q9" s="8">
         <f t="shared" si="1"/>
-        <v>0.88255302120848345</v>
+        <v>0.94197952218430037</v>
       </c>
       <c r="R9" s="8">
         <f t="shared" si="2"/>
-        <v>0.72512797685288222</v>
+        <v>0.77565046637211588</v>
       </c>
       <c r="S9" s="2">
         <v>0</v>
@@ -1621,25 +1606,25 @@
         <v>6144</v>
       </c>
       <c r="W9" s="2">
-        <v>7199</v>
+        <v>7239</v>
       </c>
       <c r="X9" s="2">
-        <v>4360</v>
+        <v>4336</v>
       </c>
       <c r="Y9" s="1">
-        <v>3525</v>
+        <v>3398</v>
       </c>
       <c r="Z9" s="8">
         <f t="shared" si="3"/>
-        <v>1.5287746867700149</v>
+        <v>1.615487614371792</v>
       </c>
       <c r="AA9" s="9">
         <f t="shared" si="4"/>
-        <v>0.87234893957583037</v>
+        <v>0.92491467576791808</v>
       </c>
       <c r="AB9" s="9">
         <f t="shared" si="5"/>
-        <v>0.7845537502782105</v>
+        <v>0.83406971035837019</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
@@ -1659,13 +1644,13 @@
         <v>310</v>
       </c>
       <c r="F10" s="2">
-        <v>7196</v>
+        <v>5501</v>
       </c>
       <c r="G10" s="2">
-        <v>6922</v>
+        <v>5254</v>
       </c>
       <c r="H10" s="2">
-        <v>6373</v>
+        <v>4708</v>
       </c>
       <c r="I10" s="2">
         <v>2</v>
@@ -1680,25 +1665,25 @@
         <v>9846</v>
       </c>
       <c r="M10" s="2">
-        <v>4786</v>
+        <v>4766</v>
       </c>
       <c r="N10" s="2">
-        <v>2419</v>
+        <v>2528</v>
       </c>
       <c r="O10" s="1">
-        <v>1553</v>
+        <v>1467</v>
       </c>
       <c r="P10" s="8">
         <f t="shared" si="0"/>
-        <v>0.66509171762090047</v>
+        <v>0.86638792946736953</v>
       </c>
       <c r="Q10" s="8">
         <f t="shared" si="1"/>
-        <v>0.34946547240681886</v>
+        <v>0.48115721355157975</v>
       </c>
       <c r="R10" s="8">
         <f t="shared" si="2"/>
-        <v>0.24368429311156442</v>
+        <v>0.31159728122344943</v>
       </c>
       <c r="S10" s="2">
         <v>0</v>
@@ -1713,25 +1698,25 @@
         <v>6772</v>
       </c>
       <c r="W10" s="2">
-        <v>4397</v>
+        <v>4404</v>
       </c>
       <c r="X10" s="2">
-        <v>2408</v>
+        <v>2627</v>
       </c>
       <c r="Y10" s="1">
-        <v>1724</v>
+        <v>1680</v>
       </c>
       <c r="Z10" s="8">
         <f t="shared" si="3"/>
-        <v>0.61103390772651478</v>
+        <v>0.80058171241592435</v>
       </c>
       <c r="AA10" s="9">
         <f t="shared" si="4"/>
-        <v>0.34787633631898296</v>
+        <v>0.5</v>
       </c>
       <c r="AB10" s="9">
         <f t="shared" si="5"/>
-        <v>0.27051624038914168</v>
+        <v>0.356839422259983</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -2768,8 +2753,8 @@
       <c r="G22" s="2">
         <v>1468</v>
       </c>
-      <c r="H22" s="30">
-        <v>2940</v>
+      <c r="H22">
+        <v>1172</v>
       </c>
       <c r="I22" s="2">
         <v>0</v>
@@ -2790,7 +2775,7 @@
         <v>679</v>
       </c>
       <c r="O22" s="1">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="P22" s="8">
         <f t="shared" si="0"/>
@@ -2802,7 +2787,7 @@
       </c>
       <c r="R22" s="8">
         <f t="shared" si="2"/>
-        <v>0.10544217687074831</v>
+        <v>0.25682593856655289</v>
       </c>
       <c r="S22" s="2">
         <v>0</v>
@@ -2823,7 +2808,7 @@
         <v>837</v>
       </c>
       <c r="Y22" s="1">
-        <v>557</v>
+        <v>536</v>
       </c>
       <c r="Z22" s="8">
         <f t="shared" si="3"/>
@@ -2835,7 +2820,7 @@
       </c>
       <c r="AB22" s="9">
         <f t="shared" si="5"/>
-        <v>0.18945578231292518</v>
+        <v>0.45733788395904434</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
@@ -3320,8 +3305,8 @@
       <c r="G28" s="2">
         <v>2602</v>
       </c>
-      <c r="H28" s="30">
-        <v>4356</v>
+      <c r="H28">
+        <v>2246</v>
       </c>
       <c r="I28" s="2">
         <v>0</v>
@@ -3342,7 +3327,7 @@
         <v>1585</v>
       </c>
       <c r="O28" s="1">
-        <v>829</v>
+        <v>796</v>
       </c>
       <c r="P28" s="8">
         <f t="shared" si="0"/>
@@ -3354,7 +3339,7 @@
       </c>
       <c r="R28" s="8">
         <f t="shared" si="2"/>
-        <v>0.19031221303948576</v>
+        <v>0.35440783615316118</v>
       </c>
       <c r="S28" s="2">
         <v>0</v>
@@ -3375,7 +3360,7 @@
         <v>1648</v>
       </c>
       <c r="Y28" s="1">
-        <v>1187</v>
+        <v>1158</v>
       </c>
       <c r="Z28" s="8">
         <f t="shared" si="3"/>
@@ -3387,7 +3372,7 @@
       </c>
       <c r="AB28" s="9">
         <f t="shared" si="5"/>
-        <v>0.27249770431588616</v>
+        <v>0.51558325912733749</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.25">
@@ -3596,8 +3581,8 @@
       <c r="G31" s="2">
         <v>1428</v>
       </c>
-      <c r="H31" s="30">
-        <v>3044</v>
+      <c r="H31">
+        <v>1135</v>
       </c>
       <c r="I31" s="2">
         <v>0</v>
@@ -3630,7 +3615,7 @@
       </c>
       <c r="R31" s="8">
         <f t="shared" si="2"/>
-        <v>0.19218134034165571</v>
+        <v>0.51541850220264318</v>
       </c>
       <c r="S31" s="2">
         <v>0</v>
@@ -3651,7 +3636,7 @@
         <v>1318</v>
       </c>
       <c r="Y31" s="1">
-        <v>811</v>
+        <v>781</v>
       </c>
       <c r="Z31" s="8">
         <f t="shared" si="3"/>
@@ -3663,7 +3648,7 @@
       </c>
       <c r="AB31" s="9">
         <f t="shared" si="5"/>
-        <v>0.2664257555847569</v>
+        <v>0.68810572687224669</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
@@ -3852,7 +3837,7 @@
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B34" s="2">
         <v>65536</v>
@@ -3944,7 +3929,7 @@
     </row>
     <row r="35" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B35" s="11">
         <v>65536</v>
@@ -4036,7 +4021,7 @@
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B36" s="25">
         <f>COUNTIF(B2:B5,"=0")/4</f>
@@ -4122,7 +4107,7 @@
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B37" s="26">
         <f>COUNTIF(B6:B35,"=0")/COUNTA(B6:B35)</f>
@@ -4164,15 +4149,15 @@
       <c r="O37" s="2"/>
       <c r="P37" s="19">
         <f>AVERAGE(P6:P35)</f>
-        <v>0.60199152481784046</v>
+        <v>0.61472539450412378</v>
       </c>
       <c r="Q37" s="19">
         <f>AVERAGE(Q6:Q35)</f>
-        <v>0.38827183858512698</v>
+        <v>0.39861294292294763</v>
       </c>
       <c r="R37" s="19">
         <f>AVERAGE(R6:R35)</f>
-        <v>0.23098505843105394</v>
+        <v>0.25899015235550887</v>
       </c>
       <c r="S37" s="26">
         <f>COUNTIF(S6:S35,"=0")/COUNTA(S6:S35)</f>
@@ -4195,21 +4180,21 @@
       <c r="Y37" s="2"/>
       <c r="Z37" s="19">
         <f>AVERAGE(Z6:Z35)</f>
-        <v>0.78234558874832694</v>
+        <v>0.79667979868358962</v>
       </c>
       <c r="AA37" s="19">
         <f>AVERAGE(AA6:AA35)</f>
-        <v>0.44894796751099408</v>
+        <v>0.45951034874923208</v>
       </c>
       <c r="AB37" s="28">
         <f>AVERAGE(AB6:AB35)</f>
-        <v>0.31753112348197976</v>
+        <v>0.35656474063864046</v>
       </c>
       <c r="AC37" s="29"/>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B38" s="27">
         <f>COUNTIF(B2:B35,"=0")/COUNTA(B2:B35)</f>
@@ -4251,15 +4236,15 @@
       <c r="O38" s="14"/>
       <c r="P38" s="20">
         <f>AVERAGE(P2:P35)</f>
-        <v>0.61223114345375762</v>
+        <v>0.62346691082400774</v>
       </c>
       <c r="Q38" s="20">
         <f>AVERAGE(Q2:Q35)</f>
-        <v>0.435061370482344</v>
+        <v>0.4441858743098327</v>
       </c>
       <c r="R38" s="20">
         <f>AVERAGE(R2:R35)</f>
-        <v>0.22102907093343044</v>
+        <v>0.24573944792559654</v>
       </c>
       <c r="S38" s="27">
         <f>COUNTIF(S2:S35,"=0")/COUNTA(S2:S35)</f>
@@ -4282,15 +4267,15 @@
       <c r="Y38" s="14"/>
       <c r="Z38" s="20">
         <f>AVERAGE(Z2:Z35)</f>
-        <v>0.84380230623046648</v>
+        <v>0.85645013852628682</v>
       </c>
       <c r="AA38" s="21">
         <f>AVERAGE(AA2:AA35)</f>
-        <v>0.50414702169258752</v>
+        <v>0.51346676984397399</v>
       </c>
       <c r="AB38" s="21">
         <f>AVERAGE(AB2:AB35)</f>
-        <v>0.35544273825433254</v>
+        <v>0.38988416515726837</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented and tested gamma functions.
git-svn-id: https://svn.code.sf.net/p/half/code/branches/clean@381 ba856b29-48f5-46b1-a3e5-b459205bce89
</commit_message>
<xml_diff>
--- a/test/results.xlsx
+++ b/test/results.xlsx
@@ -217,7 +217,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,13 +240,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="16">
@@ -445,11 +457,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -480,8 +493,11 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -3840,24 +3856,24 @@
         <v>54</v>
       </c>
       <c r="B34" s="2">
-        <v>65536</v>
+        <v>17</v>
       </c>
       <c r="C34" s="2">
-        <v>65536</v>
+        <v>16</v>
       </c>
       <c r="D34" s="2">
-        <v>65536</v>
+        <v>16</v>
       </c>
       <c r="E34" s="2">
-        <v>65536</v>
+        <v>16</v>
       </c>
       <c r="F34" s="2">
-        <v>22222</v>
+        <v>31192</v>
       </c>
       <c r="G34" s="2">
-        <v>22222</v>
-      </c>
-      <c r="H34" s="2">
+        <v>32155</v>
+      </c>
+      <c r="H34" s="30">
         <v>22222</v>
       </c>
       <c r="I34" s="2">
@@ -3873,21 +3889,21 @@
         <v>6</v>
       </c>
       <c r="M34" s="2">
-        <v>8838</v>
+        <v>9089</v>
       </c>
       <c r="N34" s="2">
-        <v>5658</v>
+        <v>5915</v>
       </c>
       <c r="O34" s="2">
         <v>3916</v>
       </c>
       <c r="P34" s="15">
         <f t="shared" si="0"/>
-        <v>0.39771397713977141</v>
+        <v>0.29138881764555014</v>
       </c>
       <c r="Q34" s="15">
         <f t="shared" si="1"/>
-        <v>0.25461254612546125</v>
+        <v>0.18395272896905612</v>
       </c>
       <c r="R34" s="8">
         <f t="shared" si="2"/>
@@ -3906,21 +3922,21 @@
         <v>0</v>
       </c>
       <c r="W34" s="2">
-        <v>9880</v>
+        <v>10178</v>
       </c>
       <c r="X34" s="2">
-        <v>7167</v>
+        <v>7494</v>
       </c>
       <c r="Y34" s="2">
         <v>5196</v>
       </c>
       <c r="Z34" s="15">
         <f t="shared" si="3"/>
-        <v>0.44460444604446042</v>
+        <v>0.32630161579892281</v>
       </c>
       <c r="AA34" s="16">
         <f t="shared" si="4"/>
-        <v>0.32251822518225182</v>
+        <v>0.2330586222982429</v>
       </c>
       <c r="AB34" s="9">
         <f t="shared" si="5"/>
@@ -3932,24 +3948,24 @@
         <v>55</v>
       </c>
       <c r="B35" s="11">
-        <v>65536</v>
+        <v>121</v>
       </c>
       <c r="C35" s="11">
-        <v>65536</v>
+        <v>58</v>
       </c>
       <c r="D35" s="11">
-        <v>65536</v>
+        <v>57</v>
       </c>
       <c r="E35" s="11">
-        <v>65536</v>
+        <v>58</v>
       </c>
       <c r="F35" s="11">
-        <v>22222</v>
+        <v>24722</v>
       </c>
       <c r="G35" s="11">
-        <v>22222</v>
-      </c>
-      <c r="H35" s="11">
+        <v>24292</v>
+      </c>
+      <c r="H35" s="31">
         <v>22222</v>
       </c>
       <c r="I35" s="11">
@@ -3965,21 +3981,21 @@
         <v>13140</v>
       </c>
       <c r="M35" s="11">
-        <v>9272</v>
+        <v>9583</v>
       </c>
       <c r="N35" s="11">
-        <v>5035</v>
+        <v>5250</v>
       </c>
       <c r="O35" s="11">
         <v>3489</v>
       </c>
       <c r="P35" s="12">
         <f t="shared" si="0"/>
-        <v>0.4172441724417244</v>
+        <v>0.38763045061079199</v>
       </c>
       <c r="Q35" s="12">
         <f t="shared" si="1"/>
-        <v>0.22657726577265772</v>
+        <v>0.21612053350897414</v>
       </c>
       <c r="R35" s="12">
         <f t="shared" si="2"/>
@@ -3998,21 +4014,21 @@
         <v>9794</v>
       </c>
       <c r="W35" s="11">
-        <v>22618</v>
+        <v>23479</v>
       </c>
       <c r="X35" s="11">
-        <v>15505</v>
+        <v>15897</v>
       </c>
       <c r="Y35" s="11">
         <v>11068</v>
       </c>
       <c r="Z35" s="12">
         <f t="shared" si="3"/>
-        <v>1.0178201782017819</v>
+        <v>0.94972089636760781</v>
       </c>
       <c r="AA35" s="13">
         <f t="shared" si="4"/>
-        <v>0.69773197731977321</v>
+        <v>0.65441297546517374</v>
       </c>
       <c r="AB35" s="13">
         <f t="shared" si="5"/>
@@ -4149,11 +4165,11 @@
       <c r="O37" s="2"/>
       <c r="P37" s="19">
         <f>AVERAGE(P6:P35)</f>
-        <v>0.61472539450412378</v>
+        <v>0.61019409845995198</v>
       </c>
       <c r="Q37" s="19">
         <f>AVERAGE(Q6:Q35)</f>
-        <v>0.39861294292294763</v>
+        <v>0.39590905794227799</v>
       </c>
       <c r="R37" s="19">
         <f>AVERAGE(R6:R35)</f>
@@ -4180,11 +4196,11 @@
       <c r="Y37" s="2"/>
       <c r="Z37" s="19">
         <f>AVERAGE(Z6:Z35)</f>
-        <v>0.79667979868358962</v>
+        <v>0.79046639494759918</v>
       </c>
       <c r="AA37" s="19">
         <f>AVERAGE(AA6:AA35)</f>
-        <v>0.45951034874923208</v>
+        <v>0.45508439525794514</v>
       </c>
       <c r="AB37" s="28">
         <f>AVERAGE(AB6:AB35)</f>
@@ -4236,11 +4252,11 @@
       <c r="O38" s="14"/>
       <c r="P38" s="20">
         <f>AVERAGE(P2:P35)</f>
-        <v>0.62346691082400774</v>
+        <v>0.61946870843209145</v>
       </c>
       <c r="Q38" s="20">
         <f>AVERAGE(Q2:Q35)</f>
-        <v>0.4441858743098327</v>
+        <v>0.44180009344453591</v>
       </c>
       <c r="R38" s="20">
         <f>AVERAGE(R2:R35)</f>
@@ -4267,11 +4283,11 @@
       <c r="Y38" s="14"/>
       <c r="Z38" s="20">
         <f>AVERAGE(Z2:Z35)</f>
-        <v>0.85645013852628682</v>
+        <v>0.85096772346511873</v>
       </c>
       <c r="AA38" s="21">
         <f>AVERAGE(AA2:AA35)</f>
-        <v>0.51346676984397399</v>
+        <v>0.50956151676342676</v>
       </c>
       <c r="AB38" s="21">
         <f>AVERAGE(AB2:AB35)</f>

</xml_diff>

<commit_message>
Added precondition error handling to mathematical functions.
git-svn-id: https://svn.code.sf.net/p/half/code/branches/errors@397 ba856b29-48f5-46b1-a3e5-b459205bce89
</commit_message>
<xml_diff>
--- a/test/results.xlsx
+++ b/test/results.xlsx
@@ -2295,13 +2295,13 @@
         <v>4</v>
       </c>
       <c r="C17" s="2">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="D17" s="2">
-        <v>475</v>
+        <v>20</v>
       </c>
       <c r="E17" s="2">
-        <v>465</v>
+        <v>7</v>
       </c>
       <c r="F17" s="2">
         <v>7782</v>

</xml_diff>

<commit_message>
Tested exception detection and handling.
git-svn-id: https://svn.code.sf.net/p/half/code/branches/errors@399 ba856b29-48f5-46b1-a3e5-b459205bce89
</commit_message>
<xml_diff>
--- a/test/results.xlsx
+++ b/test/results.xlsx
@@ -810,7 +810,10 @@
   </sheetPr>
   <dimension ref="A1:AC39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -966,10 +969,10 @@
         <v>0</v>
       </c>
       <c r="F3" s="1">
-        <v>5482</v>
+        <v>5950</v>
       </c>
       <c r="G3" s="1">
-        <v>4236</v>
+        <v>4275</v>
       </c>
       <c r="H3" s="1">
         <v>3762</v>
@@ -987,21 +990,21 @@
         <v>92258304</v>
       </c>
       <c r="M3" s="1">
-        <v>2542</v>
+        <v>2531</v>
       </c>
       <c r="N3" s="1">
-        <v>2068</v>
+        <v>2090</v>
       </c>
       <c r="O3" s="1">
         <v>378</v>
       </c>
       <c r="P3" s="6">
         <f>M3/F3</f>
-        <v>0.46369937978839837</v>
+        <v>0.42537815126050421</v>
       </c>
       <c r="Q3" s="6">
         <f>N3/G3</f>
-        <v>0.48819641170915956</v>
+        <v>0.48888888888888887</v>
       </c>
       <c r="R3" s="6">
         <f>O3/H3</f>
@@ -1020,21 +1023,21 @@
         <v>0</v>
       </c>
       <c r="W3" s="1">
-        <v>4682</v>
+        <v>4672</v>
       </c>
       <c r="X3" s="1">
-        <v>2513</v>
+        <v>2532</v>
       </c>
       <c r="Y3" s="1">
         <v>1147</v>
       </c>
       <c r="Z3" s="6">
         <f>W3/F3</f>
-        <v>0.85406785844582267</v>
+        <v>0.78521008403361348</v>
       </c>
       <c r="AA3" s="7">
         <f>X3/G3</f>
-        <v>0.59324834749763933</v>
+        <v>0.59228070175438596</v>
       </c>
       <c r="AB3" s="7">
         <f>Y3/H3</f>
@@ -1058,10 +1061,10 @@
         <v>0</v>
       </c>
       <c r="F4" s="2">
-        <v>6983</v>
+        <v>7512</v>
       </c>
       <c r="G4" s="2">
-        <v>4255</v>
+        <v>4336</v>
       </c>
       <c r="H4" s="2">
         <v>3791</v>
@@ -1079,21 +1082,21 @@
         <v>92258304</v>
       </c>
       <c r="M4" s="2">
-        <v>2548</v>
+        <v>2541</v>
       </c>
       <c r="N4" s="2">
-        <v>2083</v>
+        <v>2088</v>
       </c>
       <c r="O4" s="1">
         <v>376</v>
       </c>
       <c r="P4" s="6">
         <f t="shared" ref="P4:P36" si="0">M4/F4</f>
-        <v>0.36488615208363168</v>
+        <v>0.33825878594249204</v>
       </c>
       <c r="Q4" s="6">
         <f t="shared" ref="Q4:Q36" si="1">N4/G4</f>
-        <v>0.48954171562867216</v>
+        <v>0.48154981549815495</v>
       </c>
       <c r="R4" s="6">
         <f t="shared" ref="R4:R36" si="2">O4/H4</f>
@@ -1112,21 +1115,21 @@
         <v>0</v>
       </c>
       <c r="W4" s="2">
-        <v>5713</v>
+        <v>5712</v>
       </c>
       <c r="X4" s="2">
-        <v>2494</v>
+        <v>2505</v>
       </c>
       <c r="Y4" s="1">
         <v>1144</v>
       </c>
       <c r="Z4" s="6">
         <f t="shared" ref="Z4:Z36" si="3">W4/F4</f>
-        <v>0.81812974366318203</v>
+        <v>0.76038338658146964</v>
       </c>
       <c r="AA4" s="7">
         <f t="shared" ref="AA4:AA36" si="4">X4/G4</f>
-        <v>0.58613396004700358</v>
+        <v>0.57772140221402213</v>
       </c>
       <c r="AB4" s="7">
         <f t="shared" ref="AB4:AB36" si="5">Y4/H4</f>
@@ -1150,10 +1153,10 @@
         <v>0</v>
       </c>
       <c r="F5" s="2">
-        <v>3288</v>
+        <v>3142</v>
       </c>
       <c r="G5" s="2">
-        <v>2502</v>
+        <v>2623</v>
       </c>
       <c r="H5" s="2">
         <v>1820</v>
@@ -1171,21 +1174,21 @@
         <v>0</v>
       </c>
       <c r="M5" s="2">
-        <v>3281</v>
+        <v>3279</v>
       </c>
       <c r="N5" s="2">
-        <v>2826</v>
+        <v>2823</v>
       </c>
       <c r="O5" s="1">
         <v>376</v>
       </c>
       <c r="P5" s="6">
         <f t="shared" si="0"/>
-        <v>0.99787104622871048</v>
+        <v>1.0436028007638447</v>
       </c>
       <c r="Q5" s="6">
         <f t="shared" si="1"/>
-        <v>1.1294964028776979</v>
+        <v>1.0762485703393061</v>
       </c>
       <c r="R5" s="6">
         <f t="shared" si="2"/>
@@ -1204,21 +1207,21 @@
         <v>0</v>
       </c>
       <c r="W5" s="2">
-        <v>5411</v>
+        <v>5420</v>
       </c>
       <c r="X5" s="2">
-        <v>3158</v>
+        <v>3150</v>
       </c>
       <c r="Y5" s="1">
         <v>1775</v>
       </c>
       <c r="Z5" s="6">
         <f t="shared" si="3"/>
-        <v>1.6456812652068127</v>
+        <v>1.7250159134309357</v>
       </c>
       <c r="AA5" s="7">
         <f t="shared" si="4"/>
-        <v>1.2621902478017586</v>
+        <v>1.2009149828440717</v>
       </c>
       <c r="AB5" s="7">
         <f t="shared" si="5"/>
@@ -1242,10 +1245,10 @@
         <v>0</v>
       </c>
       <c r="F6" s="2">
-        <v>3969</v>
+        <v>3888</v>
       </c>
       <c r="G6" s="2">
-        <v>3205</v>
+        <v>3200</v>
       </c>
       <c r="H6" s="2">
         <v>2104</v>
@@ -1263,21 +1266,21 @@
         <v>0</v>
       </c>
       <c r="M6" s="2">
-        <v>3651</v>
+        <v>3634</v>
       </c>
       <c r="N6" s="2">
-        <v>3167</v>
+        <v>3181</v>
       </c>
       <c r="O6" s="1">
         <v>377</v>
       </c>
       <c r="P6" s="6">
         <f t="shared" si="0"/>
-        <v>0.91987906273620557</v>
+        <v>0.93467078189300412</v>
       </c>
       <c r="Q6" s="6">
         <f t="shared" si="1"/>
-        <v>0.98814352574102959</v>
+        <v>0.99406249999999996</v>
       </c>
       <c r="R6" s="6">
         <f t="shared" si="2"/>
@@ -1296,7 +1299,7 @@
         <v>0</v>
       </c>
       <c r="W6" s="2">
-        <v>7604</v>
+        <v>7668</v>
       </c>
       <c r="X6" s="2">
         <v>3658</v>
@@ -1306,11 +1309,11 @@
       </c>
       <c r="Z6" s="6">
         <f t="shared" si="3"/>
-        <v>1.9158478206097254</v>
+        <v>1.9722222222222223</v>
       </c>
       <c r="AA6" s="7">
         <f t="shared" si="4"/>
-        <v>1.1413416536661467</v>
+        <v>1.1431249999999999</v>
       </c>
       <c r="AB6" s="7">
         <f t="shared" si="5"/>
@@ -1334,10 +1337,10 @@
         <v>0</v>
       </c>
       <c r="F7" s="2">
-        <v>1207</v>
+        <v>1254</v>
       </c>
       <c r="G7" s="2">
-        <v>780</v>
+        <v>795</v>
       </c>
       <c r="H7" s="2">
         <v>589</v>
@@ -1355,21 +1358,21 @@
         <v>11280</v>
       </c>
       <c r="M7" s="2">
-        <v>741</v>
+        <v>735</v>
       </c>
       <c r="N7" s="2">
-        <v>603</v>
+        <v>587</v>
       </c>
       <c r="O7" s="1">
         <v>262</v>
       </c>
       <c r="P7" s="6">
         <f t="shared" si="0"/>
-        <v>0.61391880695940348</v>
+        <v>0.5861244019138756</v>
       </c>
       <c r="Q7" s="6">
         <f t="shared" si="1"/>
-        <v>0.77307692307692311</v>
+        <v>0.73836477987421378</v>
       </c>
       <c r="R7" s="6">
         <f t="shared" si="2"/>
@@ -1388,21 +1391,21 @@
         <v>0</v>
       </c>
       <c r="W7" s="2">
-        <v>1514</v>
+        <v>1501</v>
       </c>
       <c r="X7" s="2">
-        <v>664</v>
+        <v>656</v>
       </c>
       <c r="Y7" s="1">
         <v>372</v>
       </c>
       <c r="Z7" s="6">
         <f t="shared" si="3"/>
-        <v>1.2543496271748136</v>
+        <v>1.196969696969697</v>
       </c>
       <c r="AA7" s="7">
         <f t="shared" si="4"/>
-        <v>0.85128205128205126</v>
+        <v>0.82515723270440255</v>
       </c>
       <c r="AB7" s="7">
         <f t="shared" si="5"/>
@@ -1426,10 +1429,10 @@
         <v>0</v>
       </c>
       <c r="F8" s="2">
-        <v>21572</v>
+        <v>24089</v>
       </c>
       <c r="G8" s="2">
-        <v>18963</v>
+        <v>18884</v>
       </c>
       <c r="H8" s="2">
         <v>14420</v>
@@ -1447,21 +1450,21 @@
         <v>429655</v>
       </c>
       <c r="M8" s="2">
-        <v>11494</v>
+        <v>11457</v>
       </c>
       <c r="N8" s="2">
-        <v>9266</v>
+        <v>9595</v>
       </c>
       <c r="O8" s="1">
         <v>1964</v>
       </c>
       <c r="P8" s="6">
         <f t="shared" si="0"/>
-        <v>0.53282032264045986</v>
+        <v>0.47561127485574328</v>
       </c>
       <c r="Q8" s="6">
         <f t="shared" si="1"/>
-        <v>0.48863576438327266</v>
+        <v>0.50810209701334463</v>
       </c>
       <c r="R8" s="6">
         <f t="shared" si="2"/>
@@ -1480,21 +1483,21 @@
         <v>0</v>
       </c>
       <c r="W8" s="2">
-        <v>26750</v>
+        <v>26779</v>
       </c>
       <c r="X8" s="2">
-        <v>12815</v>
+        <v>12823</v>
       </c>
       <c r="Y8" s="1">
         <v>5347</v>
       </c>
       <c r="Z8" s="6">
         <f t="shared" si="3"/>
-        <v>1.2400333765992955</v>
+        <v>1.1116692266179584</v>
       </c>
       <c r="AA8" s="7">
         <f t="shared" si="4"/>
-        <v>0.67578969572325054</v>
+        <v>0.67904045753018427</v>
       </c>
       <c r="AB8" s="7">
         <f t="shared" si="5"/>
@@ -1518,10 +1521,10 @@
         <v>0</v>
       </c>
       <c r="F9" s="2">
-        <v>4819</v>
+        <v>5109</v>
       </c>
       <c r="G9" s="2">
-        <v>4475</v>
+        <v>4440</v>
       </c>
       <c r="H9" s="2">
         <v>3788</v>
@@ -1539,21 +1542,21 @@
         <v>9848</v>
       </c>
       <c r="M9" s="2">
-        <v>2221</v>
+        <v>2157</v>
       </c>
       <c r="N9" s="2">
-        <v>2445</v>
+        <v>2246</v>
       </c>
       <c r="O9" s="1">
         <v>1192</v>
       </c>
       <c r="P9" s="6">
         <f t="shared" si="0"/>
-        <v>0.46088400083004771</v>
+        <v>0.42219612448620081</v>
       </c>
       <c r="Q9" s="6">
         <f t="shared" si="1"/>
-        <v>0.54636871508379892</v>
+        <v>0.50585585585585591</v>
       </c>
       <c r="R9" s="6">
         <f t="shared" si="2"/>
@@ -1572,21 +1575,21 @@
         <v>6772</v>
       </c>
       <c r="W9" s="2">
-        <v>2739</v>
+        <v>2690</v>
       </c>
       <c r="X9" s="2">
-        <v>2292</v>
+        <v>2231</v>
       </c>
       <c r="Y9" s="1">
         <v>1483</v>
       </c>
       <c r="Z9" s="6">
         <f t="shared" si="3"/>
-        <v>0.56837518157294042</v>
+        <v>0.52652182423174787</v>
       </c>
       <c r="AA9" s="7">
         <f t="shared" si="4"/>
-        <v>0.51217877094972064</v>
+        <v>0.50247747747747751</v>
       </c>
       <c r="AB9" s="7">
         <f t="shared" si="5"/>
@@ -1610,10 +1613,10 @@
         <v>0</v>
       </c>
       <c r="F10" s="2">
-        <v>4568</v>
+        <v>4590</v>
       </c>
       <c r="G10" s="2">
-        <v>4736</v>
+        <v>4730</v>
       </c>
       <c r="H10" s="2">
         <v>4074</v>
@@ -1631,21 +1634,21 @@
         <v>9218</v>
       </c>
       <c r="M10" s="2">
-        <v>8382</v>
+        <v>8345</v>
       </c>
       <c r="N10" s="2">
-        <v>4568</v>
+        <v>4538</v>
       </c>
       <c r="O10" s="1">
         <v>3160</v>
       </c>
       <c r="P10" s="6">
         <f t="shared" si="0"/>
-        <v>1.834938704028021</v>
+        <v>1.818082788671024</v>
       </c>
       <c r="Q10" s="6">
         <f t="shared" si="1"/>
-        <v>0.96452702702702697</v>
+        <v>0.95940803382663853</v>
       </c>
       <c r="R10" s="6">
         <f t="shared" si="2"/>
@@ -1664,21 +1667,21 @@
         <v>6144</v>
       </c>
       <c r="W10" s="2">
-        <v>7435</v>
+        <v>7511</v>
       </c>
       <c r="X10" s="2">
-        <v>4528</v>
+        <v>4482</v>
       </c>
       <c r="Y10" s="1">
         <v>3398</v>
       </c>
       <c r="Z10" s="6">
         <f t="shared" si="3"/>
-        <v>1.6276269702276707</v>
+        <v>1.6363834422657952</v>
       </c>
       <c r="AA10" s="7">
         <f t="shared" si="4"/>
-        <v>0.95608108108108103</v>
+        <v>0.94756871035940804</v>
       </c>
       <c r="AB10" s="7">
         <f t="shared" si="5"/>
@@ -1702,10 +1705,10 @@
         <v>310</v>
       </c>
       <c r="F11" s="2">
-        <v>5794</v>
+        <v>5689</v>
       </c>
       <c r="G11" s="2">
-        <v>5489</v>
+        <v>5457</v>
       </c>
       <c r="H11" s="2">
         <v>4708</v>
@@ -1723,21 +1726,21 @@
         <v>9846</v>
       </c>
       <c r="M11" s="2">
-        <v>4959</v>
+        <v>4908</v>
       </c>
       <c r="N11" s="2">
-        <v>2693</v>
+        <v>2576</v>
       </c>
       <c r="O11" s="1">
         <v>1467</v>
       </c>
       <c r="P11" s="6">
         <f t="shared" si="0"/>
-        <v>0.85588539868829827</v>
+        <v>0.86271752504833887</v>
       </c>
       <c r="Q11" s="6">
         <f t="shared" si="1"/>
-        <v>0.49061759883403172</v>
+        <v>0.47205424225765075</v>
       </c>
       <c r="R11" s="6">
         <f t="shared" si="2"/>
@@ -1756,21 +1759,21 @@
         <v>6772</v>
       </c>
       <c r="W11" s="2">
-        <v>4566</v>
+        <v>4554</v>
       </c>
       <c r="X11" s="2">
-        <v>2499</v>
+        <v>2490</v>
       </c>
       <c r="Y11" s="1">
         <v>1680</v>
       </c>
       <c r="Z11" s="6">
         <f t="shared" si="3"/>
-        <v>0.78805661028650331</v>
+        <v>0.80049217788715066</v>
       </c>
       <c r="AA11" s="7">
         <f t="shared" si="4"/>
-        <v>0.45527418473310255</v>
+        <v>0.45629466739967017</v>
       </c>
       <c r="AB11" s="7">
         <f t="shared" si="5"/>
@@ -1794,10 +1797,10 @@
         <v>0</v>
       </c>
       <c r="F12" s="2">
-        <v>3623</v>
+        <v>3621</v>
       </c>
       <c r="G12" s="2">
-        <v>3306</v>
+        <v>3193</v>
       </c>
       <c r="H12" s="2">
         <v>2914</v>
@@ -1815,21 +1818,21 @@
         <v>4</v>
       </c>
       <c r="M12" s="2">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="N12" s="2">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="O12" s="1">
         <v>157</v>
       </c>
       <c r="P12" s="6">
         <f t="shared" si="0"/>
-        <v>0.21004692243996687</v>
+        <v>0.20988677161005248</v>
       </c>
       <c r="Q12" s="6">
         <f t="shared" si="1"/>
-        <v>0.1736237144585602</v>
+        <v>0.17820231756968369</v>
       </c>
       <c r="R12" s="6">
         <f t="shared" si="2"/>
@@ -1848,21 +1851,21 @@
         <v>0</v>
       </c>
       <c r="W12" s="2">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="X12" s="2">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="Y12" s="1">
         <v>348</v>
       </c>
       <c r="Z12" s="6">
         <f t="shared" si="3"/>
-        <v>0.2953353574385868</v>
+        <v>0.296050814692074</v>
       </c>
       <c r="AA12" s="7">
         <f t="shared" si="4"/>
-        <v>0.19328493647912887</v>
+        <v>0.19918571875978702</v>
       </c>
       <c r="AB12" s="7">
         <f t="shared" si="5"/>
@@ -1886,10 +1889,10 @@
         <v>0</v>
       </c>
       <c r="F13" s="2">
-        <v>3618</v>
+        <v>3661</v>
       </c>
       <c r="G13" s="2">
-        <v>3295</v>
+        <v>3250</v>
       </c>
       <c r="H13" s="2">
         <v>2896</v>
@@ -1907,21 +1910,21 @@
         <v>1</v>
       </c>
       <c r="M13" s="2">
-        <v>773</v>
+        <v>765</v>
       </c>
       <c r="N13" s="2">
-        <v>618</v>
+        <v>610</v>
       </c>
       <c r="O13" s="1">
         <v>168</v>
       </c>
       <c r="P13" s="6">
         <f t="shared" si="0"/>
-        <v>0.21365395245992261</v>
+        <v>0.20895930073750341</v>
       </c>
       <c r="Q13" s="6">
         <f t="shared" si="1"/>
-        <v>0.18755690440060699</v>
+        <v>0.18769230769230769</v>
       </c>
       <c r="R13" s="6">
         <f t="shared" si="2"/>
@@ -1940,21 +1943,21 @@
         <v>0</v>
       </c>
       <c r="W13" s="2">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="X13" s="2">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="Y13" s="1">
         <v>360</v>
       </c>
       <c r="Z13" s="6">
         <f t="shared" si="3"/>
-        <v>0.30182421227197348</v>
+        <v>0.29855230811253758</v>
       </c>
       <c r="AA13" s="7">
         <f t="shared" si="4"/>
-        <v>0.20606980273141123</v>
+        <v>0.20738461538461539</v>
       </c>
       <c r="AB13" s="7">
         <f t="shared" si="5"/>
@@ -1978,10 +1981,10 @@
         <v>0</v>
       </c>
       <c r="F14" s="2">
-        <v>5574</v>
+        <v>5235</v>
       </c>
       <c r="G14" s="2">
-        <v>3240</v>
+        <v>3451</v>
       </c>
       <c r="H14" s="2">
         <v>2915</v>
@@ -1999,21 +2002,21 @@
         <v>0</v>
       </c>
       <c r="M14" s="2">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="N14" s="2">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="O14" s="1">
         <v>923</v>
       </c>
       <c r="P14" s="6">
         <f>M14/F14</f>
-        <v>0.31880157875852172</v>
+        <v>0.33925501432664756</v>
       </c>
       <c r="Q14" s="6">
         <f>N14/G14</f>
-        <v>0.36944444444444446</v>
+        <v>0.34656621269197335</v>
       </c>
       <c r="R14" s="6">
         <f>O14/H14</f>
@@ -2032,21 +2035,21 @@
         <v>0</v>
       </c>
       <c r="W14" s="2">
-        <v>2029</v>
+        <v>2032</v>
       </c>
       <c r="X14" s="2">
-        <v>898</v>
+        <v>904</v>
       </c>
       <c r="Y14" s="1">
         <v>564</v>
       </c>
       <c r="Z14" s="6">
         <f>W14/F14</f>
-        <v>0.36401148188015786</v>
+        <v>0.38815663801337152</v>
       </c>
       <c r="AA14" s="7">
         <f>X14/G14</f>
-        <v>0.27716049382716051</v>
+        <v>0.26195305708490291</v>
       </c>
       <c r="AB14" s="7">
         <f>Y14/H14</f>
@@ -2070,10 +2073,10 @@
         <v>868</v>
       </c>
       <c r="F15" s="2">
-        <v>6638</v>
+        <v>6644</v>
       </c>
       <c r="G15" s="2">
-        <v>5972</v>
+        <v>5938</v>
       </c>
       <c r="H15" s="2">
         <v>5210</v>
@@ -2091,21 +2094,21 @@
         <v>5</v>
       </c>
       <c r="M15" s="2">
-        <v>1801</v>
+        <v>1825</v>
       </c>
       <c r="N15" s="2">
-        <v>1318</v>
+        <v>1311</v>
       </c>
       <c r="O15" s="1">
         <v>576</v>
       </c>
       <c r="P15" s="6">
         <f t="shared" si="0"/>
-        <v>0.27131666164507384</v>
+        <v>0.27468392534617703</v>
       </c>
       <c r="Q15" s="6">
         <f t="shared" si="1"/>
-        <v>0.22069658405894174</v>
+        <v>0.22078140788144157</v>
       </c>
       <c r="R15" s="6">
         <f t="shared" si="2"/>
@@ -2124,21 +2127,21 @@
         <v>0</v>
       </c>
       <c r="W15" s="2">
-        <v>2102</v>
+        <v>2108</v>
       </c>
       <c r="X15" s="2">
-        <v>1499</v>
+        <v>1487</v>
       </c>
       <c r="Y15" s="1">
         <v>885</v>
       </c>
       <c r="Z15" s="6">
         <f t="shared" si="3"/>
-        <v>0.31666164507381739</v>
+        <v>0.3172787477423239</v>
       </c>
       <c r="AA15" s="7">
         <f t="shared" si="4"/>
-        <v>0.25100468854655056</v>
+        <v>0.25042101717750082</v>
       </c>
       <c r="AB15" s="7">
         <f t="shared" si="5"/>
@@ -2162,10 +2165,10 @@
         <v>0</v>
       </c>
       <c r="F16" s="2">
-        <v>1494</v>
+        <v>1524</v>
       </c>
       <c r="G16" s="2">
-        <v>1502</v>
+        <v>1486</v>
       </c>
       <c r="H16" s="2">
         <v>1272</v>
@@ -2183,7 +2186,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="2">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="N16" s="2">
         <v>368</v>
@@ -2193,11 +2196,11 @@
       </c>
       <c r="P16" s="6">
         <f t="shared" si="0"/>
-        <v>0.28380187416331992</v>
+        <v>0.27624671916010501</v>
       </c>
       <c r="Q16" s="6">
         <f t="shared" si="1"/>
-        <v>0.24500665778961384</v>
+        <v>0.24764468371467024</v>
       </c>
       <c r="R16" s="6">
         <f t="shared" si="2"/>
@@ -2216,7 +2219,7 @@
         <v>0</v>
       </c>
       <c r="W16" s="2">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="X16" s="2">
         <v>398</v>
@@ -2226,11 +2229,11 @@
       </c>
       <c r="Z16" s="6">
         <f t="shared" si="3"/>
-        <v>0.4718875502008032</v>
+        <v>0.46325459317585299</v>
       </c>
       <c r="AA16" s="7">
         <f t="shared" si="4"/>
-        <v>0.26498002663115844</v>
+        <v>0.26783310901749663</v>
       </c>
       <c r="AB16" s="7">
         <f t="shared" si="5"/>
@@ -2254,10 +2257,10 @@
         <v>0</v>
       </c>
       <c r="F17" s="2">
-        <v>13662</v>
+        <v>13288</v>
       </c>
       <c r="G17" s="2">
-        <v>13678</v>
+        <v>13746</v>
       </c>
       <c r="H17" s="2">
         <v>12476</v>
@@ -2275,21 +2278,21 @@
         <v>0</v>
       </c>
       <c r="M17" s="2">
-        <v>4876</v>
+        <v>4862</v>
       </c>
       <c r="N17" s="2">
-        <v>3208</v>
+        <v>3189</v>
       </c>
       <c r="O17" s="1">
         <v>2242</v>
       </c>
       <c r="P17" s="6">
         <f t="shared" si="0"/>
-        <v>0.35690235690235689</v>
+        <v>0.36589403973509932</v>
       </c>
       <c r="Q17" s="6">
         <f t="shared" si="1"/>
-        <v>0.23453721304284253</v>
+        <v>0.23199476211261458</v>
       </c>
       <c r="R17" s="6">
         <f t="shared" si="2"/>
@@ -2311,18 +2314,18 @@
         <v>6438</v>
       </c>
       <c r="X17" s="2">
-        <v>4731</v>
+        <v>4686</v>
       </c>
       <c r="Y17" s="1">
         <v>3190</v>
       </c>
       <c r="Z17" s="6">
         <f t="shared" si="3"/>
-        <v>0.4712340799297321</v>
+        <v>0.48449729078868153</v>
       </c>
       <c r="AA17" s="7">
         <f t="shared" si="4"/>
-        <v>0.34588390115513962</v>
+        <v>0.34089917066783065</v>
       </c>
       <c r="AB17" s="7">
         <f t="shared" si="5"/>
@@ -2346,10 +2349,10 @@
         <v>7</v>
       </c>
       <c r="F18" s="2">
-        <v>7782</v>
+        <v>7735</v>
       </c>
       <c r="G18" s="2">
-        <v>7516</v>
+        <v>7621</v>
       </c>
       <c r="H18" s="2">
         <v>6296</v>
@@ -2367,21 +2370,21 @@
         <v>148569</v>
       </c>
       <c r="M18" s="2">
-        <v>4212</v>
+        <v>4192</v>
       </c>
       <c r="N18" s="2">
-        <v>4420</v>
+        <v>4262</v>
       </c>
       <c r="O18" s="1">
         <v>3072</v>
       </c>
       <c r="P18" s="6">
         <f t="shared" si="0"/>
-        <v>0.54124903623747112</v>
+        <v>0.54195216548157721</v>
       </c>
       <c r="Q18" s="6">
         <f t="shared" si="1"/>
-        <v>0.58807876530069181</v>
+        <v>0.5592441936753707</v>
       </c>
       <c r="R18" s="6">
         <f t="shared" si="2"/>
@@ -2400,21 +2403,21 @@
         <v>121458</v>
       </c>
       <c r="W18" s="2">
-        <v>4690</v>
+        <v>4688</v>
       </c>
       <c r="X18" s="2">
-        <v>5442</v>
+        <v>5011</v>
       </c>
       <c r="Y18" s="1">
         <v>3663</v>
       </c>
       <c r="Z18" s="6">
         <f t="shared" si="3"/>
-        <v>0.60267283474685174</v>
+        <v>0.60607627666451191</v>
       </c>
       <c r="AA18" s="7">
         <f t="shared" si="4"/>
-        <v>0.72405534858967535</v>
+        <v>0.65752525915234217</v>
       </c>
       <c r="AB18" s="7">
         <f t="shared" si="5"/>
@@ -2438,10 +2441,10 @@
         <v>0</v>
       </c>
       <c r="F19" s="2">
-        <v>3938</v>
+        <v>3850</v>
       </c>
       <c r="G19" s="2">
-        <v>3786</v>
+        <v>3869</v>
       </c>
       <c r="H19" s="2">
         <v>3257</v>
@@ -2459,21 +2462,21 @@
         <v>4</v>
       </c>
       <c r="M19" s="2">
-        <v>1361</v>
+        <v>1355</v>
       </c>
       <c r="N19" s="2">
-        <v>1074</v>
+        <v>1094</v>
       </c>
       <c r="O19" s="1">
         <v>341</v>
       </c>
       <c r="P19" s="6">
         <f t="shared" si="0"/>
-        <v>0.34560690705942104</v>
+        <v>0.35194805194805195</v>
       </c>
       <c r="Q19" s="6">
         <f t="shared" si="1"/>
-        <v>0.28367670364500791</v>
+        <v>0.28276040320496254</v>
       </c>
       <c r="R19" s="6">
         <f t="shared" si="2"/>
@@ -2492,7 +2495,7 @@
         <v>8</v>
       </c>
       <c r="W19" s="2">
-        <v>7781</v>
+        <v>7805</v>
       </c>
       <c r="X19" s="2">
         <v>1296</v>
@@ -2502,11 +2505,11 @@
       </c>
       <c r="Z19" s="6">
         <f t="shared" si="3"/>
-        <v>1.9758760792280345</v>
+        <v>2.0272727272727273</v>
       </c>
       <c r="AA19" s="7">
         <f t="shared" si="4"/>
-        <v>0.34231378763866877</v>
+        <v>0.33497027655724992</v>
       </c>
       <c r="AB19" s="7">
         <f t="shared" si="5"/>
@@ -2530,10 +2533,10 @@
         <v>0</v>
       </c>
       <c r="F20" s="2">
-        <v>4714</v>
+        <v>4777</v>
       </c>
       <c r="G20" s="2">
-        <v>4247</v>
+        <v>4489</v>
       </c>
       <c r="H20" s="2">
         <v>2919</v>
@@ -2551,21 +2554,21 @@
         <v>4062</v>
       </c>
       <c r="M20" s="2">
-        <v>1684</v>
+        <v>1667</v>
       </c>
       <c r="N20" s="2">
-        <v>1798</v>
+        <v>1804</v>
       </c>
       <c r="O20" s="1">
         <v>855</v>
       </c>
       <c r="P20" s="6">
         <f t="shared" si="0"/>
-        <v>0.35723377174374205</v>
+        <v>0.3489637848021771</v>
       </c>
       <c r="Q20" s="6">
         <f t="shared" si="1"/>
-        <v>0.42335766423357662</v>
+        <v>0.401871240810871</v>
       </c>
       <c r="R20" s="6">
         <f t="shared" si="2"/>
@@ -2584,21 +2587,21 @@
         <v>0</v>
       </c>
       <c r="W20" s="2">
-        <v>2257</v>
+        <v>2267</v>
       </c>
       <c r="X20" s="2">
-        <v>1654</v>
+        <v>1645</v>
       </c>
       <c r="Y20" s="1">
         <v>1061</v>
       </c>
       <c r="Z20" s="6">
         <f t="shared" si="3"/>
-        <v>0.47878659312685617</v>
+        <v>0.4745656269625288</v>
       </c>
       <c r="AA20" s="7">
         <f t="shared" si="4"/>
-        <v>0.38945137744290087</v>
+        <v>0.36645132546224102</v>
       </c>
       <c r="AB20" s="7">
         <f t="shared" si="5"/>
@@ -2622,10 +2625,10 @@
         <v>0</v>
       </c>
       <c r="F21" s="2">
-        <v>4911</v>
+        <v>4826</v>
       </c>
       <c r="G21" s="2">
-        <v>4445</v>
+        <v>4406</v>
       </c>
       <c r="H21" s="2">
         <v>3035</v>
@@ -2643,21 +2646,21 @@
         <v>6154</v>
       </c>
       <c r="M21" s="2">
-        <v>1650</v>
+        <v>1643</v>
       </c>
       <c r="N21" s="2">
-        <v>1592</v>
+        <v>1576</v>
       </c>
       <c r="O21" s="1">
         <v>827</v>
       </c>
       <c r="P21" s="6">
         <f t="shared" si="0"/>
-        <v>0.3359804520464264</v>
+        <v>0.34044757563199335</v>
       </c>
       <c r="Q21" s="6">
         <f t="shared" si="1"/>
-        <v>0.35815523059617549</v>
+        <v>0.35769405356332273</v>
       </c>
       <c r="R21" s="6">
         <f t="shared" si="2"/>
@@ -2676,21 +2679,21 @@
         <v>0</v>
       </c>
       <c r="W21" s="2">
-        <v>2254</v>
+        <v>2257</v>
       </c>
       <c r="X21" s="2">
-        <v>1635</v>
+        <v>1626</v>
       </c>
       <c r="Y21" s="1">
         <v>1043</v>
       </c>
       <c r="Z21" s="6">
         <f t="shared" si="3"/>
-        <v>0.45896965994705763</v>
+        <v>0.46767509324492335</v>
       </c>
       <c r="AA21" s="7">
         <f t="shared" si="4"/>
-        <v>0.36782902137232848</v>
+        <v>0.36904221516114388</v>
       </c>
       <c r="AB21" s="7">
         <f t="shared" si="5"/>
@@ -2714,10 +2717,10 @@
         <v>0</v>
       </c>
       <c r="F22" s="2">
-        <v>6135</v>
+        <v>6080</v>
       </c>
       <c r="G22" s="2">
-        <v>5326</v>
+        <v>5414</v>
       </c>
       <c r="H22" s="2">
         <v>3712</v>
@@ -2735,21 +2738,21 @@
         <v>3525</v>
       </c>
       <c r="M22" s="2">
-        <v>2263</v>
+        <v>2251</v>
       </c>
       <c r="N22" s="2">
-        <v>1557</v>
+        <v>1545</v>
       </c>
       <c r="O22" s="1">
         <v>744</v>
       </c>
       <c r="P22" s="6">
         <f t="shared" si="0"/>
-        <v>0.36886715566422168</v>
+        <v>0.37023026315789476</v>
       </c>
       <c r="Q22" s="6">
         <f t="shared" si="1"/>
-        <v>0.29233946676680433</v>
+        <v>0.28537125969708166</v>
       </c>
       <c r="R22" s="6">
         <f t="shared" si="2"/>
@@ -2768,21 +2771,21 @@
         <v>0</v>
       </c>
       <c r="W22" s="2">
-        <v>2859</v>
+        <v>2867</v>
       </c>
       <c r="X22" s="2">
-        <v>2155</v>
+        <v>2158</v>
       </c>
       <c r="Y22" s="1">
         <v>1162</v>
       </c>
       <c r="Z22" s="6">
         <f t="shared" si="3"/>
-        <v>0.46601466992665036</v>
+        <v>0.47154605263157895</v>
       </c>
       <c r="AA22" s="7">
         <f t="shared" si="4"/>
-        <v>0.40461885092001504</v>
+        <v>0.39859623199113409</v>
       </c>
       <c r="AB22" s="7">
         <f t="shared" si="5"/>
@@ -2806,10 +2809,10 @@
         <v>0</v>
       </c>
       <c r="F23" s="2">
-        <v>1630</v>
+        <v>1640</v>
       </c>
       <c r="G23" s="2">
-        <v>1550</v>
+        <v>1542</v>
       </c>
       <c r="H23">
         <v>1172</v>
@@ -2827,21 +2830,21 @@
         <v>4057</v>
       </c>
       <c r="M23" s="2">
-        <v>724</v>
+        <v>744</v>
       </c>
       <c r="N23" s="2">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="O23" s="1">
         <v>301</v>
       </c>
       <c r="P23" s="6">
         <f t="shared" si="0"/>
-        <v>0.44417177914110428</v>
+        <v>0.45365853658536587</v>
       </c>
       <c r="Q23" s="6">
         <f t="shared" si="1"/>
-        <v>0.45161290322580644</v>
+        <v>0.45265888456549935</v>
       </c>
       <c r="R23" s="6">
         <f t="shared" si="2"/>
@@ -2860,21 +2863,21 @@
         <v>0</v>
       </c>
       <c r="W23" s="2">
-        <v>981</v>
+        <v>1033</v>
       </c>
       <c r="X23" s="2">
-        <v>807</v>
+        <v>822</v>
       </c>
       <c r="Y23" s="1">
         <v>536</v>
       </c>
       <c r="Z23" s="6">
         <f t="shared" si="3"/>
-        <v>0.60184049079754598</v>
+        <v>0.62987804878048781</v>
       </c>
       <c r="AA23" s="7">
         <f t="shared" si="4"/>
-        <v>0.52064516129032257</v>
+        <v>0.53307392996108949</v>
       </c>
       <c r="AB23" s="7">
         <f t="shared" si="5"/>
@@ -2898,10 +2901,10 @@
         <v>0</v>
       </c>
       <c r="F24" s="2">
-        <v>3905</v>
+        <v>3908</v>
       </c>
       <c r="G24" s="2">
-        <v>3905</v>
+        <v>3876</v>
       </c>
       <c r="H24" s="2">
         <v>2753</v>
@@ -2919,21 +2922,21 @@
         <v>1</v>
       </c>
       <c r="M24" s="2">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="N24" s="2">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="O24" s="1">
         <v>340</v>
       </c>
       <c r="P24" s="6">
         <f t="shared" si="0"/>
-        <v>0.1851472471190781</v>
+        <v>0.18474923234390994</v>
       </c>
       <c r="Q24" s="6">
         <f t="shared" si="1"/>
-        <v>0.18489116517285531</v>
+        <v>0.18550051599587203</v>
       </c>
       <c r="R24" s="6">
         <f t="shared" si="2"/>
@@ -2952,21 +2955,21 @@
         <v>0</v>
       </c>
       <c r="W24" s="2">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="X24" s="2">
-        <v>804</v>
+        <v>807</v>
       </c>
       <c r="Y24" s="1">
         <v>536</v>
       </c>
       <c r="Z24" s="6">
         <f t="shared" si="3"/>
-        <v>0.25761843790012806</v>
+        <v>0.25716479017400207</v>
       </c>
       <c r="AA24" s="7">
         <f t="shared" si="4"/>
-        <v>0.2058898847631242</v>
+        <v>0.20820433436532507</v>
       </c>
       <c r="AB24" s="7">
         <f t="shared" si="5"/>
@@ -2990,10 +2993,10 @@
         <v>0</v>
       </c>
       <c r="F25" s="2">
-        <v>3959</v>
+        <v>4135</v>
       </c>
       <c r="G25" s="2">
-        <v>3697</v>
+        <v>3650</v>
       </c>
       <c r="H25" s="2">
         <v>2654</v>
@@ -3011,21 +3014,21 @@
         <v>3525</v>
       </c>
       <c r="M25" s="2">
-        <v>2012</v>
+        <v>1999</v>
       </c>
       <c r="N25" s="2">
-        <v>1667</v>
+        <v>1661</v>
       </c>
       <c r="O25" s="1">
         <v>865</v>
       </c>
       <c r="P25" s="6">
         <f t="shared" si="0"/>
-        <v>0.50820914372316239</v>
+        <v>0.48343409915356711</v>
       </c>
       <c r="Q25" s="6">
         <f t="shared" si="1"/>
-        <v>0.45090614011360564</v>
+        <v>0.45506849315068493</v>
       </c>
       <c r="R25" s="6">
         <f t="shared" si="2"/>
@@ -3044,21 +3047,21 @@
         <v>0</v>
       </c>
       <c r="W25" s="2">
-        <v>2799</v>
+        <v>2795</v>
       </c>
       <c r="X25" s="2">
-        <v>1920</v>
+        <v>1908</v>
       </c>
       <c r="Y25" s="1">
         <v>1281</v>
       </c>
       <c r="Z25" s="6">
         <f t="shared" si="3"/>
-        <v>0.70699671634251071</v>
+        <v>0.67593712212817414</v>
       </c>
       <c r="AA25" s="7">
         <f t="shared" si="4"/>
-        <v>0.51934000540979175</v>
+        <v>0.52273972602739727</v>
       </c>
       <c r="AB25" s="7">
         <f t="shared" si="5"/>
@@ -3082,10 +3085,10 @@
         <v>4083</v>
       </c>
       <c r="F26" s="2">
-        <v>7100</v>
+        <v>7120</v>
       </c>
       <c r="G26" s="2">
-        <v>6096</v>
+        <v>6255</v>
       </c>
       <c r="H26" s="2">
         <v>4136</v>
@@ -3103,21 +3106,21 @@
         <v>1176</v>
       </c>
       <c r="M26" s="2">
-        <v>5337</v>
+        <v>5465</v>
       </c>
       <c r="N26" s="2">
-        <v>2250</v>
+        <v>2244</v>
       </c>
       <c r="O26" s="1">
         <v>1358</v>
       </c>
       <c r="P26" s="6">
         <f t="shared" si="0"/>
-        <v>0.75169014084507046</v>
+        <v>0.7675561797752809</v>
       </c>
       <c r="Q26" s="6">
         <f t="shared" si="1"/>
-        <v>0.36909448818897639</v>
+        <v>0.35875299760191848</v>
       </c>
       <c r="R26" s="6">
         <f t="shared" si="2"/>
@@ -3136,21 +3139,21 @@
         <v>0</v>
       </c>
       <c r="W26" s="2">
-        <v>5568</v>
+        <v>5610</v>
       </c>
       <c r="X26" s="2">
-        <v>3074</v>
+        <v>3062</v>
       </c>
       <c r="Y26" s="1">
         <v>1832</v>
       </c>
       <c r="Z26" s="6">
         <f t="shared" si="3"/>
-        <v>0.78422535211267608</v>
+        <v>0.7879213483146067</v>
       </c>
       <c r="AA26" s="7">
         <f t="shared" si="4"/>
-        <v>0.50426509186351709</v>
+        <v>0.48952837729816145</v>
       </c>
       <c r="AB26" s="7">
         <f t="shared" si="5"/>
@@ -3174,10 +3177,10 @@
         <v>0</v>
       </c>
       <c r="F27" s="2">
-        <v>6468</v>
+        <v>6467</v>
       </c>
       <c r="G27" s="2">
-        <v>6001</v>
+        <v>5960</v>
       </c>
       <c r="H27" s="2">
         <v>5251</v>
@@ -3195,21 +3198,21 @@
         <v>13892</v>
       </c>
       <c r="M27" s="2">
-        <v>10687</v>
+        <v>10723</v>
       </c>
       <c r="N27" s="2">
-        <v>3214</v>
+        <v>2900</v>
       </c>
       <c r="O27" s="1">
         <v>1824</v>
       </c>
       <c r="P27" s="6">
         <f t="shared" si="0"/>
-        <v>1.6522881880024738</v>
+        <v>1.658110406680068</v>
       </c>
       <c r="Q27" s="6">
         <f t="shared" si="1"/>
-        <v>0.53557740376603902</v>
+        <v>0.48657718120805371</v>
       </c>
       <c r="R27" s="6">
         <f t="shared" si="2"/>
@@ -3228,21 +3231,21 @@
         <v>6771</v>
       </c>
       <c r="W27" s="2">
-        <v>10780</v>
+        <v>10761</v>
       </c>
       <c r="X27" s="2">
-        <v>2993</v>
+        <v>2960</v>
       </c>
       <c r="Y27" s="1">
         <v>2112</v>
       </c>
       <c r="Z27" s="6">
         <f t="shared" si="3"/>
-        <v>1.6666666666666667</v>
+        <v>1.6639863924539973</v>
       </c>
       <c r="AA27" s="7">
         <f t="shared" si="4"/>
-        <v>0.49875020829861688</v>
+        <v>0.49664429530201343</v>
       </c>
       <c r="AB27" s="7">
         <f t="shared" si="5"/>
@@ -3266,10 +3269,10 @@
         <v>0</v>
       </c>
       <c r="F28" s="2">
-        <v>7424</v>
+        <v>7398</v>
       </c>
       <c r="G28" s="2">
-        <v>6737</v>
+        <v>6710</v>
       </c>
       <c r="H28" s="2">
         <v>5789</v>
@@ -3287,21 +3290,21 @@
         <v>19670</v>
       </c>
       <c r="M28" s="2">
-        <v>10637</v>
+        <v>10703</v>
       </c>
       <c r="N28" s="2">
-        <v>3227</v>
+        <v>2924</v>
       </c>
       <c r="O28" s="1">
         <v>1852</v>
       </c>
       <c r="P28" s="6">
         <f t="shared" si="0"/>
-        <v>1.4327855603448276</v>
+        <v>1.446742362800757</v>
       </c>
       <c r="Q28" s="6">
         <f t="shared" si="1"/>
-        <v>0.47899658601751521</v>
+        <v>0.43576751117734724</v>
       </c>
       <c r="R28" s="6">
         <f t="shared" si="2"/>
@@ -3320,21 +3323,21 @@
         <v>13542</v>
       </c>
       <c r="W28" s="2">
-        <v>10778</v>
+        <v>10760</v>
       </c>
       <c r="X28" s="2">
-        <v>3015</v>
+        <v>2923</v>
       </c>
       <c r="Y28" s="1">
         <v>2003</v>
       </c>
       <c r="Z28" s="6">
         <f t="shared" si="3"/>
-        <v>1.4517780172413792</v>
+        <v>1.4544471478778047</v>
       </c>
       <c r="AA28" s="7">
         <f t="shared" si="4"/>
-        <v>0.44752857354905745</v>
+        <v>0.43561847988077496</v>
       </c>
       <c r="AB28" s="7">
         <f t="shared" si="5"/>
@@ -3358,10 +3361,10 @@
         <v>0</v>
       </c>
       <c r="F29" s="2">
-        <v>3002</v>
+        <v>3030</v>
       </c>
       <c r="G29" s="2">
-        <v>2666</v>
+        <v>2657</v>
       </c>
       <c r="H29">
         <v>2246</v>
@@ -3379,21 +3382,21 @@
         <v>16707</v>
       </c>
       <c r="M29" s="2">
-        <v>4950</v>
+        <v>5073</v>
       </c>
       <c r="N29" s="2">
-        <v>1630</v>
+        <v>1634</v>
       </c>
       <c r="O29" s="1">
         <v>796</v>
       </c>
       <c r="P29" s="6">
         <f t="shared" si="0"/>
-        <v>1.6489007328447702</v>
+        <v>1.6742574257425742</v>
       </c>
       <c r="Q29" s="6">
         <f t="shared" si="1"/>
-        <v>0.61140285071267819</v>
+        <v>0.61497929996236356</v>
       </c>
       <c r="R29" s="6">
         <f t="shared" si="2"/>
@@ -3412,21 +3415,21 @@
         <v>12097</v>
       </c>
       <c r="W29" s="2">
-        <v>5214</v>
+        <v>5222</v>
       </c>
       <c r="X29" s="2">
-        <v>1651</v>
+        <v>1641</v>
       </c>
       <c r="Y29" s="1">
         <v>1158</v>
       </c>
       <c r="Z29" s="6">
         <f t="shared" si="3"/>
-        <v>1.736842105263158</v>
+        <v>1.7234323432343235</v>
       </c>
       <c r="AA29" s="7">
         <f t="shared" si="4"/>
-        <v>0.61927981995498871</v>
+        <v>0.61761385020700033</v>
       </c>
       <c r="AB29" s="7">
         <f t="shared" si="5"/>
@@ -3450,10 +3453,10 @@
         <v>0</v>
       </c>
       <c r="F30" s="2">
-        <v>8605</v>
+        <v>8414</v>
       </c>
       <c r="G30" s="2">
-        <v>8030</v>
+        <v>8162</v>
       </c>
       <c r="H30" s="2">
         <v>6956</v>
@@ -3471,21 +3474,21 @@
         <v>4490</v>
       </c>
       <c r="M30" s="2">
-        <v>4234</v>
+        <v>4216</v>
       </c>
       <c r="N30" s="2">
-        <v>3051</v>
+        <v>3044</v>
       </c>
       <c r="O30" s="1">
         <v>1892</v>
       </c>
       <c r="P30" s="6">
         <f t="shared" si="0"/>
-        <v>0.49203951191167927</v>
+        <v>0.50106964582838132</v>
       </c>
       <c r="Q30" s="6">
         <f t="shared" si="1"/>
-        <v>0.37995018679950188</v>
+        <v>0.37294780691007107</v>
       </c>
       <c r="R30" s="6">
         <f t="shared" si="2"/>
@@ -3504,21 +3507,21 @@
         <v>0</v>
       </c>
       <c r="W30" s="2">
-        <v>4339</v>
+        <v>4354</v>
       </c>
       <c r="X30" s="2">
-        <v>3497</v>
+        <v>3440</v>
       </c>
       <c r="Y30" s="1">
         <v>2212</v>
       </c>
       <c r="Z30" s="6">
         <f t="shared" si="3"/>
-        <v>0.50424171993027311</v>
+        <v>0.51747088186356072</v>
       </c>
       <c r="AA30" s="7">
         <f t="shared" si="4"/>
-        <v>0.43549190535491905</v>
+        <v>0.4214653271257045</v>
       </c>
       <c r="AB30" s="7">
         <f t="shared" si="5"/>
@@ -3542,10 +3545,10 @@
         <v>0</v>
       </c>
       <c r="F31" s="2">
-        <v>3229</v>
+        <v>3169</v>
       </c>
       <c r="G31" s="2">
-        <v>2743</v>
+        <v>2747</v>
       </c>
       <c r="H31" s="2">
         <v>2478</v>
@@ -3563,21 +3566,21 @@
         <v>1</v>
       </c>
       <c r="M31" s="2">
-        <v>949</v>
+        <v>945</v>
       </c>
       <c r="N31" s="2">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="O31" s="1">
         <v>266</v>
       </c>
       <c r="P31" s="6">
         <f t="shared" si="0"/>
-        <v>0.29389903995044908</v>
+        <v>0.29820132533922372</v>
       </c>
       <c r="Q31" s="6">
         <f t="shared" si="1"/>
-        <v>0.21946773605541378</v>
+        <v>0.21805606115762649</v>
       </c>
       <c r="R31" s="6">
         <f t="shared" si="2"/>
@@ -3596,21 +3599,21 @@
         <v>0</v>
       </c>
       <c r="W31" s="2">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="X31" s="2">
-        <v>685</v>
+        <v>676</v>
       </c>
       <c r="Y31" s="1">
         <v>379</v>
       </c>
       <c r="Z31" s="6">
         <f t="shared" si="3"/>
-        <v>0.29018271910808302</v>
+        <v>0.29630798359103816</v>
       </c>
       <c r="AA31" s="7">
         <f t="shared" si="4"/>
-        <v>0.24972657674079474</v>
+        <v>0.24608663997087732</v>
       </c>
       <c r="AB31" s="7">
         <f t="shared" si="5"/>
@@ -3634,10 +3637,10 @@
         <v>0</v>
       </c>
       <c r="F32" s="2">
-        <v>1705</v>
+        <v>1699</v>
       </c>
       <c r="G32" s="2">
-        <v>1484</v>
+        <v>1446</v>
       </c>
       <c r="H32">
         <v>1135</v>
@@ -3655,21 +3658,21 @@
         <v>3009</v>
       </c>
       <c r="M32" s="2">
-        <v>1756</v>
+        <v>1731</v>
       </c>
       <c r="N32" s="2">
-        <v>1186</v>
+        <v>1166</v>
       </c>
       <c r="O32" s="1">
         <v>585</v>
       </c>
       <c r="P32" s="6">
         <f t="shared" si="0"/>
-        <v>1.0299120234604107</v>
+        <v>1.0188346085932902</v>
       </c>
       <c r="Q32" s="6">
         <f t="shared" si="1"/>
-        <v>0.79919137466307277</v>
+        <v>0.80636237897648688</v>
       </c>
       <c r="R32" s="6">
         <f t="shared" si="2"/>
@@ -3688,21 +3691,21 @@
         <v>0</v>
       </c>
       <c r="W32" s="2">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="X32" s="2">
-        <v>1357</v>
+        <v>1351</v>
       </c>
       <c r="Y32" s="1">
         <v>781</v>
       </c>
       <c r="Z32" s="6">
         <f t="shared" si="3"/>
-        <v>1.1173020527859236</v>
+        <v>1.1206592113007652</v>
       </c>
       <c r="AA32" s="7">
         <f t="shared" si="4"/>
-        <v>0.91442048517520214</v>
+        <v>0.93430152143845091</v>
       </c>
       <c r="AB32" s="7">
         <f t="shared" si="5"/>
@@ -3726,10 +3729,10 @@
         <v>153</v>
       </c>
       <c r="F33" s="2">
-        <v>5480</v>
+        <v>5558</v>
       </c>
       <c r="G33" s="2">
-        <v>7503</v>
+        <v>7603</v>
       </c>
       <c r="H33" s="2">
         <v>6171</v>
@@ -3747,21 +3750,21 @@
         <v>14432</v>
       </c>
       <c r="M33" s="2">
-        <v>2140</v>
+        <v>2133</v>
       </c>
       <c r="N33" s="2">
-        <v>1578</v>
+        <v>1536</v>
       </c>
       <c r="O33" s="2">
         <v>689</v>
       </c>
       <c r="P33" s="13">
         <f t="shared" si="0"/>
-        <v>0.39051094890510951</v>
+        <v>0.38377114069809282</v>
       </c>
       <c r="Q33" s="13">
         <f t="shared" si="1"/>
-        <v>0.21031587365053978</v>
+        <v>0.20202551624358805</v>
       </c>
       <c r="R33" s="6">
         <f t="shared" si="2"/>
@@ -3780,21 +3783,21 @@
         <v>13864</v>
       </c>
       <c r="W33" s="2">
-        <v>2989</v>
+        <v>3013</v>
       </c>
       <c r="X33" s="2">
-        <v>1818</v>
+        <v>1787</v>
       </c>
       <c r="Y33" s="2">
         <v>1152</v>
       </c>
       <c r="Z33" s="13">
         <f t="shared" si="3"/>
-        <v>0.54543795620437951</v>
+        <v>0.54210147535084563</v>
       </c>
       <c r="AA33" s="14">
         <f t="shared" si="4"/>
-        <v>0.24230307876849261</v>
+        <v>0.23503880047349732</v>
       </c>
       <c r="AB33" s="7">
         <f t="shared" si="5"/>
@@ -3818,10 +3821,10 @@
         <v>185</v>
       </c>
       <c r="F34" s="2">
-        <v>5288</v>
+        <v>5174</v>
       </c>
       <c r="G34" s="2">
-        <v>7462</v>
+        <v>7370</v>
       </c>
       <c r="H34" s="2">
         <v>6082</v>
@@ -3839,21 +3842,21 @@
         <v>14454</v>
       </c>
       <c r="M34" s="2">
-        <v>4840</v>
+        <v>4815</v>
       </c>
       <c r="N34" s="2">
-        <v>2666</v>
+        <v>2621</v>
       </c>
       <c r="O34" s="2">
         <v>1477</v>
       </c>
       <c r="P34" s="13">
         <f t="shared" si="0"/>
-        <v>0.91527987897125562</v>
+        <v>0.93061461151913416</v>
       </c>
       <c r="Q34" s="13">
         <f t="shared" si="1"/>
-        <v>0.35727686947199144</v>
+        <v>0.35563093622795117</v>
       </c>
       <c r="R34" s="6">
         <f t="shared" si="2"/>
@@ -3872,21 +3875,21 @@
         <v>13867</v>
       </c>
       <c r="W34" s="2">
-        <v>5466</v>
+        <v>5450</v>
       </c>
       <c r="X34" s="2">
-        <v>3001</v>
+        <v>2952</v>
       </c>
       <c r="Y34" s="2">
         <v>1907</v>
       </c>
       <c r="Z34" s="13">
         <f t="shared" si="3"/>
-        <v>1.0336611195158851</v>
+        <v>1.0533436412833397</v>
       </c>
       <c r="AA34" s="14">
         <f t="shared" si="4"/>
-        <v>0.40217099973197534</v>
+        <v>0.4005427408412483</v>
       </c>
       <c r="AB34" s="7">
         <f t="shared" si="5"/>
@@ -3910,10 +3913,10 @@
         <v>16</v>
       </c>
       <c r="F35" s="2">
-        <v>25855</v>
+        <v>25318</v>
       </c>
       <c r="G35" s="2">
-        <v>30854</v>
+        <v>30673</v>
       </c>
       <c r="H35" s="28">
         <v>22222</v>
@@ -3931,21 +3934,21 @@
         <v>6</v>
       </c>
       <c r="M35" s="2">
-        <v>9178</v>
+        <v>9189</v>
       </c>
       <c r="N35" s="2">
-        <v>5889</v>
+        <v>5850</v>
       </c>
       <c r="O35" s="2">
         <v>3916</v>
       </c>
       <c r="P35" s="13">
         <f t="shared" si="0"/>
-        <v>0.35497969444981631</v>
+        <v>0.36294336045501224</v>
       </c>
       <c r="Q35" s="13">
         <f t="shared" si="1"/>
-        <v>0.19086666234523886</v>
+        <v>0.19072148143318227</v>
       </c>
       <c r="R35" s="6">
         <f t="shared" si="2"/>
@@ -3964,21 +3967,21 @@
         <v>0</v>
       </c>
       <c r="W35" s="2">
-        <v>10253</v>
+        <v>10270</v>
       </c>
       <c r="X35" s="2">
-        <v>7596</v>
+        <v>7386</v>
       </c>
       <c r="Y35" s="2">
         <v>5196</v>
       </c>
       <c r="Z35" s="13">
         <f t="shared" si="3"/>
-        <v>0.39655772577837944</v>
+        <v>0.40564025594438741</v>
       </c>
       <c r="AA35" s="14">
         <f t="shared" si="4"/>
-        <v>0.24619174175147468</v>
+        <v>0.24079809604538194</v>
       </c>
       <c r="AB35" s="7">
         <f t="shared" si="5"/>
@@ -4002,10 +4005,10 @@
         <v>56</v>
       </c>
       <c r="F36" s="9">
-        <v>23510</v>
+        <v>23520</v>
       </c>
       <c r="G36" s="9">
-        <v>23643</v>
+        <v>23455</v>
       </c>
       <c r="H36" s="29">
         <v>22222</v>
@@ -4023,21 +4026,21 @@
         <v>13140</v>
       </c>
       <c r="M36" s="9">
-        <v>9623</v>
+        <v>9580</v>
       </c>
       <c r="N36" s="9">
-        <v>5523</v>
+        <v>5206</v>
       </c>
       <c r="O36" s="9">
         <v>3489</v>
       </c>
       <c r="P36" s="10">
         <f t="shared" si="0"/>
-        <v>0.4093151850276478</v>
+        <v>0.40731292517006801</v>
       </c>
       <c r="Q36" s="10">
         <f t="shared" si="1"/>
-        <v>0.23359979698007868</v>
+        <v>0.22195693881901513</v>
       </c>
       <c r="R36" s="10">
         <f t="shared" si="2"/>
@@ -4056,21 +4059,21 @@
         <v>9794</v>
       </c>
       <c r="W36" s="9">
-        <v>23511</v>
+        <v>23473</v>
       </c>
       <c r="X36" s="9">
-        <v>16004</v>
+        <v>15871</v>
       </c>
       <c r="Y36" s="9">
         <v>11068</v>
       </c>
       <c r="Z36" s="10">
         <f t="shared" si="3"/>
-        <v>1.0000425350914504</v>
+        <v>0.99800170068027216</v>
       </c>
       <c r="AA36" s="11">
         <f t="shared" si="4"/>
-        <v>0.6769022543670431</v>
+        <v>0.6766574291195907</v>
       </c>
       <c r="AB36" s="11">
         <f t="shared" si="5"/>
@@ -4121,11 +4124,11 @@
       <c r="O37" s="1"/>
       <c r="P37" s="15">
         <f>AVERAGE(P3:P6)</f>
-        <v>0.68658391020923648</v>
+        <v>0.68547762996496131</v>
       </c>
       <c r="Q37" s="15">
         <f>AVERAGE(Q3:Q6)</f>
-        <v>0.77384451398913989</v>
+        <v>0.76018744368158753</v>
       </c>
       <c r="R37" s="15">
         <f>AVERAGE(R3:R6)</f>
@@ -4152,11 +4155,11 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="15">
         <f>AVERAGE(Z3:Z6)</f>
-        <v>1.3084316719813858</v>
+        <v>1.3107079015670604</v>
       </c>
       <c r="AA37" s="16">
         <f>AVERAGE(AA3:AA6)</f>
-        <v>0.89572855225313708</v>
+        <v>0.87851052170311994</v>
       </c>
       <c r="AB37" s="16">
         <f>AVERAGE(AB3:AB6)</f>
@@ -4207,11 +4210,11 @@
       <c r="O38" s="2"/>
       <c r="P38" s="17">
         <f>AVERAGE(P7:P36)</f>
-        <v>0.61370123256545106</v>
+        <v>0.61214851958657301</v>
       </c>
       <c r="Q38" s="17">
         <f>AVERAGE(Q7:Q36)</f>
-        <v>0.40376164714352114</v>
+        <v>0.39468712849572218</v>
       </c>
       <c r="R38" s="17">
         <f>AVERAGE(R7:R36)</f>
@@ -4238,11 +4241,11 @@
       <c r="Y38" s="2"/>
       <c r="Z38" s="17">
         <f>AVERAGE(Z7:Z36)</f>
-        <v>0.79250365147900592</v>
+        <v>0.78977516267503556</v>
       </c>
       <c r="AA38" s="17">
         <f>AVERAGE(AA7:AA36)</f>
-        <v>0.45667212687075548</v>
+        <v>0.45077046966479656</v>
       </c>
       <c r="AB38" s="26">
         <f>AVERAGE(AB7:AB36)</f>
@@ -4294,11 +4297,11 @@
       <c r="O39" s="12"/>
       <c r="P39" s="18">
         <f>AVERAGE(P3:P36)</f>
-        <v>0.62227566522942568</v>
+        <v>0.62077547374873621</v>
       </c>
       <c r="Q39" s="18">
         <f>AVERAGE(Q3:Q36)</f>
-        <v>0.44730080794888805</v>
+        <v>0.43768716557641224</v>
       </c>
       <c r="R39" s="18">
         <f>AVERAGE(R3:R36)</f>
@@ -4325,11 +4328,11 @@
       <c r="Y39" s="12"/>
       <c r="Z39" s="18">
         <f>AVERAGE(Z3:Z36)</f>
-        <v>0.8532010656557566</v>
+        <v>0.85106136725056791</v>
       </c>
       <c r="AA39" s="19">
         <f>AVERAGE(AA3:AA36)</f>
-        <v>0.50832582397456505</v>
+        <v>0.50109282872812877</v>
       </c>
       <c r="AB39" s="19">
         <f>AVERAGE(AB3:AB36)</f>

</xml_diff>